<commit_message>
first working files update
</commit_message>
<xml_diff>
--- a/data_files/level_1.xlsx
+++ b/data_files/level_1.xlsx
@@ -651,81 +651,6 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">**https://portal.hse.ru/about**
-Наше подразделение осуществляет  концептуальную и структурную разработку и сопровождение корпоративного портала НИУ ВШЭ. Проще говоря, мы развиваем корпоративный портал университета: поддерживаем и создаем новые тематические разделы, открываем сайты подразделений, образовательных программ, конференций, учебных курсов, спецпроектов, публикуем на главной странице анонсы, обучаем сотрудников редактированию сайтов, ведем несколько баз данных.
-**Корпоративный портал (hse.ru) – это…**
-Над порталом работаем не только мы, и нам было бы очень тяжело обойтись без наших коллег из других подразделений.
-**Новости и анонсы на главной странице портала**
-Управление по связям с общественностью  – основной поставщик новостей для главной страницы корпоративного портала Университета. Без них портал не был бы таким интересным. Если у вашего подразделения есть новостной повод, то не забудьте проинформировать об этом наших коллег. Мы же можем помочь проанонсировать ваше мероприятие.
-Чтобы опубликовать анонс на главной странице портала, необходимо разместить анонс на сайте подразделения и прислать ссылку на него на адрес portalnews@hse.ru. Подробнее об анонсировании мероприятий можно прочитать здесь.
-**Персональные страницы**
-У каждого сотрудника (будь то именитый профессор или менеджер, бухгалтер или программист) на портале есть своя страница. Заглянув на персональную страницу, можно узнать, чем занимается ученый, какие предметы преподает профессор, какие вопросы помогает решить административный сотрудник. Создается она автоматически после внесения приказа о приеме сотрудника в базу Управления персонала ИС-ПРО.
-Мы даем сотрудникам все необходимые права для редактирования персональной страницы. Для того чтобы получить доступ к редактированию, необходимо написать заявку на адрес portal@hse.ru. Если у вас есть вопросы по тому, как появляется та или иная информация на странице, что именно публикуете вы, а что появляется автоматически из баз данных университета, то ответ можно найти на этой странице. Если вопросы все-таки остались, обратитесь к ответственному от своего подразделения. Английская версия личной страницы активируется английской редакцией портала. Заполнять открытые для редактирования поля необходимо самостоятельно.
-**База учебных курсов**
-Мы осуществляем техническую поддержку базы учебных курсов на портале НИУ ВШЭ, однако за описание курса мы ответственность не несем. Вся информация загружается к нам автоматически из учебных планов и модуля нагрузки системы «Абитуриент-Студент-Выпускник-Аспирант» (АСАВ). Из АСАВ мы получаем также и английское название курса для отображения в расписании.
-Если вы являетесь ответственным от кафедры/департамента, то вам необходимо получить права, написав об этом на адрес portal@hse.ru.
-**Сайты подразделений и образовательных программ**
-Вместе с сотрудниками подразделений мы работаем над сайтами подразделений, образовательных программ, мероприятий и проектов.
-Сайты подразделений создаются автоматически после того, как сведения внесены в ИС-ПРО. Подробнее о сайтах подразделений можно прочитать здесь.
-Сайты образовательных программ открываем мы, но только после внесения программы в АСАВ (иначе на сайте не будут отображаться рабочие учебные планы, расписание). При дальнейшей работе с сайтом вам поможет инструкция.
-Сайты мероприятий, семинаров, школ для школьников мы можем создать только при наличии у вас материалов для наполнения сайта. Пустые сайты (с надписью «В разработке») мы не открываем.
-Мы осуществляем первичное наполнение сайтов и потом только оказываем техническую поддержку. Поддержание актуальности сайта – ответственность сотрудника подразделения, для которого сайт был создан.
-По вопросам создания сайта обращайтесь, пожалуйста, на portal@hse.ru.
-**Английская версия портала**
-Англоязычный сайт Высшей школы экономики занял в 2015 году первое место в рейтинге сайтов университетов, составленном Российским советом по международным делам.
-Мы осуществляем перевод новостей для главной ленты портала, также можем помочь перевести основную информацию для сайта подразделения  (тексты «О подразделении», «Научная деятельность» и другие тексты, которые меняются редко). Переводом новостей, анонсов и прочих текстов подразделение занимается самостоятельно. Мы также размещаем в главной ленте портала анонсы англоязычных мероприятий и активируем английские версии личных страниц.
-Англоязычные версии сайтов обязательно создаются для подразделений, осуществляющих международную деятельность и/или взаимодействующих с иностранными организациями, студентами и преподавателями, а также для образовательных программ, на которых преподавание ведется на английском языке. В других случаях сайты создаются  только при условии готовности подразделения оперативно их поддерживать и регулярно обновлять своими силами.
-Английская версия создается по заявке от подразделения на адрес portal@hse.ru или непосредственно при обращении в Отдел развития и поддержки англоязычной версии портала (Мария Бесова).
-При создании текстов необходимо руководствоваться Глоссарием терминов ВШЭ и  Стилистическим справочником.
-**Раздел «Цифры и факты»**
-В НИУ ВШЭ постоянно что-то меняется: открываются новые программы, проводятся исследования, появляются новые подразделения. Подготовить статистическую информацию о жизни Университета нам помогает Аналитический центр.
-Когда вы используете какие-то цифры для статей, интервью и проч., пожалуйста, уточните у нас или в Аналитическом центре, не будут ли эти сведения обновлены в ближайшее время.
-**Система «Антиплагиат»**
-Мы предоставляем права преподавателям НИУ ВШЭ для проверки студенческих работ в системе «Антиплагиат».
-Чтобы получить доступ, достаточно написать заявку с любого адреса корпоративной почты на адрес antiplagiat@hse.ru.
-**Отчеты**
-Мы можем дать доступ к заполнению следующих электронных форм отчетов:
-отчет о деятельности научно-учебных и проектно-учебных лабораторий (отчет принимает Управление академического развития);
-отчет участника группы высокого профессионального потенциала НИУ ВШЭ (отчет кадрового резерва) (отчет принимает Управление академического развития). 
-Мы можем рассказать, как вносить информацию, но не можем рассказать, что именно должно быть внесено в отчет – на эти вопросы вам смогут ответить сотрудники соответствующих подразделений.
-Чтобы получить доступ к отчету, достаточно написать письмо на адрес portal@hse.ru
-Пожалуйста, указывайте в письме, за заполнение какого отчета вы отвечаете. Некоторые отчеты сдаются в одно время и нам сложно понять, какой именно вас интересует.
-**Новый функционал на портале**
-Разработкой портала занимается Управление разработки информационных систем портала. Если есть объективная необходимость в появлении чего-то нового, то мы готовы обсудить это вместе. Пожалуйста, до обсуждения постарайтесь кратко сформулировать основные пожелания, прикинуть, какие системы внутри университета это может затронуть. И, пожалуйста, не нужно пытаться заказать разработку одновременно Дирекции информационных технологий и Дирекции по порталу и мобильным приложениям. Желание подстраховаться естественно, но, поверьте, никому не хочется делать работу в стол. 
-Если, прочитав все это, вы не нашли ответ на свой вопрос, напишите директору по порталу Дмитрию Коптюбенко.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/help**
-        		    Шаг 1
-Необходимо удостовериться, что ваша персональная страница появилась на сайте. Персональная страница появляется на портале автоматически после внесения данных в базу сотрудниками Управления персонала. 
-        		    Шаг 2
-Следует авторизоваться в Едином личном кабинете (ЕЛК). Для этого необходимо в качестве логина ввести адрес корпоративной почты сотрудника, в качестве пароля – пароль от этой почты.
-Если вы не помните пароль от своей почты или у вас возникает ошибка при авторизации, обращайтесь на digital@hse.ru
-        		    Шаг 3
-В ЕЛК нужно перейти в раздел «Корпоративный портал» и нажать на «Персональная страница портала». Если вы не сможете войти в редактирование персональной страницы, значит, ваш корпоративный e-mail не прописан в необходимом поле. Напишите, пожалуйста, на portal@hse.ru.
-В письме укажите:
-• ФИО сотрудника
-• Адрес корпоративной почты
-Служба портала пропишет e-mail, и вы сможете войти.
-Письмо должно быть отправлено строго с корпоративной почты сотрудника @hse.ru 
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
           <t xml:space="preserve">**https://portal.hse.ru/persons**
 				Сотрудники
 Все подразделения
@@ -799,11 +724,63 @@
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/about**
+Наше подразделение осуществляет  концептуальную и структурную разработку и сопровождение корпоративного портала НИУ ВШЭ. Проще говоря, мы развиваем корпоративный портал университета: поддерживаем и создаем новые тематические разделы, открываем сайты подразделений, образовательных программ, конференций, учебных курсов, спецпроектов, публикуем на главной странице анонсы, обучаем сотрудников редактированию сайтов, ведем несколько баз данных.
+**Корпоративный портал (hse.ru) – это…**
+Над порталом работаем не только мы, и нам было бы очень тяжело обойтись без наших коллег из других подразделений.
+**Новости и анонсы на главной странице портала**
+Управление по связям с общественностью  – основной поставщик новостей для главной страницы корпоративного портала Университета. Без них портал не был бы таким интересным. Если у вашего подразделения есть новостной повод, то не забудьте проинформировать об этом наших коллег. Мы же можем помочь проанонсировать ваше мероприятие.
+Чтобы опубликовать анонс на главной странице портала, необходимо разместить анонс на сайте подразделения и прислать ссылку на него на адрес portalnews@hse.ru. Подробнее об анонсировании мероприятий можно прочитать здесь.
+**Персональные страницы**
+У каждого сотрудника (будь то именитый профессор или менеджер, бухгалтер или программист) на портале есть своя страница. Заглянув на персональную страницу, можно узнать, чем занимается ученый, какие предметы преподает профессор, какие вопросы помогает решить административный сотрудник. Создается она автоматически после внесения приказа о приеме сотрудника в базу Управления персонала ИС-ПРО.
+Мы даем сотрудникам все необходимые права для редактирования персональной страницы. Для того чтобы получить доступ к редактированию, необходимо написать заявку на адрес portal@hse.ru. Если у вас есть вопросы по тому, как появляется та или иная информация на странице, что именно публикуете вы, а что появляется автоматически из баз данных университета, то ответ можно найти на этой странице. Если вопросы все-таки остались, обратитесь к ответственному от своего подразделения. Английская версия личной страницы активируется английской редакцией портала. Заполнять открытые для редактирования поля необходимо самостоятельно.
+**База учебных курсов**
+Мы осуществляем техническую поддержку базы учебных курсов на портале НИУ ВШЭ, однако за описание курса мы ответственность не несем. Вся информация загружается к нам автоматически из учебных планов и модуля нагрузки системы «Абитуриент-Студент-Выпускник-Аспирант» (АСАВ). Из АСАВ мы получаем также и английское название курса для отображения в расписании.
+Если вы являетесь ответственным от кафедры/департамента, то вам необходимо получить права, написав об этом на адрес portal@hse.ru.
+**Сайты подразделений и образовательных программ**
+Вместе с сотрудниками подразделений мы работаем над сайтами подразделений, образовательных программ, мероприятий и проектов.
+Сайты подразделений создаются автоматически после того, как сведения внесены в ИС-ПРО. Подробнее о сайтах подразделений можно прочитать здесь.
+Сайты образовательных программ открываем мы, но только после внесения программы в АСАВ (иначе на сайте не будут отображаться рабочие учебные планы, расписание). При дальнейшей работе с сайтом вам поможет инструкция.
+Сайты мероприятий, семинаров, школ для школьников мы можем создать только при наличии у вас материалов для наполнения сайта. Пустые сайты (с надписью «В разработке») мы не открываем.
+Мы осуществляем первичное наполнение сайтов и потом только оказываем техническую поддержку. Поддержание актуальности сайта – ответственность сотрудника подразделения, для которого сайт был создан.
+По вопросам создания сайта обращайтесь, пожалуйста, на portal@hse.ru.
+**Английская версия портала**
+Англоязычный сайт Высшей школы экономики занял в 2015 году первое место в рейтинге сайтов университетов, составленном Российским советом по международным делам.
+Мы осуществляем перевод новостей для главной ленты портала, также можем помочь перевести основную информацию для сайта подразделения  (тексты «О подразделении», «Научная деятельность» и другие тексты, которые меняются редко). Переводом новостей, анонсов и прочих текстов подразделение занимается самостоятельно. Мы также размещаем в главной ленте портала анонсы англоязычных мероприятий и активируем английские версии личных страниц.
+Англоязычные версии сайтов обязательно создаются для подразделений, осуществляющих международную деятельность и/или взаимодействующих с иностранными организациями, студентами и преподавателями, а также для образовательных программ, на которых преподавание ведется на английском языке. В других случаях сайты создаются  только при условии готовности подразделения оперативно их поддерживать и регулярно обновлять своими силами.
+Английская версия создается по заявке от подразделения на адрес portal@hse.ru или непосредственно при обращении в Отдел развития и поддержки англоязычной версии портала (Мария Бесова).
+При создании текстов необходимо руководствоваться Глоссарием терминов ВШЭ и  Стилистическим справочником.
+**Раздел «Цифры и факты»**
+В НИУ ВШЭ постоянно что-то меняется: открываются новые программы, проводятся исследования, появляются новые подразделения. Подготовить статистическую информацию о жизни Университета нам помогает Аналитический центр.
+Когда вы используете какие-то цифры для статей, интервью и проч., пожалуйста, уточните у нас или в Аналитическом центре, не будут ли эти сведения обновлены в ближайшее время.
+**Система «Антиплагиат»**
+Мы предоставляем права преподавателям НИУ ВШЭ для проверки студенческих работ в системе «Антиплагиат».
+Чтобы получить доступ, достаточно написать заявку с любого адреса корпоративной почты на адрес antiplagiat@hse.ru.
+**Отчеты**
+Мы можем дать доступ к заполнению следующих электронных форм отчетов:
+отчет о деятельности научно-учебных и проектно-учебных лабораторий (отчет принимает Управление академического развития);
+отчет участника группы высокого профессионального потенциала НИУ ВШЭ (отчет кадрового резерва) (отчет принимает Управление академического развития). 
+Мы можем рассказать, как вносить информацию, но не можем рассказать, что именно должно быть внесено в отчет – на эти вопросы вам смогут ответить сотрудники соответствующих подразделений.
+Чтобы получить доступ к отчету, достаточно написать письмо на адрес portal@hse.ru
+Пожалуйста, указывайте в письме, за заполнение какого отчета вы отвечаете. Некоторые отчеты сдаются в одно время и нам сложно понять, какой именно вас интересует.
+**Новый функционал на портале**
+Разработкой портала занимается Управление разработки информационных систем портала. Если есть объективная необходимость в появлении чего-то нового, то мы готовы обсудить это вместе. Пожалуйста, до обсуждения постарайтесь кратко сформулировать основные пожелания, прикинуть, какие системы внутри университета это может затронуть. И, пожалуйста, не нужно пытаться заказать разработку одновременно Дирекции информационных технологий и Дирекции по порталу и мобильным приложениям. Желание подстраховаться естественно, но, поверьте, никому не хочется делать работу в стол. 
+Если, прочитав все это, вы не нашли ответ на свой вопрос, напишите директору по порталу Дмитрию Коптюбенко.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t xml:space="preserve">**https://portal.hse.ru/events**
 **https://portal.hse.ru/events**
@@ -839,11 +816,528 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/instev**
+Вход в редакторский режим https://www.hse.ru/adm/  Логин и пароль такие же как, от вашего личного кабинета (ЕЛК).
+**Оформление главной страницы**
+Основные вкладки, с которыми Вы будете работать, — это «Страницы» (создание и редактирование статических страниц сайта), «Опросы» (создание формы регистрации на мероприятие) и «Блоки».
+Основное управление контентом происходит во вкладке «Блоки» («Блоки (англ.)» — для английской версии сайта).
+Чтобы Вам было легче сориентироваться, в редакторском интерфейсе есть пояснения к разным полям для внесения информации, отмеченные звездочками или серым шрифтом.  
+**1 — 5 пункт заполняется в Блоки — Правая колонка — Данные о мероприятии.**
+**1. Заголовок**
+Рекомендуется заполнять оба верхних поля. Текст первой строки отображается мелким шрифтом. Тогда как текст — основное название мероприятия — отображается крупно.
+**2. Даты мероприятия3. Кнопка регистрации (ссылка на регистрацию)**
+Создание формы регистрации.
+**4. Ключевые даты**
+Заполняется в поле «Пояснение». Надпись «Важные даты» может варьироваться по усмотрению.
+**5. Место проведения, Контакты**
+В этой же вкладке Вы можете заполнять и использовать все другие поля. «Время начала мероприятия», «Языки мероприятия», ссылка на карту «Как добраться», «Важные ссылки», «Файлы» — все эти данные будут отображаться в правой части сайта.
+**6. Меню (горизонтальное) в центральной части страницы**
+**Блоки — Настройки — Меню**
+Необходимо создать новую группу, а внутри группы «Добавить ссылку», где первая строка — название пункта меню, вторая — ссылка на страницу (создание и редактирование статических страниц).
+Для того чтобы пункты меню выстраивались в горизонтальную линию, необходимо под каждый пункт меню создавать новую группу. При добавлении ссылки в той же группе, следующий пункт меню будет располагаться под предыдущим.
+Возможен еще один вариант расположения меню — в правой части сайта под датой мероприятия (см. рисунок ниже).
+По логике заполнения и редактирования правой части сайта, данные пункты вносятся в
+**Блоки — Правая колонка — Данные о мероприятии — Важные ссылки.**
+**Оформление аннотации/главной страницы сайта мероприятия**
+Информация, которая размещается на главной странице сайта, является ключевой и должна отражать важность проводимого мероприятия.
+Для заполнения/редактирования аннотации необходимо зайти в редакторский интерфейс главной страницы: любо через https://www.hse.ru/adm/ — Данные, либо с помощью значка «Редактору» в нижнем правом углу главной страницы.
+Аннотация находится в поле «О подразделении» и верстается по аналогии с версткой текста на статических страницах, с использованием такого же инструментария.
+**Оформление нижней части сайта мероприятия**
+Внизу главной страницы Вы можете разместить членов программного или организационного комитета, ключевых спикеров, докладчиков, партнеров и пр. с фото, регалиями и ссылками на персоны.
+**Это делается в Блоки — Подвал — Участники**
+Внутри Вы заводите соответствующую группу («Ключевые спикеры», например) и поочередно добавляете персон. Ссылка на персональную страницу и фотография сотрудников Вышки подгружается автоматически. Для персон не из ВШЭ Вы можете подгружать фото и ссылку в открывшемся окне вручную.
+По аналогичному принципу устроен пункт оформления партнеров мероприятия.
+**Блоки — Подвал — Партнеры**
+где необходимо добавлять логотип организации-партнера и ссылку на них.
+Однако зачастую бывает удобнее размещать партнеров в правой части сайта.
+Здесь снова работает логика работы с правой колонкой.
+**Блоки — Правая колонка — Текстовые блоки**
+Необходимо завести новый текстовый блок и заполнить его картинками-логотипами и, при желании, ссылками на сайты партнеров.
+**Оформление программы мероприятия**
+Также у Вас есть возможность сверстать программу вашего мероприятия. Она будет располагаться на главной странице сайта мероприятия под аннотацией.
+**Данный инструмент находится в Блоки — Контент — Расписание мероприятий**
+Структуру программы Вы выстраиваете путем добавления пунктов «Добавить день», «Добавить мероприятие» или «Добавить событие», в зависимости от структуры и продолжительности вашего мероприятия.
+**Оформление страницы организационного комитета (программного комитета, докладчиков и др.).**
+Если Вы решили создать отдельную статическую страницу для перечисления членов организационного или программного комитетов, докладчиков и др., Вам необходимо использовать создать составную страницу и выбрать виджет "Список персон". Как это сделать, вы можете прочитать в инструкции: https://portal.hse.ru/sostav.
+И главное — не забывайте нажимать на кнопку «Сохранить» внизу каждой карточки, которую Вы заполняете.
+</t>
+        </is>
+      </c>
+    </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/poll**
+**https://portal.hse.ru/poll**
+ Быстрые ссылки  Создание формы Уведомления на свою почту Ответное письмо пользователю Ссылка на форму/клонирование/выгрузка результатов CRM-система  
+**https://portal.hse.ru/poll**
+**Создание формы**
+Для создания регистрационных форм, форм подписки на новости, опросов и др. необходимо на сайте вашего подразделения зайти в Редактору – Данные – Опросы и регистрационные формы.
+Нажимаем на +, чтобы создать форму.
+Далее нужно указать:
+ название (если в названии используются длинные слова, вы можете поставить галочку расставить мягкие переносы); время проведения (тот период времени, в течение которого можно ответить на вопросы); статус (меняете на «активно» после того, как форма будет готова); язык (если форма на английском языке, необходимо выставить язык – «английский»). 
+Если у вас регистрация на мероприятие с ограниченным количеством участников, то существует возможность закрыть регистрацию после определенного количества заявок. В ином случае вы оставляете это поле незаполненным.
+Галочка «пройти можно только раз» нужна только в том случае, если вы создаете опрос.
+Галочка «автоматически нумеровать вопросы» стоит по умолчанию. Однако бывают случаи, когда автоматическая нумерация не нужна, – тогда галочку нужно убрать.
+Далее необходимо нажать на кнопку «Добавить блок вопросов».
+Если вам нужно разбить вопросы на несколько тематических блоков, то вы заполняете поле «Блок вопросов» (при необходимости также поле «Описание»).
+Пример блоков
+Если ваши вопросы должны идти подряд без разбивки на блоки, вы это поле не заполняете, а сразу переходите к кнопке «Добавить вопрос». В поле «Вопрос» вписываем непосредственно вопрос. В поле «Описание» можно добавить комментарии к вопросу.
+Далее нажимаем кнопку «Добавить ответ» и вписываем необходимый вариант.
+Если ответ на данный вопрос обязателен, ставим галочку напротив соответствующего пункта.
+Если на вопрос допускается один ответ, то выбираем соответствующую строку в поле «Формат ответа». Если на вопрос допускается несколько вариантов ответов, также выбираем соответствующую строку в поле «Формат ответа»
+Ответы можно сделать «выпадающим списком», тогда в поле «Формат ответа» нужно выбрать соответствующую строку.
+Если ответы не заданы, и тот, кто заполняет форму, должен вписать свой вариант ответа, в поле «Формат ответа» выбираем значение «Строка» или «Несколько строк». Вы можете добавить какой-то комментарий к свободному ответу в «Пояснительном тексте», а также ограничить в ответе количество символов.
+Если в ответе предполагается указание даты, номер телефона, e-mail, страны проживания или загрузка файла, то надо выбрать строку «Специальный вопрос» в поле «Формат ответа», а далее в выпадающем списке выбрать нужный вариант.
+Обратите внимание, что если вы выберете тип специального вопроса email, при заполнении формы браузер пользователя постарается автозаполнить это поле из кеша. Это облегчает пользователю заполнение формы. Автозаполнение из кеша браузера возможно также в отношении полей "Фамилия" (нужно выбрать Код вопроса "lastname") и имя (Код вопроса "firstname"). Автозаполнение не гарантируется, однако, как правило работает.
+После заполнения необходимо сохранить форму, нажав на кнопку «Создать».
+**https://portal.hse.ru/poll**
+**Дополнительные параметры**
+Чтобы открыть «Дополнительные параметры», необходимо нажать на стрелку.
+В открывшемся окне вы можете:
+ Добавить к форме пояснительный текст (будет отображаться сразу после заголовка); Добавить сообщение на странице после отправки формы (будет выводится на экране, напр.: «Спасибо за регистрацию. Ждем вас по адресу...»); Добавить сообщение на странице по завершении регистрации (будет заменять стандартную фразу «Извините, регистрация закончена»); Изменить текст согласия на обработку персональных данных (используется только при необходимости заменить стандартный текст); 
+В разделе «Дополнительные параметры» вы также сможете:
+ Поставить ссылку перехода после сохранения (надо иметь в виду, что если вы заполните это поле, сообщения типа «Спасибо за регистрацию» и «Регистрация завершена» выводиться не будут); Изменить схему показа вопросов (по умолчанию они идут друг за другом, схема «вопросы в виде таблицы» позволяет выстраивать их в две колонки); Привязать форму к определенному сайту (например, вы сделали ее на одном сайте, а вам нужно, чтобы форма была на другом, либо нужно привязать еще один сайт); Указать корпоративный e-mail сотрудника ВШЭ, на который будут приходить уведомления о новых ответах (каждый адрес должен быть добавлен отдельно, через кнопку «добавить»);  Связать с формой на другом языке (чтобы работала переключалка языков, если у вас есть такая же форма, например, на английском); 
+Если вы хотите, чтобы на почту пользователя приходило ответное письмо, надо поставить галочку напротив «Направить ответное письмо пользователю». Данная функция будет работать в том случае, если в форме нужно указывать email и ответ на этот вопрос обязателен. В поле «Текст письма» нужно разместить текст, а в коде вопроса про электронную почту надо прописать слово «email». Большая просьба в тексте письма указывать контактную информацию – куда пользователь может обратиться с вопросами, т.к. письма приходят с адреса robot@hse.ru.
+Если вы хотите, чтобы ответное письмо пользователю было персонализировано, то в поле «Текст письма» в начале нужно разместить фразу: Здравствуйте %%ANSWER_TO_QUESTION_lastname%% — %%ANSWER_TO_QUESTION_firstname%%. При этом необходимо, чтобы кроме e-mail, в вашей форме обязательными вопросами были отдельно «фамилия» и «имя» (или «имя-отчество»). В коде вопроса нужно прописать слова lastname и firstname.
+**https://portal.hse.ru/poll**
+**Ссылка на форму/Клонирование/Выгрузка ответов**
+Необходимо зайти в Редактору – Данные – Опросы и регистрационные формы и там вы сможете:
+1. Редактировать форму (чтобы сохранить изменения, нужно будет нажать кнопку «Сохранить»).
+2. Клонировать форму (если вам необходимо создать форму с теми же или похожими вопросами).
+3. Найти ссылку на форму (нажимаете на "встраивание", в открывшемся окне выбираете ссылку с названием вашего подразделения, чтобы форма открывалась внутри вашего сайта; кликаете на ссылку и в адресной строке открышегося окна копируете ссылку на вашу форму). Пример:
+4. Выгрузить ответы на форму (у вас есть возможность посмотреть результаты в pdf, html и excel).
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/format**
+**https://portal.hse.ru/format**
+ Быстрые ссылки  Оформление Вставка текста Списки Заголовки Якорь Вставка картинки/фото Загрузка файлов Вставка таблицы  
+**https://portal.hse.ru/format**
+**Оформление**
+ Все элементы форматирования и оформления придуманы не просто так. Любая страница сайта должна иметь правильную структуру, которая определённым образом обрабатывается браузерами и поисковыми системами. Чем проще, логичнее и понятнее структура страницы, тем быстрее она открывается (загружается), тем правильнее она индексируется поисковыми роботами (что влияет на выдачу сайта в поисковых системах). Не надо создавать пустые страницы (и выводить их в меню), страницы для размещения ссылки на другую страницу, страницы для размещения одного или нескольких файлов – это плохо влияет на имидж вашего сайта, а также на его индексацию в поисковых системах. Не надо задавать красную строку, выравнивать текст по ширине, по центру, по левому краю, по правому краю. Данный тип верстки не используется на веб-страницах. Например, при веб-верстке выравнивание по ширине приводит к тому, что слова расползаются, появляются большие интервалы. Внимательно также следите за тем, чтобы не было наследуемых из Word двойных пробелов.  Не надо использовать дополнительное форматирование текста. Оформление должно быть строго в корпоративном стиле. Не должно быть лишних подчёркиваний (в веб-верстке это выглядит как гиперссылка, которая никуда не ведет), выделения информации множеством восклицательных знаков, принудительного увеличения размера шрифта, изменения стиля шрифта или раскрашивания текста в разные цвета. Пожалуйста, пользуйтесь штатными инструментами форматирования. Для более интересного оформления можно воспользоваться виджетами, которые есть в функционале составной страницы. Если что-то не получается или не знаете, как оформить, пишите на portal@hse.ru 
+**Вставка текста**
+При копировании информации из документа Microsoft Word используйте следующую последовательность действий:
+1) Скопируйте текст из документа и нажмите на значок вставки информации из word файла. Вставьте скопированные материалы в открывшемся окне и нажмите «Вставить»;
+2) Выделите весь вставленный текст в поле и затем последовательно нажмите значок очистки лишнего кода и очистки формата;
+3) Удалите лишние пробелы и переносы строк;
+4) Разбейте текст на абзацы. Для этого необходимо выделить весь текст и выбрать «Абзац» на панели редактирования:
+Чтобы разбить текст на абзацы, можно также использовать сочетание клавиш Shift+Enter. 
+Если текст вставлен из Word некорректно, всё форматирование, отображающееся в редакторском интерфейсе, может пропасть или отображаться неправильно на готовой странице. Лучше всего форматировать тексты не в текстовых редакторах (Word), а непосредственно в визуальном редакторе.
+**Списки**
+Существует возможность создать как нумерованный, так и маркированный список. Для этого необходимо выделить текст и нажать на соответствующие кнопки на панели инструментов.
+Получается:
+   маркированный список маркированный список    нумерованный список нумерованный список  
+**Заголовки**
+Когда на странице размещён текст большого объёма, и его необходимо разбить на логические части (структурировать), название каждой такой части можно оформить элементом "Заголовок".
+ Предусмотрены 6 уровней заголовков:
+**Заголовок 2**
+**Заголовок 3**
+**Заголовок 4**
+Заголовки используются последовательно, по мере понижения значимости информации. 
+Заголовок 1 — заголовок первого уровня, самый важный, который используется в поле "Заголовок страницы" при отображении готовой страницы (не нужно в поле "Заголовок страницы" принудительно выбирать "Заголовок 1"). На странице нельзя использовать несколько заголовков первого уровня! Поэтому в поле "Текст" оформлять какой-либо заголовок стилем "Заголовок 1" не нужно.
+Для выделения информации одинаковой значимости в рамках одной страницы используются заголовки одинакового уровня (например, "Заголовок 3"). Если внутри такого заголовка необходим подзаголовок, для его оформления используется заголовок четвёртого уровня ("Заголовок 4"). Крайне не желательно пропускать уровни заголовков. Например, если для заголовка используется "Заголовок 3", для подзаголовка должен использоваться "Заголовок 4", а не "Заголовок 5" или "Заголовок 6".
+Заголовки — важный элемент для поисковых систем! Они задают правильную структуру страницы. "Заголовком" нельзя оформлять отдельные предложения или абзацы. 
+**Якорь**
+Якорем называется закладка на определенном месте страницы, предназначенная для создания перехода к ней по ссылке. Якоря удобно применять в документах большого объема, чтобы можно было быстро переходить к нужному разделу.
+Чтобы создать якорь, необходимо поставить курсор в соответствующем месте страницы, на панели инструментов нажать на значок "якорь", в открывшемся окне прописать латинскими буквами "имя якоря" (напр: anchor), нажать "вставить".
+Если ссылку на якорь нужно разместить на той же странице, где сделан якорь, необходимо нажать на значок "ссылка" на панели инструментов, в поле "якоря" выбрать соответствующее имя якоря, далее нажать "вставить".
+Если ссылку на якорь нужно разместить на другой странице, то необходимо нажать на значок "ссылка" на панели инструментов, в поле "адрес" прописать ссылку на страницу с якорем, а также имя якоря с символом решетки (#) впереди (напр: https://portal.hse.ru/format#anchor), нажать "вставить".
+**Вставка картинки/фото**
+При загрузке изображений обращайте внимание на его размер. Чем шире изображение, тем больше места оно занимает на странице. Изменить размер изображения можно непосредственно при его загрузке.
+1. Нажимаем кнопку "Загрузка и вставка картинки"
+2. Ждём загрузки изображения. Переходим на вкладку "Положение", поле "Размер". Первая цифра — размер в пикселях по ширине, вторая — размер в пикселях по высоте.
+3. Если размер изображения по ширине и высоте устраивает, нажимаем вставить.
+4. В том случае, если при размещении картинки она занимает слишком много места (непосредственно в редакторском интерфейсе или на готовой странице при её сохранении), в редакторском интерфейсе кликаем на картинку левой кнопкой мыши (тем самым выбирая изображение), после того, как на границах изображения появилась рамка, кликаем правой кнопкой мыши. В появившемся меню выбираем пункт "Добавить/изменить изображение".
+5. В открывшемся окне снова выбираем вкладку "Положение" и меняем размеры картинки. Нажимаем кнопку "Обновить".
+Если Вы собираетесь разместить несколько изображений на странице, лучше воспользоваться опцией «Фотоальбом» (внизу страницы).  Нажимаете кнопку «Добавить изображение», выбираете нужный файл и далее сохраняете страницу.  
+****
+**Загрузка файлов**
+Для размещения файлов на странице необходимо воспользоваться кнопкой  на панели редактирования:
+После этого откроется диалоговое окно загрузки файла:
+В поле "Выберите файл" выбираем нужный файл (желательно, чтобы в имени файла были латинские буквы и между словами не было пробелов). В поле "Название" обязательно указываем название файла! Именно это название будет выводиться на сайте и использоваться для поиска по порталу и в поисковых системах. Обратите внимание на то, что у загружаемого файла должно быть внятное название без сокращений, многоточий и т.п. Нельзя называть файл "Регламент исп-я...тем...технич-го рег-та" и т.п. Пользователь ничего не поймет из подобного названия.
+Нажимаем кнопку "Загрузить". После того как файл загрузится, вид окна изменится. Для вставки файла на страницу нажимаем "Вставить":
+После того как файл появился в редакторском интерфейсе, его название при необходимости можно поправить.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/tables**
+ Быстрые ссылки  Копирование таблицы из Word и Excel Создание таблицы в визуальном редакторе Специальные шаблоны для создания таблицы  
+**Копирование таблицы из Word и Excel**
+В том случае, если Вы копируете таблицу из Word или Excel, необходимо пользоваться инструментами очистки лишнего кода и форматирования.
+Сначала нужно воспользоваться кнопкой "очистка стилей таблицы":
+Далее необходимо использовать "метелку" и "ластик" для очистки формата текста.
+Если таблица будет вставлена некорректно, она будет некорректно отображаться на экранах компьютеров и мобильных устройств.
+ Оформление должно быть в строгом корпоративном стиле! Не надо задавать красную строку, выравнивать текст по ширине, по центру, по левому краю, по правому краю. Выравнивание по ширине применяется только при книжной верстке, где есть переносы, при веб-верстке переносы отсутствуют и выравнивание по ширине приводит к тому, что слова расползаются, появляются большие интервалы. Внимательно следите за тем, чтобы не было двойных пробелов, лишних подчёркиваний, выделения информации множеством восклицательных знаков и путем раскрашивания текста во все цвета радуги. 
+**Создание таблицы в визуальном редакторе**
+Создавать таблицы лучше непосредственно в визуальном редакторе статической страницы. Для создания таблицы кликните на иконку 
+В появившемся окне укажите необходимое количество строк и столбцов. При необходимости отметьте флажок «Заголовок ячейки». В этом случае у первой строчки таблицы ячейки будут объединены. В момент первоначального создания таблицы не рекомендуем задавать границы таблицы, поскольку в этом случае в визуальном редакторе границы таблицы отображаться не будут (хотя при сохранении страницы и при просмотре её в обычном режиме все границы отобразятся).
+После заполнения необходимых полей нажимаем кнопку «Вставить». После этого работа с таблицей в редакторском интерфейсе происходит так же, как в любом текстовом редакторе. Правой кнопкой мышки либо при помощи кнопок работы с таблицей можно добавлять и удалять строки, объединять и разбивать ячейки, устанавливать ширину и высоту строк (в случае, если это действительно необходимо).
+Если вы в самом начале работы с таблицей не поставили значение границы, а границы для данной таблицы необходимы, то задать их можно двумя способами: 1) ставим курсор в любом месте таблицы, кликаем правой кнопкой мышки, в появившемся контекстном меню выбираем «Параметры таблицы», в поле «Граница» проставляем значение толщины границ (1 – практически универсальный размер границ); 2) ставим курсор в любом месте таблицы и снова нажимаем на иконку создания таблицы. В появившемся окошке в поле «Граница» проставляем значение толщины границ (1 – практически универсальный размер границ).
+**Специальные шаблоны для создания таблиц**
+Таблицу можно также добавить через «специальные шаблоны». Нажмите на кнопку добавления специального элемента.
+Строка данных включает в себя заголовок и 2 строки с данными, значения и их расшифровка. Можно разместить до 6 столбцов с возможностью их объединения.
+Блок данных представляет из себя несколько колонок с информацией, максимальное количество колонок также равно 6.
+Воздушная таблица отделена от верхнего контента на странице линией, при наведении на строку таблицы будет изменяться ее цвет.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/sostav**
+Для создания составной статической страницы необходимо проделать все те же шаги, что и для создания простой статической страницы. После заполнения основных полей переходим к полю "Вид страницы" (расположено над полем "Текст"). По умолчанию флажок установлен в положение "Простая". Кликаем на него и выбираем "Составная":
+Слева расположены виджеты, отвечающие за формат размещения информации в том или ином блоке: текст, фото, видео... Справа — непосредственно поле для размещения виджетов и, соответственно, информации.
+Выбираем виджет, подходящий для информации, которую необходимо разместить на странице, цепляем его курсором в левой колонке и тянем мышкой вправо, в большую центральную колонку. 
+Внутри центральной части страницы в редакторском интерфейсе все виджеты можно легко менять местами, просто перетягивая их мышью, удалять ненужные и добавлять новые.
+После размещения необходимой информации нажимаем "Сохранить" и обязательно проверяем, что получилось!
+**ВИДЖЕТЫ:**
+**Текст**
+ Для размещения текста нужно выбрать виджет "Фрагмент текста с заголовком".  После вставки текста его нужно обязательно выделить и нажать на панели инструментов кнопку Tx для очистки лишнего кода. Далее необходимо разбить текст на абзацы, для этого можно использовать клавишу Enter. В остальном принципы оформления текста те же, что и на простой статической странице. 
+**Изображения**
+ Вы можете разместить как одиночное изображение, так и фотогалерею.  При загрузке изображений обязательно помните, что сначала их необходимо оптимизировать 
+**Видео**
+ Видео сначала необходимо разместить на Youtube. Затем выбираете виджет "Видео", ставите галочку "Стороннее видео", в поле URL проставляете ссылку вида: https://www.youtube.com/embed/pWeQh4ocVUk/. Чтобы получить такую ссылку, находясь непосредственно на Youtube, нажимаете на кнопку «Поделиться» (она располагается под видео). Выбираете самый первый вариант – «Встроить». У вас откроется окно, где слева будет видео, а справа – встраиваемый код. Копируете оттуда значение c embed и вставляете эту ссылку в виджет. Если необходимо, можно добавить заголовок.  
+**Якорь**
+ Якорем называется закладка на определенном месте страницы, предназначенная для создания перехода к ней по ссылке. Чтобы создать якорь, необходимо переместить виджет "Якорь" в нужное место и прописать в нем латинскими буквами "имя якоря" (напр: anchor). В ссылке, по которой пользователь будет переходить в опеределенное место страницы, в поле "адрес" нужно прописать ссылку на страницу плюс имя якоря с символом решетки (#) впереди (напр: https://portal.hse.ru/#anchor).  
+**Цветные блоки**
+ Для оформления контента в виде цветных блоков нужно выбрать одноименный виджет. Регулируете количество блоков в строке – их может быть 2 или 3, нажимаете на кнопку "добавить", открывается окно, в котором вы прописывает заголовок, ссылку, боковое меню (если нужно), а также загружаете фоновую фотографию.  Пример:  
+**Связанные материалы**
+ Если нужно вынести на главную страницу материалы, которые связаны между собой какой-то общей темой, вы можете воспользоваться виджетом "Связанные материалы". Например, у вас есть несколько интервью выпускников или студентов, вы ставите их фотографии (предварительно вырезав), подписи (ФИО, м.б. также краткий заголовок интервью) и ссылку.  Пример:  
+**Список персон**
+ Информацию о персонах можно представить на странице разными способами. Горизонтальный список Перемещаете виджет "Список персон". Заполняете поле "Заголовок". Выбираете вид "Список". Нажимаете "Добавить персону". Если персона из ВШЭ, то вводите ФИО, нажимаете "Найти" и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение «Из ВШЭ» на "Не из ВШЭ". Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете "Вырезать", чтобы выбрать область фотографии, которая будет показываться на странице. Это необходимо сделать, чтобы показывалось именно круглое фото, а не овальное. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL  Пример:  Вертикальный список Перемещаете виджет "Список персон". Заполняете поле "Заголовок". Выбираете вид "Список". Проставляете галочку "Отображать вертикальным списком". Нажимаете "Добавить персону". Если персона из ВШЭ, то вы вводите ФИО, нажимаете "Найти" и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. В поле "Описание/контакты" добавляете необходимую информацию. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение "Из ВШЭ" на "Не из ВШЭ". Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете "Вырезать", чтобы выбрать область фотографии, которая будет показываться на странице. Это необходимо сделать, чтобы показывалось именно круглое фото, а не овальное. В поле "Описание/контакты" добавляете необходимую информацию. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL  Пример:  Одиночное круглое большое фото Если вам нужно разместить одиночное большое фото с подписью и текстом, вы выбираете виджет "Список персон", заполняете поле "Заголовок", далее выбираете вид "Одиночный", стиль "Большое фото". Если персона из ВШЭ, то вы вводите ФИО, нажимаете "Найти" и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. В поле "Описание/контакты" добавляете необходимую информацию. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение "Из ВШЭ" на "Не из ВШЭ". Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете "Вырезать", чтобы выбрать область фотографии, которая будет показываться на странице. В поле "Описание/контакты" добавляете необходимую информацию. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL.  Пример:  Круглое большое фото в колонках Если вы хотите разместить несколько подряд круглых фото в колонке, то перемещаете сначала виджет "Строка с колонками", а потом непосредственного в него добавляете виджет "Список персон". Выставляете ширину колонки "4", если вы хотите 3 персоны в ряд. Выставляете ширину колонки "3", если вы хотите 4 персоны в ряд. В сумме ширина всех колонок должна быть равна числу "12". Остальные действия – те же, что при размещении одиночного круглого фото.  Пример:  Карусель Если у вас много персон, и вы хотите, чтобы они выстраивались в один ряд, то выбираете виджет "Список персон", заполняете поле "Заголовок", далее выбираете вид "Карусель". Нажимаете "Добавить персону". Если персона из ВШЭ, то вы вводите ФИО, нажимаете "Найти" и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение "Из ВШЭ" на "Не из ВШЭ". Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете "Вырезать", чтобы выбрать область фотографии, которая будет показываться на странице. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL  Пример:  
+**Хронология**
+ С помощью виджета "Хронология" можно создать таймлайн или пошаговую инструкцию. Перемещаете из левой колонки виджет "Хронология". Если нужно сделать пошаговую инструкцию, то ставите галочку возле слова "Нумерация". Выбираете цвет, далее нажимаете "Добавить запись". В появившемся окне вписываете заголовок и текст, далее нажимаете опять "Добавить запись" за пределами окна. Если вам нужно добавить плашки (они выстраиваются в колонки), то нажимаете "Добавить запись" внутри окна.  Пример:    
+**Партнеры**
+ Чтобы разместить логотипы партнеров, нужно переместить из левой колонки виджет "Партнеры", заполнить поле "Заголовок", загрузить логотип, поставить ссылку и написать название компании-партнера. Логотипы встают в колонки по 4 в строке.  Пример:  
+**Колонки**
+ Если нужно разместить информацию в колонки, пожалуйста, не создавайте таблицу, пользуйтесь виджетом "Строка с колонками". У колонки нужно задать ширину. В сумме ширина всех колонок должна быть равна числу "12". Далее внутрь этого виджета нужно вставить другой виджет, в который вы будете непосредственно размещать информацию. Например, виджет "Фрагмент текста с заголовком".  Пример:  
+**Соцсети**
+ Если необходимо разместить иконки социальных сетей, нужно переместить из левой колонки виджет "Соцсети", нажать "Добавить запись", заполнить поле "Заголовок", поставить ссылку на соцсеть, а также выбрать из перечня нужную вам иконку. При необходимости иконки можно расположить по центру, поставив соответствующую галочку.  Пример:  
+**Плашка**
+ Для выделения значимых пунктов в тексте можно воспользоваться виджетом "Плашка с цифрой". Перемещаете виджет в центральную колонку, заполняете поле Заголовок (раздела), выбираете цвет цифры, ставите галочку около "Нумерация", нажимаете "Добавить запись". Внутри заполняете поле "Заголовок" (если нужно) и поле "Текст". Пример:  Можно сделать плашки без цифры, тогда вы не ставите галочку около "Нумерация". Пример:  Плашки можно поставить в колонки. Тогда предварительно нужно переместить виджет "Строка с колонками" (о том, как это сделать смотрите выше), а потом в него переместить виджет "Плашка с цифрой". Пример:  
+**Даты**
+ Когда нужно красиво оформить даты мероприятия, воспользуйтесь виджетом "Связанные события". После того как вы переместили виджет, нажимаете "Добавить запись", далее заполняете поля "Число", "Месяц" и "Текст". Если вы хотите, чтобы между датами стояли стрелки, ставите галочку "Показывать стрелку".  Пример:  
+**Цифра**
+ Если в тексте нужно разместить блок со значимыми цифрами, то вы выбираете виджет "Цифра дня", перемещаете его, выбираете цвет цифры и текста и заполняете необходимые поля.  Пример:  
+**Выпадайки**
+ Если нужно разместить раскрывающийся цветной блок, то вы выбираете виджет "Набор с выпадайками". Нажимаете кнопку "Добавить блок", проставляете заголовок, в поле "Описание" ставите текст, который будет показываться до скрытого текста, в поле "Открывающийся текст" вписываете текст, который будет открываться по клику. Далее выбираете цвет блока.  Пример:  Если вам нужно просто сделать выпадающий список, то вы выбираете виджет "Набор с выпадайками 2". Нажимаете кнопку "Добавить блок", в поле "Заголовок" вписываете текст, по которому будут кликать, в поле "Открывающийся текст" вписываете текст, который будет открываться по клику.  Пример:  
+**Кнопка**
+ Если вам нужно создать кнопку, например "Регистрация", вы выбираете виджет "Декоратор", выбираете опцию "Кнопка", размещаете название кнопки и ссылку на страницу, на которую кнопка должна вести.  Пример:  
+**Часто задаваемые вопросы**
+   Чтобы разместить все вопросы на странице, надо выбрать виджет "Вопросы и ответы (FAQ)", нажать "Добавить вопрос" и заполнить поля "Вопрос" и "Ответ".  Пример:  
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/photo**
+Почему это важно? Во многом трафик на ваш сайт и, как следствие, степень интереса к вашим продуктам и результатам деятельности, зависит от скорости загрузки страниц. Вот что о некоторых страницах портала думает искусственный интеллект:
+Вы можете сами проверить свой сайт с помощью этого инструмента.
+Как с этим бороться? Прежде всего, тщательно следя за тем, чтобы загружаемые вами на портал фотографии не были чрезмерно тяжелыми. Помните, что размер фотографий вес фотографии только отчасти зависит от ее размера в пикселях. И самое маленькое изображение может весить более чем достаточно, если оно хорошего качества.
+ Для начала уменьшите изображение до нужных размеров. Это можно сделать в любом графическом редакторе. Если у вас нет на компьютере установленной программы, вы можете воспользоваться, например, онлайн-сервисом Photoshop Express или Pixlr. Самая широкая картинка на портале не превышает 1600 пикселей по ширине. Ориентируйтесь на эту ширину как на максимальную. Оптимизируйте изображение с помощью сервиса Tinypng. Это очень просто. Заходите на сайт и перетаскиваете изображение в специальный контейнер прямо на сайте. После вам останется только скачать обратно на свой компьютер сжатую картинку. Теперь ее можно использовать на портале. 
+Можно, конечно, продолжать работать с сайтом, не оптимизируя изображения. Но в таком случае нужно помнить, что это повлечет за собой потерю части посетителей вашего сайта, прежде всего самых продвинутых, заходящих в интернет с мобильного телефона, а также потенциальных клиентов из ряда зарубежных стран, где скорость интернета оставляет желать лучшего. Команда портала, со своей стороны, прикладывает все усилия, чтобы оптимизировать другие элементы страниц технологическими средствами.
+Чтобы узнать, какие изображения из числа тех, что уже размещены на вашем сайте, нуждаются в оптимизации, воспользуйтесь сервисом Google PageSpeed Insights. Зайдите на страницу сервиса, введите адрес страницы, которую нужно проверить, дождитесь результата, найдите вкладку «Оптимизируйте изображения». Например, для главной страницы портала она выглядит так:
+А для главной страницы типичной образовательной программы – так:
+Разница в объеме потенциально оптимизируемого – в 17 раз.
+Вы можете оптимизировать уже размещенные на сайте изображения с помощью встроенных инструментов Google PageSpeed Insights. Для этого внизу страницы с результатами обследования вашей страницы найдите ссылку «Скачать оптимизированные изображения, ресурсы JavaScript и CSS для этой страницы».
+К вам на компьютер будет скачан архив, в одной из папке которого будут содержаться ужатые изображения. Их необходимо опубликовать на вашем сайте взамен тех, которые там были ранее.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/pages**
+Перейдите в раздел «Страницы» верхнего меню в режиме редактирования сайта.
+Создайте страницу, кликнув по иконке 
+При заполнении поля «Заголовок» не используйте форматирование текста, не разбивайте текст на строки, не вставляйте в поле картинки. Если вы копируете в это поле текст из Word, обязательно очистите форматирование. Это поле предназначено исключительно для текста, а форматирование в любом случае не будет отражено на готовой странице!
+Техническое имя страницы (поле «Путь») указывается только латинскими строчными буквами. Желательно, чтобы техническое имя состояло из одного слова. Если необходимо использовать два слова в названии страницы, ни в коем случае нельзя делать пробелы между словами — «help managers». Должно быть: либо «help_managers», либо «help/managers».
+Нельзя создавать пустые страницы, страницы для размещения ссылки на другую страницу, страницы для размещения одного-единственного файла.
+Английские версии русских страниц должны иметь такие же технические имена, как и русскоязычные страницы. Единственное отличие — при создании английской страницы в поле «Язык» необходимо проставить значение «английский».
+В рамках одного сайта не должно быть статических страниц с одинаковым адресом (поле "Путь") на одном языке!
+После того как вы наполнили страницу, прописали у нее техническое имя, вам необходимо сохранить страницу.
+После сохранения страница будет доступна по адресу: адрес-главной-страницы-сайта/путь. Например, у данной страницы адрес: https://portal.hse.ru/pages/, где https://portal.hse.ru/ — адрес главной страницы сайта, pages — путь страницы.
+Чтобы на страницу могли заходить пользователи, ссылку на неё необходимо добавить в меню. 
+Ссылка в меню добавляется только после того, как страница полностью готова, наполнена содержимым.
+Инструкцию по дальнейшей работе со страницей вы можете найти здесь.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/landing**
+**https://portal.hse.ru/landing**
+Для входа в режим редактирования перейдите по ссылке «Редактору» с главной страницы сайта, нажмите наверху ссылку «Данные», после чего перейдите в раздел "Блоки" (русская версия) и "Блоки_англ" (английская версия).
+**https://portal.hse.ru/landing**
+ Быстрые ссылки  Шапка Меню Основная колонка Виджеты  
+**https://portal.hse.ru/landing**
+**Шапка**
+В данном разделе редактируется то, что размещается в шапке сайта (картинка, заголовок, подзаголовок, кнопки).
+При выборе картинки в шапку имейте в виду, что соотношение сторон при разном разрешении экрана будет меняться, поэтому значимая часть изображения (если есть) должна находиться по центру. Размер изображения ­— 1600 пикселей по ширине, вес — 200-300 кб. Изображения, заливаемые на портал, должны быть оптимизированы для веб, для этого можно воспользоваться, например, сервисом https://tinypng.com/. Если у проекта есть свой фирстиль, который должен быть отражен в шапке, то необходимо учитывать требования к картинке.
+Чтобы шапка отображалась не только на главной, но и на внутренних страницах сайта, нужно зайти в раздел «Шапка на вторых страницах» и выбрать: «Шапка с главной страницы» или «Своя шапка». Обычно для показа на внутренних страницах сайта используется «Шапка с главной страницы».
+**Меню**
+Отображение меню регулируется в разделе «Шапка». По умолчанию меню скрыто. Если нужно, чтобы оно показывалось, надо выбрать, где вы хотите его вывести — «снизу» или «сверху».
+Есть также опция сделать меню «по центру». Сами пункты меню редактируются в Данные-Блоки-Меню
+**Основная колонка**
+«Основная колонка главной страницы» — главный раздел, которым вы пользуетесь. Слева расположен набор виджетов, справа — поле, куда виджет нужно переместить и где будет располагаться ваш контент.
+Выбираем виджет, подходящий для информации, которую необходимо разместить на странице, цепляем его курсором в левой колонке и тянем мышкой вправо, в большую центральную колонку. Нажимаем «Сохранить» в конце страницы и обязательно проверяем, что получилось!
+**Текст**
+ Для размещения текста нужно выбрать виджет «Фрагмент текста с заголовком».  После вставки текста его нужно обязательно выделить и нажать на панели инструментов кнопку Tx для очистки лишнего кода. Далее необходимо разбить текст на абзацы, для этого можно использовать клавишу Enter. Чтобы текст лучше смотрелся в браузере (были удалены лишние пробелы, стояли кавычки «елочки» и „лапки“, слова и цифры соединяли тире, а не дефисы), используйте программу «Типограф». 
+**Изображения**
+ Вы можете разместить как одиночное изображение, так и фотогалерею.  При загрузке изображений обязательно помните, что сначала их необходимо оптимизировать 
+**Видео**
+ Видео сначала необходимо разместить на Youtube. Затем выбираете виджет «Видео», ставите галочку «Стороннее видео», в поле URL проставляете ссылку вида: https://www.youtube.com/embed/pWeQh4ocVUk/. Чтобы получить такую ссылку, находясь непосредственно на Youtube, нажимаете на кнопку «Поделиться» (она располагается под видео). Выбираете самый первый вариант — «Встроить». У вас откроется окно, где слева будет видео, а справа — встраиваемый код. Копируете оттуда значение c embed и вставляете эту ссылку в виджет. Если необходимо, можно добавить заголовок.  
+**Якорь**
+ Якорем называется закладка на определенном месте страницы, предназначенная для создания перехода к ней по ссылке. Чтобы создать якорь, необходимо переместить виджет «Якорь» в нужное место и прописать в нем латинскими буквами «имя якоря» (напр: anchor). В ссылке, по которой пользователь будет переходить в определенное место страницы, в поле «адрес» нужно прописать ссылку на страницу плюс имя якоря с символом решетки (#) впереди (напр: https://portal.hse.ru/#anchor).  
+**Цветные блоки**
+ Для оформления контента в виде цветных блоков нужно выбрать одноименный виджет. Регулируете количество блоков в строке — их может быть 2 или 3, нажимаете на кнопку «добавить», открывается окно, в котором вы прописывает заголовок, ссылку, боковое меню (если нужно), а также загружаете фоновую фотографию.  Пример:  
+**Новости**
+ Новости размещаются в разделе «Новости», см. инструкцию. При этом, чтобы они показывались на странице, их нужно вывести с помощью виджета «Новости», выбрав оформление «Плитки». Если вы хотите, чтобы заголовок раздела выводился, вам нужно вписать слово «Новости» в поле «Заголовок».  Пример:  
+**Мероприятия (анонсы)**
+ Анонсы размещаются в разделе «Анонсы», см. инструкцию. При этом, чтобы анонсы показывались на странице, их нужно вывести с помощью виджета «Мероприятия», выбрав стиль «Карточки». Если вы хотите, чтобы заголовок раздела выводился, вам нужно вписать слово «Мероприятия» в поле «Заголовок».  Пример:  
+**Связанные материалы**
+ Если нужно вынести на главную страницу материалы, которые связаны между собой какой-то общей темой, вы можете воспользоваться виджетом «Связанные материалы». Например, у вас есть несколько интервью выпускников или студентов, вы ставите их фотографии (предварительно вырезав), подписи (ФИО, м.б. также краткий заголовок интервью) и ссылку.  Пример:  
+**Список персон**
+ Информацию о персонах можно представить на странице разными способами. Горизонтальный список Перемещаете виджет «Список персон». Заполняете поле «Заголовок». Выбираете вид «Список». Нажимаете «Добавить персону». Если персона из ВШЭ, то вводите ФИО, нажимаете «Найти» и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение «Из ВШЭ» на «Не из ВШЭ». Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете «Вырезать», чтобы выбрать область фотографии, которая будет показываться на странице. Это необходимо сделать, чтобы показывалось именно круглое фото, а не овальное. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL  Пример:  Вертикальный список Перемещаете виджет «Список персон». Заполняете поле «Заголовок». Выбираете вид «Список». Проставляете галочку «Отображать вертикальным списком». Нажимаете «Добавить персону». Если персона из ВШЭ, то вы вводите ФИО, нажимаете «Найти» и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. В поле «Описание/контакты» добавляете необходимую информацию. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение «Из ВШЭ» на «Не из ВШЭ». Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете «Вырезать», чтобы выбрать область фотографии, которая будет показываться на странице. Это необходимо сделать, чтобы показывалось именно круглое фото, а не овальное. В поле «Описание/контакты» добавляете необходимую информацию. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL  Пример:  Одиночное круглое большое фото Если вам нужно разместить одиночное большое фото с подписью и текстом, вы выбираете виджет «Список персон», заполняете поле «Заголовок», далее выбираете вид «Одиночный», стиль «Большое фото». Если персона из ВШЭ, то вы вводите ФИО, нажимаете «Найти» и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. В поле «Описание/контакты» добавляете необходимую информацию. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение «Из ВШЭ» на «Не из ВШЭ». Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете «Вырезать», чтобы выбрать область фотографии, которая будет показываться на странице. В поле «Описание/контакты» добавляете необходимую информацию. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL.  Пример:  Круглое большое фото в колонках Если вы хотите разместить несколько подряд круглых фото в колонке, то перемещаете сначала виджет «Строка с колонками», а потом непосредственного в него добавляете виджет «Список персон». Выставляете ширину колонки «4», если вы хотите 3 персоны в ряд. Выставляете ширину колонки «3», если вы хотите 4 персоны в ряд. В сумме ширина всех колонок должна быть равна числу «12». Остальные действия — те же, что при размещении одиночного круглого фото.  Пример:  Карусель Если у вас много персон, и вы хотите, чтобы они выстраивались в один ряд, то выбираете виджет «Список персон», заполняете поле «Заголовок», далее выбираете вид «Карусель». Нажимаете «Добавить персону». Если персона из ВШЭ, то вы вводите ФИО, нажимаете «Найти» и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение «Из ВШЭ» на «Не из ВШЭ». Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете «Вырезать», чтобы выбрать область фотографии, которая будет показываться на странице. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL  Пример:  
+**Хронология**
+ С помощью виджета «Хронология» можно создать таймлайн или пошаговую инструкцию. Перемещаете из левой колонки виджет «Хронология». Если нужно сделать пошаговую инструкцию, то ставите галочку возле слова «Нумерация». Выбираете цвет, далее нажимаете «Добавить запись». В появившемся окне вписываете заголовок и текст, далее нажимаете опять «Добавить запись» за пределами окна. Если вам нужно добавить плашки (они выстраиваются в колонки), то нажимаете «Добавить запись» внутри окна.  Пример:    
+**Партнеры**
+ Чтобы разместить логотипы партнеров, нужно переместить из левой колонки виджет «Партнеры», заполнить поле «Заголовок», загрузить логотип, поставить ссылку и написать название компании-партнера. Логотипы встают в колонки по 4 в строке.  Пример:  
+**Колонки**
+ Если нужно разместить информацию в колонки, пожалуйста, не создавайте таблицу, пользуйтесь виджетом «Строка с колонками». У колонки нужно задать ширину. В сумме ширина всех колонок должна быть равна числу «12». Далее внутрь этого виджета нужно вставить другой виджет, в который вы будете непосредственно размещать информацию. Например, виджет «Фрагмент текста с заголовком».  Пример:  
+**Контент-блок**
+ Если необходимо разбить текст на смысловые части, наложив текст на фон (цвет или картинка), то надо воспользоваться виджетом «Контент-блок». Переносите виджет, добавляете цвет или картинку, внутрь переносите еще один виджет, в который непосредственно будете размещать информацию — например, виджет «Фрагмент текста с заголовком».  Пример:  
+**Соцсети**
+ Если необходимо разместить иконки социальных сетей, нужно переместить из левой колонки виджет «Соцсети», нажать «Добавить запись», заполнить поле «Заголовок», поставить ссылку на соцсеть, а также выбрать из перечня нужную вам иконку. При необходимости иконки можно расположить по центру, поставив соответствующую галочку.  Пример:  
+**Плашка**
+ Для выделения значимых пунктов в тексте можно воспользоваться виджетом «Плашка с цифрой». Перемещаете виджет в центральную колонку, заполняете поле Заголовок (раздела), выбираете цвет цифры, ставите галочку около «Нумерация», нажимаете «Добавить запись». Внутри заполняете поле «Заголовок» (если нужно) и поле «Текст». Пример:  Можено сделать плашки без цифры, тогда вы не ставите галочку около «Нумерация». Пример:  Плашки можно поставить в колонки. Тогда предварительно нужно переместить виджет «Строка с колонками» (о том, как это сделать смотрите выше), а потом в него переместить виджет «Плашка с цифрой». Пример:  
+**Даты**
+ Когда нужно красиво оформить даты мероприятия, воспользуйтесь виджетом «Связанные события». После того как вы переместили виджет, нажимаете «Добавить запись», далее заполняете поля «Число», «Месяц» и «Текст». Если вы хотите, чтобы между датами стояли стрелки, ставите галочку «Показывать стрелку».  Пример:  
+**Цифра**
+ Если в тексте нужно разместить блок со значимыми цифрами, то вы выбираете виджет «Цифра дня», перемещаете его, выбираете цвет цифры и текста и заполняете необходимые поля.  Пример:  
+**Выпадайки**
+ Если нужно разместить раскрывающийся цветной блок, то вы выбираете виджет «Набор с выпадайками». Нажимаете кнопку «Добавить блок», проставляете заголовок, в поле «Описание» ставите текст, который будет показываться до скрытого текста, в поле «Открывающийся текст» вписываете текст, который будет открываться по клику. Далее выбираете цвет блока.  Пример:  Если вам нужно просто сделать выпадающий список, то вы выбираете виджет «Набор с выпадайками 2». Нажимаете кнопку «Добавить блок», в поле «Заголовок» вписываете текст, по которому будут кликать, в поле «Открывающийся текст» вписываете текст, который будет открываться по клику.  Пример:  
+**Кнопка**
+ Если вам нужно создать кнопку, например «Регистрация», вы выбираете виджет «Декоратор», выбираете опцию «Кнопка», размещаете название кнопки и ссылку на страницу, на которую кнопка должна вести.  Пример:  
+**Часто задаваемые вопросы**
+ Если вам нужно создать блок «Часто задаваемые вопросы», то вы выбираете виджет «Декоратор», выбираете опцию «Часто задаваемые вопросы». Заполняете поля «Вопрос» и «Ответ». Далее нажимаете «Добавить». В открывшемся поле заполняете название кнопки и ссылку на страницу, куда кнопка должна вести. Кнопок может быть несколько. Кнопку можно сделать как с заливкой, так и прозрачной.  Пример:  Чтобы разместить все вопросы на странице, надо выбрать виджет «Вопросы и ответы (FAQ)», нажать «Добавить вопрос» и заполнить поля «Вопрос» и «Ответ».  Пример:  
+**Вкладки**
+ Если вы хотите разместить информацию в виде переключающихся между собой блоков, то нужно выбрать виджет «Вкладки». Далее вы нажимаете «Добавить вкладку», в поле «Заголовок» пишите название вкладки, в пустое поле перемещаете виджет «Фрагмент текста с заголовком», где и размещаете информацию.  Пример:  
+**Слайдер**
+ Инструкцию по размещению баннера в виджете «Слайдер» вы можете прочитать здесь. 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/header-banner**
+**Простой вариант**
+Состоит из текста и фонового изображения. Фон должен быть таким, чтобы на нем хорошо читался текст белого цвета. На фоне не должно быть значимых элементов, которые нельзя обрезать или пересекать текстом. Ширина фонового изображения – 1600px. Картинка обязательно должна быть оптимизирована: https://portal.hse.ru/photo
+**Сложный вариант – используется, когда у проекта есть свой фирстиль**
+Баннер/шапка представляет из себя композицию из 3 (или меньше) основных элементов:
+1. Фон (пример: заливка цветом, паттерн).
+2. Значимый текст (пример: заголовки, название мероприятия, опциональные кнопки).
+3. Графический элемент (пример: логотип, иллюстрация, фото).
+При подготовке макета, важно предусмотреть его адаптацию (размеры и взаимное расположение основных элементов) для разной ширины экрана. Макеты направляются команде портала в 3-х вариантах с шириной:
+1. 375px для мобильных устройств;
+2. 800px для планшетов;
+3. 1600px для пк и ноутбуков.
+Высота баннера на главной странице портала: 600px; 180px сверху и 80px снизу – служебные поля, в которых может быть размещен только фон.
+Высота шапки в лендинге: 490px; 45px сверху и 50px снизу – служебные поля, в которых может быть размещен только фон.
+Для верстки сложного варианта баннера/шапки следует прислать послойную картинку. Это означает, что отдельные элементы лежат на разных слоях изображения и верстальщик может использовать их отдельно друг от друга.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/slider_banners**
+**https://portal.hse.ru/slider_banners**
+Баннеры размещаются на главной странице сайта. Это не просто элемент оформления «чтобы было повеселее». Баннер призван обратить внимание посетителя на какой-то контент. Например, ссылка с баннера может вести на анонс конференции или новость о крупном проекте.
+**https://portal.hse.ru/slider_banners**
+ Заголовок. Несколько слов, кратко и емко описывающих тему. Если заголовок будет слишком длинным, вместе с текстом анонса он может не поместиться на мобильной версии.
+Анонс. Более детально раскрывает тему баннера. Задается обычным шрифтом, поэтому его длина может быть больше, чем у заголовка.
+ Как на мобильной версии скрыть часть анонса Если вы видите, что на экране мобильного текст анонса не помещается полностью, оберните его в тэг &lt;span class="is-desktop"&gt;и этот текст будет скрыт для мобильных&lt;/span&gt;. Если нужно наоборот, отображать какой-то фрагмент текста только на мобильном и скрывать для больших экранов, используйте &lt;span class="is-mobile"&gt;…текст…&lt;/span&gt; 
+**https://portal.hse.ru/slider_banners**
+**Как оформить баннер**
+Существует два варианта оформления баннера: заливка цветом и фоновая картинка.
+По умолчанию редактор предлагает стиль Amethyst и другие градиентные фоны. Вы можете выбрать тот, который наиболее подходит под цвет вашего сайта. Старайтесь избегать кричащих цветов.
+Если вы хотите использовать в качестве фона картинку, то в поле «Стиль» выбираете «Свой баннер»
+Фон сплешки. Это фоновая фотография баннера. Выбирая изображение, ориентируйтесь на фотостиль Вышки. Размер: обычные пропорции горизонтально ориентированного фото 1600 px по ширине. Перед загрузкой картинки необходимо оптимизировать. Подробно о том, почему важно оптимизировать фото, можно прочитать здесь.  На этой странице вы найдете ссылки на бесплатные фотобанки и фотографии нашего университета. Используя их, вы можете быть уверены, что не нарушаете авторские права. На баннерах нельзя размещать изображения с готовым текстом — с большой вероятностью он будет обрезаться на различных устройствах. Похожая рекомендация относится к композиции: следует следить, чтобы на экране мобильного отображались все значимые части фотографии или иллюстрации. Если фоновое фото достаточно светлое и текст на нем теряется, его можно затемнить.
+ Как затемнить фоновое изображение Можно воспользоваться программой Photoshop или бесплатным онлайн-фотошопом. Открываем изображение в программе, выбираем в верхнем меню — Изображение — Коррекция — Кривые или используем горячие клавиши Ctrl + M. Далее с помощью изменения точек кривой затемняем изображение до нужного уровня. 
+Стили CSS. В этом поле можно установить позиционирование фонового баннера на странице. Чем меньше значение, тем ниже будет изображение. Значение первого класса (в примере выше это .vp) должно быть уникальным для каждого баннера и написанным на латинице. Так, .vp — cокращение от «Высший пилотаж». Используйте следующий код, заменив первое значение:
+.vp.splash.pseudo { background-position: 50% 25%; }
+CSS класс. Чтобы стили работали, скопируйте значение первого класса из Стилей CSS, но без точки (в примере это vp).
+Темный текст. Устанавливаете, если фон сплешки светлый.
+**https://portal.hse.ru/slider_banners**
+**Как скрыть/удалить баннер**
+Если вам нужно скрыть баннер, делаете его неактивным, убрав галочку «Слайд активен». Чтобы совсем удалить неактуальный баннер, необходимо нажать на крестик в правом углу и сохранить изменения.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/tools**
+Многие из вас используют в своей работе фото и видео с изображениями университета. Дирекция по связям с общественностью подготовила и собрала фото- и видеоконтент, который показывает наши корпуса, учебный процесс и передает всю атмосферу Вышки.
+На YouTube-канале вы можете найти плейлист с имиджевыми роликами (экскурсия по зданиям, летающий видеогид по Покровке, ролик про университетские лаборатории, вопросы ученым и многое другое).
+Также можно воспользоваться фотографиями университета. На странице love.hse размещены варианты обоев/фонов для зума и стикерпаки.
+А на этой странице собраны ссылки на зарекомендовавшие себя бесплатные онлайн-инструменты, которые могут облегчить работу редактора с сайтами корпоративного портала. Большая часть этих сервисов используется сотрудниками Дирекции по порталу и мобильным приложениям  в повседневной работе, однако необходимо иметь в виду, что сотрудники дирекции не осуществляют их поддержку, в том числе не имеют возможности консультировать по их использованию. Если вы пользуетесь удобным ресурсом, о котором мы еще не знаем, присылайте информацию на адрес dkoptubenko@hse.ru.
+**Обработка фотографий**
+Colordot — инструмент для определения HTML-кода для требуемого цвета. В отличие от аналогов имеет визуально удобную палитру
+Pixlr — не только обработка фото для тех, у кого под рукой нет фотошопа и аналогов. Здесь удобно делать коллажи из нескольких изображений
+TinyPNG — один из проверенных инструментов для сжатия изображений перед публикацией их на сайте
+**Бесплатные фотобанки**
+Unsplash — изумительной красоты фотографии, в основном, видовые
+Gratisography — бесплатные жанровые фотографии
+StockSnap.io — каждую неделю сервис пополняется сотнями новых разрешенных к свободному использованию изображений
+Picjumbo — платный ресурс, но часть фотографий можно брать оттуда за просто так
+Picography — небольшая по объему коллекция бесплатных фотографий
+Library of Congress — исторические фотографии из коллекции Библиотеки Конгресса США. Перед использованием каждой фотографии прочитайте, распространяется ли на нее право использования без разрешения
+Morguefile — в основном пользовательские фотографии невысокого качества, но иногда встречаются превосходные снимки
+Textures — подборка паттернов и фоновых изображений
+L+T — альтернативный сервис по подборке фоновых изображений
+FreeStockTextures — более 800 паттернов
+TextureZoom — тематические текстуры
+**Решения для инфографики**
+draw.io — интерактивные блок-схемы мы создаем при помощи этого инструмента
+easelly — простой в употреблении сервис инфографики. Следует обратить внимание, что не все русскоязычные шрифты отображаются так, как задумывалось
+MyBalsamiq — сервис для создания прототипов. Можно использовать для взаимодействия с иллюстраторами
+**Визуальные решения для сайта**
+StoryMap — с его помощью можно создавать интерактивные карты.
+Juxtapose — элегантный инструмент для демонстрации изменений на однотипных объектах. С помощью слайдера пользователь может сравнить, как было, и как стало. Подобные инструменты активно применяются СМИ для демонстрации изменений, например, при реконструкции домов или улиц, снятых с одного ракурса
+Timeline JS — с его помощью можно создавать таймлайны (интерактивные истории, растянутые во времени). На портале использовался, например, при создании страницы к 20-летию нижегородского кампуса
+Soundcite — инструмент для создания аудиопрезентаций
+Prezi — мощная альтернатива Powerpoint для создания презентаций
+Fliphtml5 — инструмент для размещения pdf-файлов в виде раскрытой книги с возможностью листания страниц мышкой. Единственный известный нам стабильный бесплатный инструмент подобного рода.
+Формулы — инструмент для отображения формул на сайте. 
+**Создание опросов**
+Google Формы — бесплатный генератор опросов. Может пригодиться, если вам нужно провести опрос за периметром портала. Для формирования опросных или регистрационных форм на портале есть штатный инструмент
+**Работа с соцсетями**
+ВКонтакте pages.clearCache —  инструмент ВКонтакте, позволяющий сбросить кэш соцсети для конкретной ссылки. После этого соцсеть запросит новые данные с искомой страницы и учтет внесенные на нее изменения
+vk.com/cc — инструмент для генерации коротких ссылок для «ВКонтакте»
+SMMPlanner — отложенный постинг в социальные сети
+Ezgif — создание gif-изображений из видеозаписей, а также их редактура (изменение размеров, обрезка и так далее)
+Make Beliefs Comix — создание комиксов
+**Оптимизация файлов**
+Онлайн-инструменты для любителей PDF — полностью бесплатные онлайн-инструменты для объединения, разделения, сжатия PDF-файлов, преобразования документов Office в PDF-файлы, преобразования PDF-файлов в JPG и JPG в PDF. Без необходимости установки.
+**Узнать больше**
+Tutorialspoint — обширный набор учебников и инструкций: как пользоваться MS Word, Powepoint, Excel и сотнями других программ и приложений
+html academy — на сайте есть отличный бесплатный базовый курс по html и css, «настольная книга» для каждого, кто имеет доступ к редактированию страниц на портале
+Codecademy — интерактивные курсы по программированию
+https://smmplanner.com/
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/nov**
+**https://portal.hse.ru/nov**
+ Быстрые ссылки  Создание новости Предосмотр новости Составной редактор Иллюстрация новости Копирование на другой сайт  
+**https://portal.hse.ru/nov**
+Раздел «Новости» предусматривает размещение репортажей о прошедших мероприятиях, сообщений о получении наград, профессиональном и общественном признании образовательных программ (для мегафакультетов), преподавателей и т.п.
+ Новость обязательно должна содержать: заголовок, краткую аннотацию, текст новости, рубрику, ключевые слова, при желании текст новости может сопровождаться иллюстрациями. 
+Недопустимо размещение английских текстов в русской версии сайта и русских текстов в английской версии! (Инструкция по размещению английских новостей в новостной ленте)
+Не надо размещать в ленту новостей анонсы мероприятий! Если вы не уверены, куда размещать информацию (в «Новости» или «Анонсы»), зайдите на главную страницу портала, там разделение на новости и анонсы представлено достаточно наглядно.
+Если у вас возникают вопросы технического характера по размещению новостей, пишите на portal@hse.ru.
+**Создание новости**
+Для добавления новости необходимо зайти в Редактору — Данные — Новости. Новая запись добавляется кликом по иконке  .
+Заголовок: кратко указывается самая суть события. Заголовок должен быть назывным и кратким. Не надо в заголовок ставить несколько предложений или одно длинное предложение с большим количеством подробностей. Примеры длины заголовков можно посмотреть в главной ленте портала. В заголовке не употребляются слова "внимание!", "важная информация", "дорогие друзья!" и т.д. Точка в конце заголовка не ставится. CapsLock (все заглавные буквы) не используем.
+Аннотация: (должна быть обязательно!) краткое изложение того, о чём читатель узнает из статьи. 2-3 предложения.
+Текст: (должен быть обязательно!) непосредственно тело новости. Подробно раскрывает суть события. Новость не может состоять из одного предложения, фотографий без подробного сопроводительного текста.
+Дублировать аннотацию в поле "Текст" не нужно! Если ваша аннотация повторяет первый абзац текста новости, вы ставите напротив поля «Отображать аннотацию» — «Нет».
+При копировании текста из Word и вставке его на сайт необходимо в обязательном порядке чистить формат.
+Обязательно выбираете рубрику и ключевые слова.
+Если имеющиеся рубрики не соответствуют тематике вашего сайта, напишите на portal@hse.ru, пришлите список необходимых рубрик, и мы заведем их специально для вашего сайта.
+Если необходимо, вы можете выбрать тип материала/статус новости/сферу деятельности (выбирайте то, что действительно соответствует содержанию новости). Эти разделы были разработаны для главной ленты hse.ru. Если они не подходят для новостей вашего подразделения, вы их пропускаете.
+Ключевые слова выбирайте в соответствии с содержанием вашей новости. Они в дальнейшем позволяют делать выборку новостей по тем или иным темам внутри вашего сайта.
+Ключевые слова и рубрики нужны для того, чтобы читатели могли по ним найти нужную или интересную им новость. Поэтому надо выбирать только те рубрики и ключевые слова, которые соответствуют тематике новости, иначе это будет просто набор рубрик и ключевых слов, по которым вашу новость не найдут.
+Необходимо нажать на «добавить ключевое слово», вписать необходимое вам слово, нажать «поиск», а затем на выбранное слово или словосочетание. Если вы не нашли нужного ключевого словам, вы можете ввести его в самостоятельно, и оно попадет в базу ключевых слов (настоятельная просьба: прежде чем это сделать, убедитесь, что нужное вам ключевое слово действительно отсутствует).
+**Предосмотр новости**
+Прежде чем выводить новость в ленту вашего сайта, посмотрите, пожалуйста, что у вас получилось. Для этого вам нужно воспользоваться функцией «Предосмотр». Ссылка расположена в редакторском интерфейсе рядом с заголовком новости.
+**Составной редактор**
+Если в новости вам требуется использовать сложную верстку, то вы можете воспользоваться составным редактором. Для этого в поле «Тип редактора» выбираем «составной»:
+Далее следуем инструкции по составной странице.
+**Иллюстрация новости**
+Обратите внимание, что картинки, используемые в новостях и на сайте в целом, должны размещаться с соблюдением закона об авторских правах. Т.е. это должны быть фото, либо сделанные непосредственно сотрудниками/студентами, либо приобретённые в фотоагентствах. Фото/картинки, найденные случайным образом на просторах интернета, недопустимы к размещению!
+Фото не является обязательным элементом новости. Фотография должна быть горизонтальной и быть хорошего качества. Если картинка плохого качества или она не несёт никакой смысловой нагрузки, не нужно загружать её в новость! Не нужно загружать в качестве иллюстрации новости на главной странице сайта сканы, скриншоты, баннеры, постеры, обложки, логотипы, портретные фото (где крупно одно лицо).
+Чтобы картинка появилась в ленте новостей вашего сайта, ее нужно загрузить в «Сплеш-картинка для новости», размер фото 1083*722:
+Если вы собираетесь разместить несколько изображений, надо воспользоваться опцией «Фотоальбом». Нажимаете кнопку «Добавить изображение», выбираете нужный файл и далее сохраняете новость. Либо вы можете воспользоваться функционалом составного редактора.
+Обратите ваше внимание, что все фото, размещаемые на портале, необходимо оптимизировать.
+**Копирование на другой сайт**
+Чтобы воспользоваться этой функцией, необходимо залогиниться на портале. После этого открываем нужную вам новость. Ссылка «Разместить в подразделении» находится справа от заголовка, если зайти в полный текст новости.
+В списке подразделений отображаются все подразделения, на которые у редактора есть права редактирования. Здесь нужно выбрать необходимое и затем нажать кнопку «Импортировать».
+Разместить новость можно двумя способами – «Ссылкой на оригинальную новость» и «Полным клонированием». В первом случае на сайте вашего подразделения появится лишь заголовок и аннотация, которые будут уводить на оригинальную новость. Вы не сможете ее редактировать. Во втором случае новость целиком копируется на сайт вашего подразделения, Вы сможете ее редактировать. Однако надо иметь в виду, что все изменения, которые будут вноситься в оригинальную новость, в вашей отражаться не будут. Например, если добавится перевод на английский язык, к новости, размещенной через «полное клонирование», он не подтянется.
+Если Вам необходимо убрать новость, размещенную «Ссылкой на оригинальную новость», Вам необходимо зайти в раздел «Новости» – «Импортированные новости» (ссылка справа), найти нужную новость, нажать слева на иконку «карандаш», далее нажать на «Убрать новость из подразделения».
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t xml:space="preserve">**https://portal.hse.ru/instann**
 **https://portal.hse.ru/instann**
@@ -944,528 +1438,11 @@
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/format**
-**https://portal.hse.ru/format**
- Быстрые ссылки  Оформление Вставка текста Списки Заголовки Якорь Вставка картинки/фото Загрузка файлов Вставка таблицы  
-**https://portal.hse.ru/format**
-**Оформление**
- Все элементы форматирования и оформления придуманы не просто так. Любая страница сайта должна иметь правильную структуру, которая определённым образом обрабатывается браузерами и поисковыми системами. Чем проще, логичнее и понятнее структура страницы, тем быстрее она открывается (загружается), тем правильнее она индексируется поисковыми роботами (что влияет на выдачу сайта в поисковых системах). Не надо создавать пустые страницы (и выводить их в меню), страницы для размещения ссылки на другую страницу, страницы для размещения одного или нескольких файлов – это плохо влияет на имидж вашего сайта, а также на его индексацию в поисковых системах. Не надо задавать красную строку, выравнивать текст по ширине, по центру, по левому краю, по правому краю. Данный тип верстки не используется на веб-страницах. Например, при веб-верстке выравнивание по ширине приводит к тому, что слова расползаются, появляются большие интервалы. Внимательно также следите за тем, чтобы не было наследуемых из Word двойных пробелов.  Не надо использовать дополнительное форматирование текста. Оформление должно быть строго в корпоративном стиле. Не должно быть лишних подчёркиваний (в веб-верстке это выглядит как гиперссылка, которая никуда не ведет), выделения информации множеством восклицательных знаков, принудительного увеличения размера шрифта, изменения стиля шрифта или раскрашивания текста в разные цвета. Пожалуйста, пользуйтесь штатными инструментами форматирования. Для более интересного оформления можно воспользоваться виджетами, которые есть в функционале составной страницы. Если что-то не получается или не знаете, как оформить, пишите на portal@hse.ru 
-**Вставка текста**
-При копировании информации из документа Microsoft Word используйте следующую последовательность действий:
-1) Скопируйте текст из документа и нажмите на значок вставки информации из word файла. Вставьте скопированные материалы в открывшемся окне и нажмите «Вставить»;
-2) Выделите весь вставленный текст в поле и затем последовательно нажмите значок очистки лишнего кода и очистки формата;
-3) Удалите лишние пробелы и переносы строк;
-4) Разбейте текст на абзацы. Для этого необходимо выделить весь текст и выбрать «Абзац» на панели редактирования:
-Чтобы разбить текст на абзацы, можно также использовать сочетание клавиш Shift+Enter. 
-Если текст вставлен из Word некорректно, всё форматирование, отображающееся в редакторском интерфейсе, может пропасть или отображаться неправильно на готовой странице. Лучше всего форматировать тексты не в текстовых редакторах (Word), а непосредственно в визуальном редакторе.
-**Списки**
-Существует возможность создать как нумерованный, так и маркированный список. Для этого необходимо выделить текст и нажать на соответствующие кнопки на панели инструментов.
-Получается:
-   маркированный список маркированный список    нумерованный список нумерованный список  
-**Заголовки**
-Когда на странице размещён текст большого объёма, и его необходимо разбить на логические части (структурировать), название каждой такой части можно оформить элементом "Заголовок".
- Предусмотрены 6 уровней заголовков:
-**Заголовок 2**
-**Заголовок 3**
-**Заголовок 4**
-Заголовки используются последовательно, по мере понижения значимости информации. 
-Заголовок 1 — заголовок первого уровня, самый важный, который используется в поле "Заголовок страницы" при отображении готовой страницы (не нужно в поле "Заголовок страницы" принудительно выбирать "Заголовок 1"). На странице нельзя использовать несколько заголовков первого уровня! Поэтому в поле "Текст" оформлять какой-либо заголовок стилем "Заголовок 1" не нужно.
-Для выделения информации одинаковой значимости в рамках одной страницы используются заголовки одинакового уровня (например, "Заголовок 3"). Если внутри такого заголовка необходим подзаголовок, для его оформления используется заголовок четвёртого уровня ("Заголовок 4"). Крайне не желательно пропускать уровни заголовков. Например, если для заголовка используется "Заголовок 3", для подзаголовка должен использоваться "Заголовок 4", а не "Заголовок 5" или "Заголовок 6".
-Заголовки — важный элемент для поисковых систем! Они задают правильную структуру страницы. "Заголовком" нельзя оформлять отдельные предложения или абзацы. 
-**Якорь**
-Якорем называется закладка на определенном месте страницы, предназначенная для создания перехода к ней по ссылке. Якоря удобно применять в документах большого объема, чтобы можно было быстро переходить к нужному разделу.
-Чтобы создать якорь, необходимо поставить курсор в соответствующем месте страницы, на панели инструментов нажать на значок "якорь", в открывшемся окне прописать латинскими буквами "имя якоря" (напр: anchor), нажать "вставить".
-Если ссылку на якорь нужно разместить на той же странице, где сделан якорь, необходимо нажать на значок "ссылка" на панели инструментов, в поле "якоря" выбрать соответствующее имя якоря, далее нажать "вставить".
-Если ссылку на якорь нужно разместить на другой странице, то необходимо нажать на значок "ссылка" на панели инструментов, в поле "адрес" прописать ссылку на страницу с якорем, а также имя якоря с символом решетки (#) впереди (напр: https://portal.hse.ru/format#anchor), нажать "вставить".
-**Вставка картинки/фото**
-При загрузке изображений обращайте внимание на его размер. Чем шире изображение, тем больше места оно занимает на странице. Изменить размер изображения можно непосредственно при его загрузке.
-1. Нажимаем кнопку "Загрузка и вставка картинки"
-2. Ждём загрузки изображения. Переходим на вкладку "Положение", поле "Размер". Первая цифра — размер в пикселях по ширине, вторая — размер в пикселях по высоте.
-3. Если размер изображения по ширине и высоте устраивает, нажимаем вставить.
-4. В том случае, если при размещении картинки она занимает слишком много места (непосредственно в редакторском интерфейсе или на готовой странице при её сохранении), в редакторском интерфейсе кликаем на картинку левой кнопкой мыши (тем самым выбирая изображение), после того, как на границах изображения появилась рамка, кликаем правой кнопкой мыши. В появившемся меню выбираем пункт "Добавить/изменить изображение".
-5. В открывшемся окне снова выбираем вкладку "Положение" и меняем размеры картинки. Нажимаем кнопку "Обновить".
-Если Вы собираетесь разместить несколько изображений на странице, лучше воспользоваться опцией «Фотоальбом» (внизу страницы).  Нажимаете кнопку «Добавить изображение», выбираете нужный файл и далее сохраняете страницу.  
-****
-**Загрузка файлов**
-Для размещения файлов на странице необходимо воспользоваться кнопкой  на панели редактирования:
-После этого откроется диалоговое окно загрузки файла:
-В поле "Выберите файл" выбираем нужный файл (желательно, чтобы в имени файла были латинские буквы и между словами не было пробелов). В поле "Название" обязательно указываем название файла! Именно это название будет выводиться на сайте и использоваться для поиска по порталу и в поисковых системах. Обратите внимание на то, что у загружаемого файла должно быть внятное название без сокращений, многоточий и т.п. Нельзя называть файл "Регламент исп-я...тем...технич-го рег-та" и т.п. Пользователь ничего не поймет из подобного названия.
-Нажимаем кнопку "Загрузить". После того как файл загрузится, вид окна изменится. Для вставки файла на страницу нажимаем "Вставить":
-После того как файл появился в редакторском интерфейсе, его название при необходимости можно поправить.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/tables**
- Быстрые ссылки  Копирование таблицы из Word и Excel Создание таблицы в визуальном редакторе Специальные шаблоны для создания таблицы  
-**Копирование таблицы из Word и Excel**
-В том случае, если Вы копируете таблицу из Word или Excel, необходимо пользоваться инструментами очистки лишнего кода и форматирования.
-Сначала нужно воспользоваться кнопкой "очистка стилей таблицы":
-Далее необходимо использовать "метелку" и "ластик" для очистки формата текста.
-Если таблица будет вставлена некорректно, она будет некорректно отображаться на экранах компьютеров и мобильных устройств.
- Оформление должно быть в строгом корпоративном стиле! Не надо задавать красную строку, выравнивать текст по ширине, по центру, по левому краю, по правому краю. Выравнивание по ширине применяется только при книжной верстке, где есть переносы, при веб-верстке переносы отсутствуют и выравнивание по ширине приводит к тому, что слова расползаются, появляются большие интервалы. Внимательно следите за тем, чтобы не было двойных пробелов, лишних подчёркиваний, выделения информации множеством восклицательных знаков и путем раскрашивания текста во все цвета радуги. 
-**Создание таблицы в визуальном редакторе**
-Создавать таблицы лучше непосредственно в визуальном редакторе статической страницы. Для создания таблицы кликните на иконку 
-В появившемся окне укажите необходимое количество строк и столбцов. При необходимости отметьте флажок «Заголовок ячейки». В этом случае у первой строчки таблицы ячейки будут объединены. В момент первоначального создания таблицы не рекомендуем задавать границы таблицы, поскольку в этом случае в визуальном редакторе границы таблицы отображаться не будут (хотя при сохранении страницы и при просмотре её в обычном режиме все границы отобразятся).
-После заполнения необходимых полей нажимаем кнопку «Вставить». После этого работа с таблицей в редакторском интерфейсе происходит так же, как в любом текстовом редакторе. Правой кнопкой мышки либо при помощи кнопок работы с таблицей можно добавлять и удалять строки, объединять и разбивать ячейки, устанавливать ширину и высоту строк (в случае, если это действительно необходимо).
-Если вы в самом начале работы с таблицей не поставили значение границы, а границы для данной таблицы необходимы, то задать их можно двумя способами: 1) ставим курсор в любом месте таблицы, кликаем правой кнопкой мышки, в появившемся контекстном меню выбираем «Параметры таблицы», в поле «Граница» проставляем значение толщины границ (1 – практически универсальный размер границ); 2) ставим курсор в любом месте таблицы и снова нажимаем на иконку создания таблицы. В появившемся окошке в поле «Граница» проставляем значение толщины границ (1 – практически универсальный размер границ).
-**Специальные шаблоны для создания таблиц**
-Таблицу можно также добавить через «специальные шаблоны». Нажмите на кнопку добавления специального элемента.
-Строка данных включает в себя заголовок и 2 строки с данными, значения и их расшифровка. Можно разместить до 6 столбцов с возможностью их объединения.
-Блок данных представляет из себя несколько колонок с информацией, максимальное количество колонок также равно 6.
-Воздушная таблица отделена от верхнего контента на странице линией, при наведении на строку таблицы будет изменяться ее цвет.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/pages**
-Перейдите в раздел «Страницы» верхнего меню в режиме редактирования сайта.
-Создайте страницу, кликнув по иконке 
-При заполнении поля «Заголовок» не используйте форматирование текста, не разбивайте текст на строки, не вставляйте в поле картинки. Если вы копируете в это поле текст из Word, обязательно очистите форматирование. Это поле предназначено исключительно для текста, а форматирование в любом случае не будет отражено на готовой странице!
-Техническое имя страницы (поле «Путь») указывается только латинскими строчными буквами. Желательно, чтобы техническое имя состояло из одного слова. Если необходимо использовать два слова в названии страницы, ни в коем случае нельзя делать пробелы между словами — «help managers». Должно быть: либо «help_managers», либо «help/managers».
-Нельзя создавать пустые страницы, страницы для размещения ссылки на другую страницу, страницы для размещения одного-единственного файла.
-Английские версии русских страниц должны иметь такие же технические имена, как и русскоязычные страницы. Единственное отличие — при создании английской страницы в поле «Язык» необходимо проставить значение «английский».
-В рамках одного сайта не должно быть статических страниц с одинаковым адресом (поле "Путь") на одном языке!
-После того как вы наполнили страницу, прописали у нее техническое имя, вам необходимо сохранить страницу.
-После сохранения страница будет доступна по адресу: адрес-главной-страницы-сайта/путь. Например, у данной страницы адрес: https://portal.hse.ru/pages/, где https://portal.hse.ru/ — адрес главной страницы сайта, pages — путь страницы.
-Чтобы на страницу могли заходить пользователи, ссылку на неё необходимо добавить в меню. 
-Ссылка в меню добавляется только после того, как страница полностью готова, наполнена содержимым.
-Инструкцию по дальнейшей работе со страницей вы можете найти здесь.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/sostav**
-Для создания составной статической страницы необходимо проделать все те же шаги, что и для создания простой статической страницы. После заполнения основных полей переходим к полю "Вид страницы" (расположено над полем "Текст"). По умолчанию флажок установлен в положение "Простая". Кликаем на него и выбираем "Составная":
-Слева расположены виджеты, отвечающие за формат размещения информации в том или ином блоке: текст, фото, видео... Справа — непосредственно поле для размещения виджетов и, соответственно, информации.
-Выбираем виджет, подходящий для информации, которую необходимо разместить на странице, цепляем его курсором в левой колонке и тянем мышкой вправо, в большую центральную колонку. 
-Внутри центральной части страницы в редакторском интерфейсе все виджеты можно легко менять местами, просто перетягивая их мышью, удалять ненужные и добавлять новые.
-После размещения необходимой информации нажимаем "Сохранить" и обязательно проверяем, что получилось!
-**ВИДЖЕТЫ:**
-**Текст**
- Для размещения текста нужно выбрать виджет "Фрагмент текста с заголовком".  После вставки текста его нужно обязательно выделить и нажать на панели инструментов кнопку Tx для очистки лишнего кода. Далее необходимо разбить текст на абзацы, для этого можно использовать клавишу Enter. В остальном принципы оформления текста те же, что и на простой статической странице. 
-**Изображения**
- Вы можете разместить как одиночное изображение, так и фотогалерею.  При загрузке изображений обязательно помните, что сначала их необходимо оптимизировать 
-**Видео**
- Видео сначала необходимо разместить на Youtube. Затем выбираете виджет "Видео", ставите галочку "Стороннее видео", в поле URL проставляете ссылку вида: https://www.youtube.com/embed/pWeQh4ocVUk/. Чтобы получить такую ссылку, находясь непосредственно на Youtube, нажимаете на кнопку «Поделиться» (она располагается под видео). Выбираете самый первый вариант – «Встроить». У вас откроется окно, где слева будет видео, а справа – встраиваемый код. Копируете оттуда значение c embed и вставляете эту ссылку в виджет. Если необходимо, можно добавить заголовок.  
-**Якорь**
- Якорем называется закладка на определенном месте страницы, предназначенная для создания перехода к ней по ссылке. Чтобы создать якорь, необходимо переместить виджет "Якорь" в нужное место и прописать в нем латинскими буквами "имя якоря" (напр: anchor). В ссылке, по которой пользователь будет переходить в опеределенное место страницы, в поле "адрес" нужно прописать ссылку на страницу плюс имя якоря с символом решетки (#) впереди (напр: https://portal.hse.ru/#anchor).  
-**Цветные блоки**
- Для оформления контента в виде цветных блоков нужно выбрать одноименный виджет. Регулируете количество блоков в строке – их может быть 2 или 3, нажимаете на кнопку "добавить", открывается окно, в котором вы прописывает заголовок, ссылку, боковое меню (если нужно), а также загружаете фоновую фотографию.  Пример:  
-**Связанные материалы**
- Если нужно вынести на главную страницу материалы, которые связаны между собой какой-то общей темой, вы можете воспользоваться виджетом "Связанные материалы". Например, у вас есть несколько интервью выпускников или студентов, вы ставите их фотографии (предварительно вырезав), подписи (ФИО, м.б. также краткий заголовок интервью) и ссылку.  Пример:  
-**Список персон**
- Информацию о персонах можно представить на странице разными способами. Горизонтальный список Перемещаете виджет "Список персон". Заполняете поле "Заголовок". Выбираете вид "Список". Нажимаете "Добавить персону". Если персона из ВШЭ, то вводите ФИО, нажимаете "Найти" и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение «Из ВШЭ» на "Не из ВШЭ". Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете "Вырезать", чтобы выбрать область фотографии, которая будет показываться на странице. Это необходимо сделать, чтобы показывалось именно круглое фото, а не овальное. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL  Пример:  Вертикальный список Перемещаете виджет "Список персон". Заполняете поле "Заголовок". Выбираете вид "Список". Проставляете галочку "Отображать вертикальным списком". Нажимаете "Добавить персону". Если персона из ВШЭ, то вы вводите ФИО, нажимаете "Найти" и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. В поле "Описание/контакты" добавляете необходимую информацию. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение "Из ВШЭ" на "Не из ВШЭ". Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете "Вырезать", чтобы выбрать область фотографии, которая будет показываться на странице. Это необходимо сделать, чтобы показывалось именно круглое фото, а не овальное. В поле "Описание/контакты" добавляете необходимую информацию. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL  Пример:  Одиночное круглое большое фото Если вам нужно разместить одиночное большое фото с подписью и текстом, вы выбираете виджет "Список персон", заполняете поле "Заголовок", далее выбираете вид "Одиночный", стиль "Большое фото". Если персона из ВШЭ, то вы вводите ФИО, нажимаете "Найти" и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. В поле "Описание/контакты" добавляете необходимую информацию. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение "Из ВШЭ" на "Не из ВШЭ". Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете "Вырезать", чтобы выбрать область фотографии, которая будет показываться на странице. В поле "Описание/контакты" добавляете необходимую информацию. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL.  Пример:  Круглое большое фото в колонках Если вы хотите разместить несколько подряд круглых фото в колонке, то перемещаете сначала виджет "Строка с колонками", а потом непосредственного в него добавляете виджет "Список персон". Выставляете ширину колонки "4", если вы хотите 3 персоны в ряд. Выставляете ширину колонки "3", если вы хотите 4 персоны в ряд. В сумме ширина всех колонок должна быть равна числу "12". Остальные действия – те же, что при размещении одиночного круглого фото.  Пример:  Карусель Если у вас много персон, и вы хотите, чтобы они выстраивались в один ряд, то выбираете виджет "Список персон", заполняете поле "Заголовок", далее выбираете вид "Карусель". Нажимаете "Добавить персону". Если персона из ВШЭ, то вы вводите ФИО, нажимаете "Найти" и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение "Из ВШЭ" на "Не из ВШЭ". Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете "Вырезать", чтобы выбрать область фотографии, которая будет показываться на странице. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL  Пример:  
-**Хронология**
- С помощью виджета "Хронология" можно создать таймлайн или пошаговую инструкцию. Перемещаете из левой колонки виджет "Хронология". Если нужно сделать пошаговую инструкцию, то ставите галочку возле слова "Нумерация". Выбираете цвет, далее нажимаете "Добавить запись". В появившемся окне вписываете заголовок и текст, далее нажимаете опять "Добавить запись" за пределами окна. Если вам нужно добавить плашки (они выстраиваются в колонки), то нажимаете "Добавить запись" внутри окна.  Пример:    
-**Партнеры**
- Чтобы разместить логотипы партнеров, нужно переместить из левой колонки виджет "Партнеры", заполнить поле "Заголовок", загрузить логотип, поставить ссылку и написать название компании-партнера. Логотипы встают в колонки по 4 в строке.  Пример:  
-**Колонки**
- Если нужно разместить информацию в колонки, пожалуйста, не создавайте таблицу, пользуйтесь виджетом "Строка с колонками". У колонки нужно задать ширину. В сумме ширина всех колонок должна быть равна числу "12". Далее внутрь этого виджета нужно вставить другой виджет, в который вы будете непосредственно размещать информацию. Например, виджет "Фрагмент текста с заголовком".  Пример:  
-**Соцсети**
- Если необходимо разместить иконки социальных сетей, нужно переместить из левой колонки виджет "Соцсети", нажать "Добавить запись", заполнить поле "Заголовок", поставить ссылку на соцсеть, а также выбрать из перечня нужную вам иконку. При необходимости иконки можно расположить по центру, поставив соответствующую галочку.  Пример:  
-**Плашка**
- Для выделения значимых пунктов в тексте можно воспользоваться виджетом "Плашка с цифрой". Перемещаете виджет в центральную колонку, заполняете поле Заголовок (раздела), выбираете цвет цифры, ставите галочку около "Нумерация", нажимаете "Добавить запись". Внутри заполняете поле "Заголовок" (если нужно) и поле "Текст". Пример:  Можно сделать плашки без цифры, тогда вы не ставите галочку около "Нумерация". Пример:  Плашки можно поставить в колонки. Тогда предварительно нужно переместить виджет "Строка с колонками" (о том, как это сделать смотрите выше), а потом в него переместить виджет "Плашка с цифрой". Пример:  
-**Даты**
- Когда нужно красиво оформить даты мероприятия, воспользуйтесь виджетом "Связанные события". После того как вы переместили виджет, нажимаете "Добавить запись", далее заполняете поля "Число", "Месяц" и "Текст". Если вы хотите, чтобы между датами стояли стрелки, ставите галочку "Показывать стрелку".  Пример:  
-**Цифра**
- Если в тексте нужно разместить блок со значимыми цифрами, то вы выбираете виджет "Цифра дня", перемещаете его, выбираете цвет цифры и текста и заполняете необходимые поля.  Пример:  
-**Выпадайки**
- Если нужно разместить раскрывающийся цветной блок, то вы выбираете виджет "Набор с выпадайками". Нажимаете кнопку "Добавить блок", проставляете заголовок, в поле "Описание" ставите текст, который будет показываться до скрытого текста, в поле "Открывающийся текст" вписываете текст, который будет открываться по клику. Далее выбираете цвет блока.  Пример:  Если вам нужно просто сделать выпадающий список, то вы выбираете виджет "Набор с выпадайками 2". Нажимаете кнопку "Добавить блок", в поле "Заголовок" вписываете текст, по которому будут кликать, в поле "Открывающийся текст" вписываете текст, который будет открываться по клику.  Пример:  
-**Кнопка**
- Если вам нужно создать кнопку, например "Регистрация", вы выбираете виджет "Декоратор", выбираете опцию "Кнопка", размещаете название кнопки и ссылку на страницу, на которую кнопка должна вести.  Пример:  
-**Часто задаваемые вопросы**
-   Чтобы разместить все вопросы на странице, надо выбрать виджет "Вопросы и ответы (FAQ)", нажать "Добавить вопрос" и заполнить поля "Вопрос" и "Ответ".  Пример:  
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/photo**
-Почему это важно? Во многом трафик на ваш сайт и, как следствие, степень интереса к вашим продуктам и результатам деятельности, зависит от скорости загрузки страниц. Вот что о некоторых страницах портала думает искусственный интеллект:
-Вы можете сами проверить свой сайт с помощью этого инструмента.
-Как с этим бороться? Прежде всего, тщательно следя за тем, чтобы загружаемые вами на портал фотографии не были чрезмерно тяжелыми. Помните, что размер фотографий вес фотографии только отчасти зависит от ее размера в пикселях. И самое маленькое изображение может весить более чем достаточно, если оно хорошего качества.
- Для начала уменьшите изображение до нужных размеров. Это можно сделать в любом графическом редакторе. Если у вас нет на компьютере установленной программы, вы можете воспользоваться, например, онлайн-сервисом Photoshop Express или Pixlr. Самая широкая картинка на портале не превышает 1600 пикселей по ширине. Ориентируйтесь на эту ширину как на максимальную. Оптимизируйте изображение с помощью сервиса Tinypng. Это очень просто. Заходите на сайт и перетаскиваете изображение в специальный контейнер прямо на сайте. После вам останется только скачать обратно на свой компьютер сжатую картинку. Теперь ее можно использовать на портале. 
-Можно, конечно, продолжать работать с сайтом, не оптимизируя изображения. Но в таком случае нужно помнить, что это повлечет за собой потерю части посетителей вашего сайта, прежде всего самых продвинутых, заходящих в интернет с мобильного телефона, а также потенциальных клиентов из ряда зарубежных стран, где скорость интернета оставляет желать лучшего. Команда портала, со своей стороны, прикладывает все усилия, чтобы оптимизировать другие элементы страниц технологическими средствами.
-Чтобы узнать, какие изображения из числа тех, что уже размещены на вашем сайте, нуждаются в оптимизации, воспользуйтесь сервисом Google PageSpeed Insights. Зайдите на страницу сервиса, введите адрес страницы, которую нужно проверить, дождитесь результата, найдите вкладку «Оптимизируйте изображения». Например, для главной страницы портала она выглядит так:
-А для главной страницы типичной образовательной программы – так:
-Разница в объеме потенциально оптимизируемого – в 17 раз.
-Вы можете оптимизировать уже размещенные на сайте изображения с помощью встроенных инструментов Google PageSpeed Insights. Для этого внизу страницы с результатами обследования вашей страницы найдите ссылку «Скачать оптимизированные изображения, ресурсы JavaScript и CSS для этой страницы».
-К вам на компьютер будет скачан архив, в одной из папке которого будут содержаться ужатые изображения. Их необходимо опубликовать на вашем сайте взамен тех, которые там были ранее.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/instev**
-Вход в редакторский режим https://www.hse.ru/adm/  Логин и пароль такие же как, от вашего личного кабинета (ЕЛК).
-**Оформление главной страницы**
-Основные вкладки, с которыми Вы будете работать, — это «Страницы» (создание и редактирование статических страниц сайта), «Опросы» (создание формы регистрации на мероприятие) и «Блоки».
-Основное управление контентом происходит во вкладке «Блоки» («Блоки (англ.)» — для английской версии сайта).
-Чтобы Вам было легче сориентироваться, в редакторском интерфейсе есть пояснения к разным полям для внесения информации, отмеченные звездочками или серым шрифтом.  
-**1 — 5 пункт заполняется в Блоки — Правая колонка — Данные о мероприятии.**
-**1. Заголовок**
-Рекомендуется заполнять оба верхних поля. Текст первой строки отображается мелким шрифтом. Тогда как текст — основное название мероприятия — отображается крупно.
-**2. Даты мероприятия3. Кнопка регистрации (ссылка на регистрацию)**
-Создание формы регистрации.
-**4. Ключевые даты**
-Заполняется в поле «Пояснение». Надпись «Важные даты» может варьироваться по усмотрению.
-**5. Место проведения, Контакты**
-В этой же вкладке Вы можете заполнять и использовать все другие поля. «Время начала мероприятия», «Языки мероприятия», ссылка на карту «Как добраться», «Важные ссылки», «Файлы» — все эти данные будут отображаться в правой части сайта.
-**6. Меню (горизонтальное) в центральной части страницы**
-**Блоки — Настройки — Меню**
-Необходимо создать новую группу, а внутри группы «Добавить ссылку», где первая строка — название пункта меню, вторая — ссылка на страницу (создание и редактирование статических страниц).
-Для того чтобы пункты меню выстраивались в горизонтальную линию, необходимо под каждый пункт меню создавать новую группу. При добавлении ссылки в той же группе, следующий пункт меню будет располагаться под предыдущим.
-Возможен еще один вариант расположения меню — в правой части сайта под датой мероприятия (см. рисунок ниже).
-По логике заполнения и редактирования правой части сайта, данные пункты вносятся в
-**Блоки — Правая колонка — Данные о мероприятии — Важные ссылки.**
-**Оформление аннотации/главной страницы сайта мероприятия**
-Информация, которая размещается на главной странице сайта, является ключевой и должна отражать важность проводимого мероприятия.
-Для заполнения/редактирования аннотации необходимо зайти в редакторский интерфейс главной страницы: любо через https://www.hse.ru/adm/ — Данные, либо с помощью значка «Редактору» в нижнем правом углу главной страницы.
-Аннотация находится в поле «О подразделении» и верстается по аналогии с версткой текста на статических страницах, с использованием такого же инструментария.
-**Оформление нижней части сайта мероприятия**
-Внизу главной страницы Вы можете разместить членов программного или организационного комитета, ключевых спикеров, докладчиков, партнеров и пр. с фото, регалиями и ссылками на персоны.
-**Это делается в Блоки — Подвал — Участники**
-Внутри Вы заводите соответствующую группу («Ключевые спикеры», например) и поочередно добавляете персон. Ссылка на персональную страницу и фотография сотрудников Вышки подгружается автоматически. Для персон не из ВШЭ Вы можете подгружать фото и ссылку в открывшемся окне вручную.
-По аналогичному принципу устроен пункт оформления партнеров мероприятия.
-**Блоки — Подвал — Партнеры**
-где необходимо добавлять логотип организации-партнера и ссылку на них.
-Однако зачастую бывает удобнее размещать партнеров в правой части сайта.
-Здесь снова работает логика работы с правой колонкой.
-**Блоки — Правая колонка — Текстовые блоки**
-Необходимо завести новый текстовый блок и заполнить его картинками-логотипами и, при желании, ссылками на сайты партнеров.
-**Оформление программы мероприятия**
-Также у Вас есть возможность сверстать программу вашего мероприятия. Она будет располагаться на главной странице сайта мероприятия под аннотацией.
-**Данный инструмент находится в Блоки — Контент — Расписание мероприятий**
-Структуру программы Вы выстраиваете путем добавления пунктов «Добавить день», «Добавить мероприятие» или «Добавить событие», в зависимости от структуры и продолжительности вашего мероприятия.
-**Оформление страницы организационного комитета (программного комитета, докладчиков и др.).**
-Если Вы решили создать отдельную статическую страницу для перечисления членов организационного или программного комитетов, докладчиков и др., Вам необходимо использовать создать составную страницу и выбрать виджет "Список персон". Как это сделать, вы можете прочитать в инструкции: https://portal.hse.ru/sostav.
-И главное — не забывайте нажимать на кнопку «Сохранить» внизу каждой карточки, которую Вы заполняете.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/poll**
-**https://portal.hse.ru/poll**
- Быстрые ссылки  Создание формы Уведомления на свою почту Ответное письмо пользователю Ссылка на форму/клонирование/выгрузка результатов CRM-система  
-**https://portal.hse.ru/poll**
-**Создание формы**
-Для создания регистрационных форм, форм подписки на новости, опросов и др. необходимо на сайте вашего подразделения зайти в Редактору – Данные – Опросы и регистрационные формы.
-Нажимаем на +, чтобы создать форму.
-Далее нужно указать:
- название (если в названии используются длинные слова, вы можете поставить галочку расставить мягкие переносы); время проведения (тот период времени, в течение которого можно ответить на вопросы); статус (меняете на «активно» после того, как форма будет готова); язык (если форма на английском языке, необходимо выставить язык – «английский»). 
-Если у вас регистрация на мероприятие с ограниченным количеством участников, то существует возможность закрыть регистрацию после определенного количества заявок. В ином случае вы оставляете это поле незаполненным.
-Галочка «пройти можно только раз» нужна только в том случае, если вы создаете опрос.
-Галочка «автоматически нумеровать вопросы» стоит по умолчанию. Однако бывают случаи, когда автоматическая нумерация не нужна, – тогда галочку нужно убрать.
-Далее необходимо нажать на кнопку «Добавить блок вопросов».
-Если вам нужно разбить вопросы на несколько тематических блоков, то вы заполняете поле «Блок вопросов» (при необходимости также поле «Описание»).
-Пример блоков
-Если ваши вопросы должны идти подряд без разбивки на блоки, вы это поле не заполняете, а сразу переходите к кнопке «Добавить вопрос». В поле «Вопрос» вписываем непосредственно вопрос. В поле «Описание» можно добавить комментарии к вопросу.
-Далее нажимаем кнопку «Добавить ответ» и вписываем необходимый вариант.
-Если ответ на данный вопрос обязателен, ставим галочку напротив соответствующего пункта.
-Если на вопрос допускается один ответ, то выбираем соответствующую строку в поле «Формат ответа». Если на вопрос допускается несколько вариантов ответов, также выбираем соответствующую строку в поле «Формат ответа»
-Ответы можно сделать «выпадающим списком», тогда в поле «Формат ответа» нужно выбрать соответствующую строку.
-Если ответы не заданы, и тот, кто заполняет форму, должен вписать свой вариант ответа, в поле «Формат ответа» выбираем значение «Строка» или «Несколько строк». Вы можете добавить какой-то комментарий к свободному ответу в «Пояснительном тексте», а также ограничить в ответе количество символов.
-Если в ответе предполагается указание даты, номер телефона, e-mail, страны проживания или загрузка файла, то надо выбрать строку «Специальный вопрос» в поле «Формат ответа», а далее в выпадающем списке выбрать нужный вариант.
-Обратите внимание, что если вы выберете тип специального вопроса email, при заполнении формы браузер пользователя постарается автозаполнить это поле из кеша. Это облегчает пользователю заполнение формы. Автозаполнение из кеша браузера возможно также в отношении полей "Фамилия" (нужно выбрать Код вопроса "lastname") и имя (Код вопроса "firstname"). Автозаполнение не гарантируется, однако, как правило работает.
-После заполнения необходимо сохранить форму, нажав на кнопку «Создать».
-**https://portal.hse.ru/poll**
-**Дополнительные параметры**
-Чтобы открыть «Дополнительные параметры», необходимо нажать на стрелку.
-В открывшемся окне вы можете:
- Добавить к форме пояснительный текст (будет отображаться сразу после заголовка); Добавить сообщение на странице после отправки формы (будет выводится на экране, напр.: «Спасибо за регистрацию. Ждем вас по адресу...»); Добавить сообщение на странице по завершении регистрации (будет заменять стандартную фразу «Извините, регистрация закончена»); Изменить текст согласия на обработку персональных данных (используется только при необходимости заменить стандартный текст); 
-В разделе «Дополнительные параметры» вы также сможете:
- Поставить ссылку перехода после сохранения (надо иметь в виду, что если вы заполните это поле, сообщения типа «Спасибо за регистрацию» и «Регистрация завершена» выводиться не будут); Изменить схему показа вопросов (по умолчанию они идут друг за другом, схема «вопросы в виде таблицы» позволяет выстраивать их в две колонки); Привязать форму к определенному сайту (например, вы сделали ее на одном сайте, а вам нужно, чтобы форма была на другом, либо нужно привязать еще один сайт); Указать корпоративный e-mail сотрудника ВШЭ, на который будут приходить уведомления о новых ответах (каждый адрес должен быть добавлен отдельно, через кнопку «добавить»);  Связать с формой на другом языке (чтобы работала переключалка языков, если у вас есть такая же форма, например, на английском); 
-Если вы хотите, чтобы на почту пользователя приходило ответное письмо, надо поставить галочку напротив «Направить ответное письмо пользователю». Данная функция будет работать в том случае, если в форме нужно указывать email и ответ на этот вопрос обязателен. В поле «Текст письма» нужно разместить текст, а в коде вопроса про электронную почту надо прописать слово «email». Большая просьба в тексте письма указывать контактную информацию – куда пользователь может обратиться с вопросами, т.к. письма приходят с адреса robot@hse.ru.
-Если вы хотите, чтобы ответное письмо пользователю было персонализировано, то в поле «Текст письма» в начале нужно разместить фразу: Здравствуйте %%ANSWER_TO_QUESTION_lastname%% — %%ANSWER_TO_QUESTION_firstname%%. При этом необходимо, чтобы кроме e-mail, в вашей форме обязательными вопросами были отдельно «фамилия» и «имя» (или «имя-отчество»). В коде вопроса нужно прописать слова lastname и firstname.
-**https://portal.hse.ru/poll**
-**Ссылка на форму/Клонирование/Выгрузка ответов**
-Необходимо зайти в Редактору – Данные – Опросы и регистрационные формы и там вы сможете:
-1. Редактировать форму (чтобы сохранить изменения, нужно будет нажать кнопку «Сохранить»).
-2. Клонировать форму (если вам необходимо создать форму с теми же или похожими вопросами).
-3. Найти ссылку на форму (нажимаете на "встраивание", в открывшемся окне выбираете ссылку с названием вашего подразделения, чтобы форма открывалась внутри вашего сайта; кликаете на ссылку и в адресной строке открышегося окна копируете ссылку на вашу форму). Пример:
-4. Выгрузить ответы на форму (у вас есть возможность посмотреть результаты в pdf, html и excel).
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/landing**
-**https://portal.hse.ru/landing**
-Для входа в режим редактирования перейдите по ссылке «Редактору» с главной страницы сайта, нажмите наверху ссылку «Данные», после чего перейдите в раздел "Блоки" (русская версия) и "Блоки_англ" (английская версия).
-**https://portal.hse.ru/landing**
- Быстрые ссылки  Шапка Меню Основная колонка Виджеты  
-**https://portal.hse.ru/landing**
-**Шапка**
-В данном разделе редактируется то, что размещается в шапке сайта (картинка, заголовок, подзаголовок, кнопки).
-При выборе картинки в шапку имейте в виду, что соотношение сторон при разном разрешении экрана будет меняться, поэтому значимая часть изображения (если есть) должна находиться по центру. Размер изображения ­— 1600 пикселей по ширине, вес — 200-300 кб. Изображения, заливаемые на портал, должны быть оптимизированы для веб, для этого можно воспользоваться, например, сервисом https://tinypng.com/. Если у проекта есть свой фирстиль, который должен быть отражен в шапке, то необходимо учитывать требования к картинке.
-Чтобы шапка отображалась не только на главной, но и на внутренних страницах сайта, нужно зайти в раздел «Шапка на вторых страницах» и выбрать: «Шапка с главной страницы» или «Своя шапка». Обычно для показа на внутренних страницах сайта используется «Шапка с главной страницы».
-**Меню**
-Отображение меню регулируется в разделе «Шапка». По умолчанию меню скрыто. Если нужно, чтобы оно показывалось, надо выбрать, где вы хотите его вывести — «снизу» или «сверху».
-Есть также опция сделать меню «по центру». Сами пункты меню редактируются в Данные-Блоки-Меню
-**Основная колонка**
-«Основная колонка главной страницы» — главный раздел, которым вы пользуетесь. Слева расположен набор виджетов, справа — поле, куда виджет нужно переместить и где будет располагаться ваш контент.
-Выбираем виджет, подходящий для информации, которую необходимо разместить на странице, цепляем его курсором в левой колонке и тянем мышкой вправо, в большую центральную колонку. Нажимаем «Сохранить» в конце страницы и обязательно проверяем, что получилось!
-**Текст**
- Для размещения текста нужно выбрать виджет «Фрагмент текста с заголовком».  После вставки текста его нужно обязательно выделить и нажать на панели инструментов кнопку Tx для очистки лишнего кода. Далее необходимо разбить текст на абзацы, для этого можно использовать клавишу Enter. Чтобы текст лучше смотрелся в браузере (были удалены лишние пробелы, стояли кавычки «елочки» и „лапки“, слова и цифры соединяли тире, а не дефисы), используйте программу «Типограф». 
-**Изображения**
- Вы можете разместить как одиночное изображение, так и фотогалерею.  При загрузке изображений обязательно помните, что сначала их необходимо оптимизировать 
-**Видео**
- Видео сначала необходимо разместить на Youtube. Затем выбираете виджет «Видео», ставите галочку «Стороннее видео», в поле URL проставляете ссылку вида: https://www.youtube.com/embed/pWeQh4ocVUk/. Чтобы получить такую ссылку, находясь непосредственно на Youtube, нажимаете на кнопку «Поделиться» (она располагается под видео). Выбираете самый первый вариант — «Встроить». У вас откроется окно, где слева будет видео, а справа — встраиваемый код. Копируете оттуда значение c embed и вставляете эту ссылку в виджет. Если необходимо, можно добавить заголовок.  
-**Якорь**
- Якорем называется закладка на определенном месте страницы, предназначенная для создания перехода к ней по ссылке. Чтобы создать якорь, необходимо переместить виджет «Якорь» в нужное место и прописать в нем латинскими буквами «имя якоря» (напр: anchor). В ссылке, по которой пользователь будет переходить в определенное место страницы, в поле «адрес» нужно прописать ссылку на страницу плюс имя якоря с символом решетки (#) впереди (напр: https://portal.hse.ru/#anchor).  
-**Цветные блоки**
- Для оформления контента в виде цветных блоков нужно выбрать одноименный виджет. Регулируете количество блоков в строке — их может быть 2 или 3, нажимаете на кнопку «добавить», открывается окно, в котором вы прописывает заголовок, ссылку, боковое меню (если нужно), а также загружаете фоновую фотографию.  Пример:  
-**Новости**
- Новости размещаются в разделе «Новости», см. инструкцию. При этом, чтобы они показывались на странице, их нужно вывести с помощью виджета «Новости», выбрав оформление «Плитки». Если вы хотите, чтобы заголовок раздела выводился, вам нужно вписать слово «Новости» в поле «Заголовок».  Пример:  
-**Мероприятия (анонсы)**
- Анонсы размещаются в разделе «Анонсы», см. инструкцию. При этом, чтобы анонсы показывались на странице, их нужно вывести с помощью виджета «Мероприятия», выбрав стиль «Карточки». Если вы хотите, чтобы заголовок раздела выводился, вам нужно вписать слово «Мероприятия» в поле «Заголовок».  Пример:  
-**Связанные материалы**
- Если нужно вынести на главную страницу материалы, которые связаны между собой какой-то общей темой, вы можете воспользоваться виджетом «Связанные материалы». Например, у вас есть несколько интервью выпускников или студентов, вы ставите их фотографии (предварительно вырезав), подписи (ФИО, м.б. также краткий заголовок интервью) и ссылку.  Пример:  
-**Список персон**
- Информацию о персонах можно представить на странице разными способами. Горизонтальный список Перемещаете виджет «Список персон». Заполняете поле «Заголовок». Выбираете вид «Список». Нажимаете «Добавить персону». Если персона из ВШЭ, то вводите ФИО, нажимаете «Найти» и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение «Из ВШЭ» на «Не из ВШЭ». Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете «Вырезать», чтобы выбрать область фотографии, которая будет показываться на странице. Это необходимо сделать, чтобы показывалось именно круглое фото, а не овальное. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL  Пример:  Вертикальный список Перемещаете виджет «Список персон». Заполняете поле «Заголовок». Выбираете вид «Список». Проставляете галочку «Отображать вертикальным списком». Нажимаете «Добавить персону». Если персона из ВШЭ, то вы вводите ФИО, нажимаете «Найти» и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. В поле «Описание/контакты» добавляете необходимую информацию. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение «Из ВШЭ» на «Не из ВШЭ». Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете «Вырезать», чтобы выбрать область фотографии, которая будет показываться на странице. Это необходимо сделать, чтобы показывалось именно круглое фото, а не овальное. В поле «Описание/контакты» добавляете необходимую информацию. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL  Пример:  Одиночное круглое большое фото Если вам нужно разместить одиночное большое фото с подписью и текстом, вы выбираете виджет «Список персон», заполняете поле «Заголовок», далее выбираете вид «Одиночный», стиль «Большое фото». Если персона из ВШЭ, то вы вводите ФИО, нажимаете «Найти» и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. В поле «Описание/контакты» добавляете необходимую информацию. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение «Из ВШЭ» на «Не из ВШЭ». Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете «Вырезать», чтобы выбрать область фотографии, которая будет показываться на странице. В поле «Описание/контакты» добавляете необходимую информацию. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL.  Пример:  Круглое большое фото в колонках Если вы хотите разместить несколько подряд круглых фото в колонке, то перемещаете сначала виджет «Строка с колонками», а потом непосредственного в него добавляете виджет «Список персон». Выставляете ширину колонки «4», если вы хотите 3 персоны в ряд. Выставляете ширину колонки «3», если вы хотите 4 персоны в ряд. В сумме ширина всех колонок должна быть равна числу «12». Остальные действия — те же, что при размещении одиночного круглого фото.  Пример:  Карусель Если у вас много персон, и вы хотите, чтобы они выстраивались в один ряд, то выбираете виджет «Список персон», заполняете поле «Заголовок», далее выбираете вид «Карусель». Нажимаете «Добавить персону». Если персона из ВШЭ, то вы вводите ФИО, нажимаете «Найти» и выбираете нужного сотрудника из базы. Должность можно ввести вручную или выбрать из предлагаемого списка должностей. Фото и ссылка на личную страницу подтягиваются автоматически. Если персона не из ВШЭ, то вы меняете положение «Из ВШЭ» на «Не из ВШЭ». Вручную вписываете фио и должность. Загружаете фото. После заливки фото обязательно нажимаете «Вырезать», чтобы выбрать область фотографии, которая будет показываться на странице. Если необходимо поставить ссылку с ФИО, вы ставите ее в поле URL  Пример:  
-**Хронология**
- С помощью виджета «Хронология» можно создать таймлайн или пошаговую инструкцию. Перемещаете из левой колонки виджет «Хронология». Если нужно сделать пошаговую инструкцию, то ставите галочку возле слова «Нумерация». Выбираете цвет, далее нажимаете «Добавить запись». В появившемся окне вписываете заголовок и текст, далее нажимаете опять «Добавить запись» за пределами окна. Если вам нужно добавить плашки (они выстраиваются в колонки), то нажимаете «Добавить запись» внутри окна.  Пример:    
-**Партнеры**
- Чтобы разместить логотипы партнеров, нужно переместить из левой колонки виджет «Партнеры», заполнить поле «Заголовок», загрузить логотип, поставить ссылку и написать название компании-партнера. Логотипы встают в колонки по 4 в строке.  Пример:  
-**Колонки**
- Если нужно разместить информацию в колонки, пожалуйста, не создавайте таблицу, пользуйтесь виджетом «Строка с колонками». У колонки нужно задать ширину. В сумме ширина всех колонок должна быть равна числу «12». Далее внутрь этого виджета нужно вставить другой виджет, в который вы будете непосредственно размещать информацию. Например, виджет «Фрагмент текста с заголовком».  Пример:  
-**Контент-блок**
- Если необходимо разбить текст на смысловые части, наложив текст на фон (цвет или картинка), то надо воспользоваться виджетом «Контент-блок». Переносите виджет, добавляете цвет или картинку, внутрь переносите еще один виджет, в который непосредственно будете размещать информацию — например, виджет «Фрагмент текста с заголовком».  Пример:  
-**Соцсети**
- Если необходимо разместить иконки социальных сетей, нужно переместить из левой колонки виджет «Соцсети», нажать «Добавить запись», заполнить поле «Заголовок», поставить ссылку на соцсеть, а также выбрать из перечня нужную вам иконку. При необходимости иконки можно расположить по центру, поставив соответствующую галочку.  Пример:  
-**Плашка**
- Для выделения значимых пунктов в тексте можно воспользоваться виджетом «Плашка с цифрой». Перемещаете виджет в центральную колонку, заполняете поле Заголовок (раздела), выбираете цвет цифры, ставите галочку около «Нумерация», нажимаете «Добавить запись». Внутри заполняете поле «Заголовок» (если нужно) и поле «Текст». Пример:  Можено сделать плашки без цифры, тогда вы не ставите галочку около «Нумерация». Пример:  Плашки можно поставить в колонки. Тогда предварительно нужно переместить виджет «Строка с колонками» (о том, как это сделать смотрите выше), а потом в него переместить виджет «Плашка с цифрой». Пример:  
-**Даты**
- Когда нужно красиво оформить даты мероприятия, воспользуйтесь виджетом «Связанные события». После того как вы переместили виджет, нажимаете «Добавить запись», далее заполняете поля «Число», «Месяц» и «Текст». Если вы хотите, чтобы между датами стояли стрелки, ставите галочку «Показывать стрелку».  Пример:  
-**Цифра**
- Если в тексте нужно разместить блок со значимыми цифрами, то вы выбираете виджет «Цифра дня», перемещаете его, выбираете цвет цифры и текста и заполняете необходимые поля.  Пример:  
-**Выпадайки**
- Если нужно разместить раскрывающийся цветной блок, то вы выбираете виджет «Набор с выпадайками». Нажимаете кнопку «Добавить блок», проставляете заголовок, в поле «Описание» ставите текст, который будет показываться до скрытого текста, в поле «Открывающийся текст» вписываете текст, который будет открываться по клику. Далее выбираете цвет блока.  Пример:  Если вам нужно просто сделать выпадающий список, то вы выбираете виджет «Набор с выпадайками 2». Нажимаете кнопку «Добавить блок», в поле «Заголовок» вписываете текст, по которому будут кликать, в поле «Открывающийся текст» вписываете текст, который будет открываться по клику.  Пример:  
-**Кнопка**
- Если вам нужно создать кнопку, например «Регистрация», вы выбираете виджет «Декоратор», выбираете опцию «Кнопка», размещаете название кнопки и ссылку на страницу, на которую кнопка должна вести.  Пример:  
-**Часто задаваемые вопросы**
- Если вам нужно создать блок «Часто задаваемые вопросы», то вы выбираете виджет «Декоратор», выбираете опцию «Часто задаваемые вопросы». Заполняете поля «Вопрос» и «Ответ». Далее нажимаете «Добавить». В открывшемся поле заполняете название кнопки и ссылку на страницу, куда кнопка должна вести. Кнопок может быть несколько. Кнопку можно сделать как с заливкой, так и прозрачной.  Пример:  Чтобы разместить все вопросы на странице, надо выбрать виджет «Вопросы и ответы (FAQ)», нажать «Добавить вопрос» и заполнить поля «Вопрос» и «Ответ».  Пример:  
-**Вкладки**
- Если вы хотите разместить информацию в виде переключающихся между собой блоков, то нужно выбрать виджет «Вкладки». Далее вы нажимаете «Добавить вкладку», в поле «Заголовок» пишите название вкладки, в пустое поле перемещаете виджет «Фрагмент текста с заголовком», где и размещаете информацию.  Пример:  
-**Слайдер**
- Инструкцию по размещению баннера в виджете «Слайдер» вы можете прочитать здесь. 
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/header-banner**
-**Простой вариант**
-Состоит из текста и фонового изображения. Фон должен быть таким, чтобы на нем хорошо читался текст белого цвета. На фоне не должно быть значимых элементов, которые нельзя обрезать или пересекать текстом. Ширина фонового изображения – 1600px. Картинка обязательно должна быть оптимизирована: https://portal.hse.ru/photo
-**Сложный вариант – используется, когда у проекта есть свой фирстиль**
-Баннер/шапка представляет из себя композицию из 3 (или меньше) основных элементов:
-1. Фон (пример: заливка цветом, паттерн).
-2. Значимый текст (пример: заголовки, название мероприятия, опциональные кнопки).
-3. Графический элемент (пример: логотип, иллюстрация, фото).
-При подготовке макета, важно предусмотреть его адаптацию (размеры и взаимное расположение основных элементов) для разной ширины экрана. Макеты направляются команде портала в 3-х вариантах с шириной:
-1. 375px для мобильных устройств;
-2. 800px для планшетов;
-3. 1600px для пк и ноутбуков.
-Высота баннера на главной странице портала: 600px; 180px сверху и 80px снизу – служебные поля, в которых может быть размещен только фон.
-Высота шапки в лендинге: 490px; 45px сверху и 50px снизу – служебные поля, в которых может быть размещен только фон.
-Для верстки сложного варианта баннера/шапки следует прислать послойную картинку. Это означает, что отдельные элементы лежат на разных слоях изображения и верстальщик может использовать их отдельно друг от друга.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/nov**
-**https://portal.hse.ru/nov**
- Быстрые ссылки  Создание новости Предосмотр новости Составной редактор Иллюстрация новости Копирование на другой сайт  
-**https://portal.hse.ru/nov**
-Раздел «Новости» предусматривает размещение репортажей о прошедших мероприятиях, сообщений о получении наград, профессиональном и общественном признании образовательных программ (для мегафакультетов), преподавателей и т.п.
- Новость обязательно должна содержать: заголовок, краткую аннотацию, текст новости, рубрику, ключевые слова, при желании текст новости может сопровождаться иллюстрациями. 
-Недопустимо размещение английских текстов в русской версии сайта и русских текстов в английской версии! (Инструкция по размещению английских новостей в новостной ленте)
-Не надо размещать в ленту новостей анонсы мероприятий! Если вы не уверены, куда размещать информацию (в «Новости» или «Анонсы»), зайдите на главную страницу портала, там разделение на новости и анонсы представлено достаточно наглядно.
-Если у вас возникают вопросы технического характера по размещению новостей, пишите на portal@hse.ru.
-**Создание новости**
-Для добавления новости необходимо зайти в Редактору — Данные — Новости. Новая запись добавляется кликом по иконке  .
-Заголовок: кратко указывается самая суть события. Заголовок должен быть назывным и кратким. Не надо в заголовок ставить несколько предложений или одно длинное предложение с большим количеством подробностей. Примеры длины заголовков можно посмотреть в главной ленте портала. В заголовке не употребляются слова "внимание!", "важная информация", "дорогие друзья!" и т.д. Точка в конце заголовка не ставится. CapsLock (все заглавные буквы) не используем.
-Аннотация: (должна быть обязательно!) краткое изложение того, о чём читатель узнает из статьи. 2-3 предложения.
-Текст: (должен быть обязательно!) непосредственно тело новости. Подробно раскрывает суть события. Новость не может состоять из одного предложения, фотографий без подробного сопроводительного текста.
-Дублировать аннотацию в поле "Текст" не нужно! Если ваша аннотация повторяет первый абзац текста новости, вы ставите напротив поля «Отображать аннотацию» — «Нет».
-При копировании текста из Word и вставке его на сайт необходимо в обязательном порядке чистить формат.
-Обязательно выбираете рубрику и ключевые слова.
-Если имеющиеся рубрики не соответствуют тематике вашего сайта, напишите на portal@hse.ru, пришлите список необходимых рубрик, и мы заведем их специально для вашего сайта.
-Если необходимо, вы можете выбрать тип материала/статус новости/сферу деятельности (выбирайте то, что действительно соответствует содержанию новости). Эти разделы были разработаны для главной ленты hse.ru. Если они не подходят для новостей вашего подразделения, вы их пропускаете.
-Ключевые слова выбирайте в соответствии с содержанием вашей новости. Они в дальнейшем позволяют делать выборку новостей по тем или иным темам внутри вашего сайта.
-Ключевые слова и рубрики нужны для того, чтобы читатели могли по ним найти нужную или интересную им новость. Поэтому надо выбирать только те рубрики и ключевые слова, которые соответствуют тематике новости, иначе это будет просто набор рубрик и ключевых слов, по которым вашу новость не найдут.
-Необходимо нажать на «добавить ключевое слово», вписать необходимое вам слово, нажать «поиск», а затем на выбранное слово или словосочетание. Если вы не нашли нужного ключевого словам, вы можете ввести его в самостоятельно, и оно попадет в базу ключевых слов (настоятельная просьба: прежде чем это сделать, убедитесь, что нужное вам ключевое слово действительно отсутствует).
-**Предосмотр новости**
-Прежде чем выводить новость в ленту вашего сайта, посмотрите, пожалуйста, что у вас получилось. Для этого вам нужно воспользоваться функцией «Предосмотр». Ссылка расположена в редакторском интерфейсе рядом с заголовком новости.
-**Составной редактор**
-Если в новости вам требуется использовать сложную верстку, то вы можете воспользоваться составным редактором. Для этого в поле «Тип редактора» выбираем «составной»:
-Далее следуем инструкции по составной странице.
-**Иллюстрация новости**
-Обратите внимание, что картинки, используемые в новостях и на сайте в целом, должны размещаться с соблюдением закона об авторских правах. Т.е. это должны быть фото, либо сделанные непосредственно сотрудниками/студентами, либо приобретённые в фотоагентствах. Фото/картинки, найденные случайным образом на просторах интернета, недопустимы к размещению!
-Фото не является обязательным элементом новости. Фотография должна быть горизонтальной и быть хорошего качества. Если картинка плохого качества или она не несёт никакой смысловой нагрузки, не нужно загружать её в новость! Не нужно загружать в качестве иллюстрации новости на главной странице сайта сканы, скриншоты, баннеры, постеры, обложки, логотипы, портретные фото (где крупно одно лицо).
-Чтобы картинка появилась в ленте новостей вашего сайта, ее нужно загрузить в «Сплеш-картинка для новости», размер фото 1083*722:
-Если вы собираетесь разместить несколько изображений, надо воспользоваться опцией «Фотоальбом». Нажимаете кнопку «Добавить изображение», выбираете нужный файл и далее сохраняете новость. Либо вы можете воспользоваться функционалом составного редактора.
-Обратите ваше внимание, что все фото, размещаемые на портале, необходимо оптимизировать.
-**Копирование на другой сайт**
-Чтобы воспользоваться этой функцией, необходимо залогиниться на портале. После этого открываем нужную вам новость. Ссылка «Разместить в подразделении» находится справа от заголовка, если зайти в полный текст новости.
-В списке подразделений отображаются все подразделения, на которые у редактора есть права редактирования. Здесь нужно выбрать необходимое и затем нажать кнопку «Импортировать».
-Разместить новость можно двумя способами – «Ссылкой на оригинальную новость» и «Полным клонированием». В первом случае на сайте вашего подразделения появится лишь заголовок и аннотация, которые будут уводить на оригинальную новость. Вы не сможете ее редактировать. Во втором случае новость целиком копируется на сайт вашего подразделения, Вы сможете ее редактировать. Однако надо иметь в виду, что все изменения, которые будут вноситься в оригинальную новость, в вашей отражаться не будут. Например, если добавится перевод на английский язык, к новости, размещенной через «полное клонирование», он не подтянется.
-Если Вам необходимо убрать новость, размещенную «Ссылкой на оригинальную новость», Вам необходимо зайти в раздел «Новости» – «Импортированные новости» (ссылка справа), найти нужную новость, нажать слева на иконку «карандаш», далее нажать на «Убрать новость из подразделения».
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/slider_banners**
-**https://portal.hse.ru/slider_banners**
-Баннеры размещаются на главной странице сайта. Это не просто элемент оформления «чтобы было повеселее». Баннер призван обратить внимание посетителя на какой-то контент. Например, ссылка с баннера может вести на анонс конференции или новость о крупном проекте.
-**https://portal.hse.ru/slider_banners**
- Заголовок. Несколько слов, кратко и емко описывающих тему. Если заголовок будет слишком длинным, вместе с текстом анонса он может не поместиться на мобильной версии.
-Анонс. Более детально раскрывает тему баннера. Задается обычным шрифтом, поэтому его длина может быть больше, чем у заголовка.
- Как на мобильной версии скрыть часть анонса Если вы видите, что на экране мобильного текст анонса не помещается полностью, оберните его в тэг &lt;span class="is-desktop"&gt;и этот текст будет скрыт для мобильных&lt;/span&gt;. Если нужно наоборот, отображать какой-то фрагмент текста только на мобильном и скрывать для больших экранов, используйте &lt;span class="is-mobile"&gt;…текст…&lt;/span&gt; 
-**https://portal.hse.ru/slider_banners**
-**Как оформить баннер**
-Существует два варианта оформления баннера: заливка цветом и фоновая картинка.
-По умолчанию редактор предлагает стиль Amethyst и другие градиентные фоны. Вы можете выбрать тот, который наиболее подходит под цвет вашего сайта. Старайтесь избегать кричащих цветов.
-Если вы хотите использовать в качестве фона картинку, то в поле «Стиль» выбираете «Свой баннер»
-Фон сплешки. Это фоновая фотография баннера. Выбирая изображение, ориентируйтесь на фотостиль Вышки. Размер: обычные пропорции горизонтально ориентированного фото 1600 px по ширине. Перед загрузкой картинки необходимо оптимизировать. Подробно о том, почему важно оптимизировать фото, можно прочитать здесь.  На этой странице вы найдете ссылки на бесплатные фотобанки и фотографии нашего университета. Используя их, вы можете быть уверены, что не нарушаете авторские права. На баннерах нельзя размещать изображения с готовым текстом — с большой вероятностью он будет обрезаться на различных устройствах. Похожая рекомендация относится к композиции: следует следить, чтобы на экране мобильного отображались все значимые части фотографии или иллюстрации. Если фоновое фото достаточно светлое и текст на нем теряется, его можно затемнить.
- Как затемнить фоновое изображение Можно воспользоваться программой Photoshop или бесплатным онлайн-фотошопом. Открываем изображение в программе, выбираем в верхнем меню — Изображение — Коррекция — Кривые или используем горячие клавиши Ctrl + M. Далее с помощью изменения точек кривой затемняем изображение до нужного уровня. 
-Стили CSS. В этом поле можно установить позиционирование фонового баннера на странице. Чем меньше значение, тем ниже будет изображение. Значение первого класса (в примере выше это .vp) должно быть уникальным для каждого баннера и написанным на латинице. Так, .vp — cокращение от «Высший пилотаж». Используйте следующий код, заменив первое значение:
-.vp.splash.pseudo { background-position: 50% 25%; }
-CSS класс. Чтобы стили работали, скопируйте значение первого класса из Стилей CSS, но без точки (в примере это vp).
-Темный текст. Устанавливаете, если фон сплешки светлый.
-**https://portal.hse.ru/slider_banners**
-**Как скрыть/удалить баннер**
-Если вам нужно скрыть баннер, делаете его неактивным, убрав галочку «Слайд активен». Чтобы совсем удалить неактуальный баннер, необходимо нажать на крестик в правом углу и сохранить изменения.
-</t>
-        </is>
-      </c>
-    </row>
     <row r="20">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/tools**
-Многие из вас используют в своей работе фото и видео с изображениями университета. Дирекция по связям с общественностью подготовила и собрала фото- и видеоконтент, который показывает наши корпуса, учебный процесс и передает всю атмосферу Вышки.
-На YouTube-канале вы можете найти плейлист с имиджевыми роликами (экскурсия по зданиям, летающий видеогид по Покровке, ролик про университетские лаборатории, вопросы ученым и многое другое).
-Также можно воспользоваться фотографиями университета. На странице love.hse размещены варианты обоев/фонов для зума и стикерпаки.
-А на этой странице собраны ссылки на зарекомендовавшие себя бесплатные онлайн-инструменты, которые могут облегчить работу редактора с сайтами корпоративного портала. Большая часть этих сервисов используется сотрудниками Дирекции по порталу и мобильным приложениям  в повседневной работе, однако необходимо иметь в виду, что сотрудники дирекции не осуществляют их поддержку, в том числе не имеют возможности консультировать по их использованию. Если вы пользуетесь удобным ресурсом, о котором мы еще не знаем, присылайте информацию на адрес dkoptubenko@hse.ru.
-**Обработка фотографий**
-Colordot — инструмент для определения HTML-кода для требуемого цвета. В отличие от аналогов имеет визуально удобную палитру
-Pixlr — не только обработка фото для тех, у кого под рукой нет фотошопа и аналогов. Здесь удобно делать коллажи из нескольких изображений
-TinyPNG — один из проверенных инструментов для сжатия изображений перед публикацией их на сайте
-**Бесплатные фотобанки**
-Unsplash — изумительной красоты фотографии, в основном, видовые
-Gratisography — бесплатные жанровые фотографии
-StockSnap.io — каждую неделю сервис пополняется сотнями новых разрешенных к свободному использованию изображений
-Picjumbo — платный ресурс, но часть фотографий можно брать оттуда за просто так
-Picography — небольшая по объему коллекция бесплатных фотографий
-Library of Congress — исторические фотографии из коллекции Библиотеки Конгресса США. Перед использованием каждой фотографии прочитайте, распространяется ли на нее право использования без разрешения
-Morguefile — в основном пользовательские фотографии невысокого качества, но иногда встречаются превосходные снимки
-Textures — подборка паттернов и фоновых изображений
-L+T — альтернативный сервис по подборке фоновых изображений
-FreeStockTextures — более 800 паттернов
-TextureZoom — тематические текстуры
-**Решения для инфографики**
-draw.io — интерактивные блок-схемы мы создаем при помощи этого инструмента
-easelly — простой в употреблении сервис инфографики. Следует обратить внимание, что не все русскоязычные шрифты отображаются так, как задумывалось
-MyBalsamiq — сервис для создания прототипов. Можно использовать для взаимодействия с иллюстраторами
-**Визуальные решения для сайта**
-StoryMap — с его помощью можно создавать интерактивные карты.
-Juxtapose — элегантный инструмент для демонстрации изменений на однотипных объектах. С помощью слайдера пользователь может сравнить, как было, и как стало. Подобные инструменты активно применяются СМИ для демонстрации изменений, например, при реконструкции домов или улиц, снятых с одного ракурса
-Timeline JS — с его помощью можно создавать таймлайны (интерактивные истории, растянутые во времени). На портале использовался, например, при создании страницы к 20-летию нижегородского кампуса
-Soundcite — инструмент для создания аудиопрезентаций
-Prezi — мощная альтернатива Powerpoint для создания презентаций
-Fliphtml5 — инструмент для размещения pdf-файлов в виде раскрытой книги с возможностью листания страниц мышкой. Единственный известный нам стабильный бесплатный инструмент подобного рода.
-Формулы — инструмент для отображения формул на сайте. 
-**Создание опросов**
-Google Формы — бесплатный генератор опросов. Может пригодиться, если вам нужно провести опрос за периметром портала. Для формирования опросных или регистрационных форм на портале есть штатный инструмент
-**Работа с соцсетями**
-ВКонтакте pages.clearCache —  инструмент ВКонтакте, позволяющий сбросить кэш соцсети для конкретной ссылки. После этого соцсеть запросит новые данные с искомой страницы и учтет внесенные на нее изменения
-vk.com/cc — инструмент для генерации коротких ссылок для «ВКонтакте»
-SMMPlanner — отложенный постинг в социальные сети
-Ezgif — создание gif-изображений из видеозаписей, а также их редактура (изменение размеров, обрезка и так далее)
-Make Beliefs Comix — создание комиксов
-**Оптимизация файлов**
-Онлайн-инструменты для любителей PDF — полностью бесплатные онлайн-инструменты для объединения, разделения, сжатия PDF-файлов, преобразования документов Office в PDF-файлы, преобразования PDF-файлов в JPG и JPG в PDF. Без необходимости установки.
-**Узнать больше**
-Tutorialspoint — обширный набор учебников и инструкций: как пользоваться MS Word, Powepoint, Excel и сотнями других программ и приложений
-html academy — на сайте есть отличный бесплатный базовый курс по html и css, «настольная книга» для каждого, кто имеет доступ к редактированию страниц на портале
-Codecademy — интерактивные курсы по программированию
-https://smmplanner.com/
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
         <is>
           <t>**https://portal.hse.ru/progs**
 **О шаблоне «Сайт образовательной программы»**
@@ -1557,16 +1534,47 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/help**
+        		    Шаг 1
+Необходимо удостовериться, что ваша персональная страница появилась на сайте. Персональная страница появляется на портале автоматически после внесения данных в базу сотрудниками Управления персонала. 
+        		    Шаг 2
+Следует авторизоваться в Едином личном кабинете (ЕЛК). Для этого необходимо в качестве логина ввести адрес корпоративной почты сотрудника, в качестве пароля – пароль от этой почты.
+Если вы не помните пароль от своей почты или у вас возникает ошибка при авторизации, обращайтесь на digital@hse.ru
+        		    Шаг 3
+В ЕЛК нужно перейти в раздел «Корпоративный портал» и нажать на «Персональная страница портала». Если вы не сможете войти в редактирование персональной страницы, значит, ваш корпоративный e-mail не прописан в необходимом поле. Напишите, пожалуйста, на portal@hse.ru.
+В письме укажите:
+• ФИО сотрудника
+• Адрес корпоративной почты
+Служба портала пропишет e-mail, и вы сможете войти.
+Письмо должно быть отправлено строго с корпоративной почты сотрудника @hse.ru 
+</t>
+        </is>
+      </c>
+    </row>
     <row r="22">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">**https://portal.hse.ru/helpsite**
-Для получения доступа к  редактированию сайта необходимо направить заявку в свободной форме по электронному адресу portal@hse.ru. В заявке необходимо указать ФИО сотрудника и адрес сайта, к которому нужен доступ. 
-Для редактирования сайта необходимо иметь доступ в личный кабинет на портале.
-Заявка должна быть отправлена с корпоративного адреса электронной почты.
+          <t xml:space="preserve">**https://portal.hse.ru/newdesignbb**
+Чтобы включить доску объявлений на сайте образовательной программы, необходимо открыть блок «Доска объявлений» (Данные −&gt; Блоки) и поставить соответствующую галочку.
+В этом блоке можно добавить новые рубрики и фильтры. Обратите внимание, что по умолчанию доски объявлений содержат ряд типовых, часто встречающихся рубрик. Каждое объявление в обязательном порядке должно быть привязано хотя бы к одному фильтру (по умолчанию это курсы) и хотя бы к одной рубрике.
+Программам, которые имеют несколько специализаций, мы рекомендуем добавить дополнительный фильтр (не рубрику) «Специализации», чтобы иметь возможность публиковать объявления для студентов, обучающихся по разным трекам.Чтобы добавить новое объявление, в меню личного кабинета (hse.ru/user) в разделе «Мои задачи» редактор сайта образовательной программы должен выбрать пункт «Объявления на досках объявлений».
+На открывшейся странице будут доступны ссылки на добавление новых объявлений. Ниже находится список размещенных ранее объявлений (если таковые есть). 
+Обратите внимание: если вы являетесь редактором сайтов нескольких программ, то при создании нового объявления следует выбрать нужную доску из списка.
+Что не следует делать:
+Создавать фильтры и темы, не несущие смысловой нагрузки. К таким, например, относятся: «Важная информация», «Важно», «Не пропустите», «Всем».
+Использовать при написании заголовков только прописные (заглавные) буквы Неправильно: ОБНОВЛЕНО РАСПИСАНИЕ Правильно: Обновлено расписание
+Пренебрегать форматированием текста. Текст с большим количеством пробелов, интервалов и т.п. неудобно читать.
+Все материалы, связанные с образовательной программой, необходимо размещать на сайте этой программы. Например, расписание должно находиться на сайте образовательной программы, а не на сайте факультета.
+Инструкция по редактированию сайтов образовательных программ размещена здесь: http://portal.hse.ru/progs
 </t>
         </is>
       </c>
@@ -1671,68 +1679,6 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve">**https://portal.hse.ru/resp**
-На сайтах подразделений существует функционал, позволяющий подразделению самостоятельно формировать списки сотрудников, к которым можно обращаться по тем или иным вопросам.
-Списки показываются в справочнике сотрудника, а также в личном кабинете сотрудника.
-В настоящее время на сайте подразделения заведены следующие категории функциональной ответственности.
-Ответственные от факультетов и филиалов за редактирование страниц подразделений
-Ответственные за персональные страницы сотрудников
-Добавление в список ответственных автоматически не дает им доступ к редактированию сайта и персональных страниц. Для этого необходимо получить соответствующие права в подразделении, отвечающем за соответствующий ресурс.
-Управление по информационным ресурсам выдает права (заявка на адрес portal@hse.ru)
-Ответственным от факультетов и филиалов за редактирование страниц подразделений
-Ответственным за персональные страницы сотрудников
-**Как изменить сведения об ответственных**
-**Добавление сотрудника:**
-Необходимо перейти в режим редактирования сайта конкретного подразделения (раздел Данные). В блоке "Функционал сотрудника подразделения" нажать кнопку "Добавить сотрудника", вбить в поле для поиска ФИО, выбрать сотрудника и галочками выбрать возможные категории его ответственности.
-**Удаление сотрудника из списка**
-Для удаления сотрудника необходимо убрать все галки в списке функциональной ответственности сотрудника.
-Обратите внимание, что ниже блока Функционал есть список "Активных ролей подразделения". В нем указаны те люди, которые имеют доступ к просмотру или редактированию данных на портале, относящихся к Вашему подразделению. Если среди них есть люди, которые больше не работают в ВШЭ или не имеют отношения к конкретному подразделению, то необходимо сообщить об этом на portal@hse.ru.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/site**
- Быстрые ссылки  Доступ к редактированию Наполнение сайта Размещение текстов Размещение новостей  
-**Доступ к редактированию**
-Доступ к редактированию сайта предоставляется в течение одного рабочего дня. Как получить доступ, написано здесь.
-Перейти к режиму редактирования сайта можно двумя способами:
- По прямой ссылке: https://www.hse.ru/adm/ (там будет высвечиваться список подразделений, к которым у вас есть права); Путем клика на ссылку «Редактору» внизу главной страницы сайта, на редактирование которого у вас есть права. Далее надо будет нажать на ссылку «Данные». Если вы нажмете на ссылку «Редактору» на статической странице, новости или анонсе внутри сайта, то сразу попадете в режим редактирования этого конкретного элемента. 
-Отдельные права для редактирования английской версии не нужны. Подробно про работу с английской версией написано здесь.
-**Наполнение сайта**
-Для работы с сайтом вам в основном будут нужны четыре подраздела сайта:
- Блоки (в этом подразделе осуществляется управление главной страницей сайта, включая добавление пунктов меню) Страницы (инструкция по созданию страницы) Новости (инструкция по созданию новости) Анонсы (инструкция по созданию анонса) 
-Если вы редактируете сайт структурного подразделения, то вам также будут нужны разделы «Функционал сотрудников подразделений» и «Показ в списках и на картах» (адреса и мета-информация подразделений).
-Очень часто первым желанием редактора бывает завести новый пункт меню. Однако в этом случае единственное, чего вы достигнете – это разочаруете посетителя своего сайта, так как при клике на пункт меню он получит ошибку. Кроме того, чем больше таких ошибок на сайте, тем хуже он индексируется поисковиками.
-Сначала надо создать страницы и наполнить их содержимым. Внимательно прочитайте про размещение текстов на портале и работу с таблицами.
-Только после того как созданы страницы, заводится пункт меню. Чтобы завести новый пункт меню необходимо перейти в раздел Блоки → Меню. В поле название пропишите название пункта меню, а в поле URL ссылку на страницу.
-**Меню: основные ошибки**
- Пункт меню создан раньше, чем соответствующая страница. Ссылка прописана правильно, но страница не открывается. Проверьте, что в конце ссылки не стоит пробел. Удалите пробел. Дана ссылка на сайт в домене hse.ru, но при этом стоит галочка около пункта «Открывать в новом окне». Этот функционал необходимо использовать, если по каким-то причинам вы хотите сослаться на внешний сайт. 
-**Как вывести страницу «Сотрудники»?**
-Мы не рекомендуем вести такую страницу вручную, вы обязательно забудете скорректировать список при изменении кадрового состава. Для того чтобы вывести в меню автоматическую страницу «Сотрудники», необходимо прописать в поле URL пункта меню слово persons. Предварительно надо убедиться, что в вашем подразделении есть хотя бы один оформленный сотрудник. Ссылку на пустую страницу добавлять не нужно.
-Если вы точно знаете, что в вашем подразделении есть оформленные сотрудники, но страница не показывается, напишите об этом на адрес portal@hse.ru, указав в письме ссылку на сайт, о котором идет речь, и ссылку на сотрудника, имеющего трудоустройство в этом подразделении (трудоустройство должно показываться на странице).
-Подробно про то, как появляются персональные страницы на портале и про то, откуда берется на них информация, написано здесь.
-**Размещение текстов: что можно и что нельзя**
-**Можно и нужно:**
- Если у вас на странице размещен не просто текст, а, например, есть необходимость вывести список участников мероприятия с фотографиями, то мы рекомендуем воспользоваться шаблоном составной страницы/новости/анонса. Инструкция по работе с такой страницей находится здесь. Принцип работы с составными страницами/новостями/анонсами одинаковый. После переключения обычной страницы в режим составной вы получаете набор готовых элементов для оформления страницы. Мы постарались, чтобы в разных браузерах и на разных устройствах эти элементы отображались корректно, однако, если вы заметили ошибку, то, пожалуйста, напишите нам об этом на portal@hse.ru. Если информация не требует сложного оформления, выбирайте режим «простой» страницы. Выделять в тексте подзаголовки разного уровня, если этого требует текст. Помните, что для этого нужно оформить текст как заголовок, а не выделить его жирным и увеличить шрифт. Заголовок — важный элемент структуры страницы, он поможет поисковикам лучше понять ваш сайт. Заголовком нельзя оформлять отдельные предложения или абзацы. Подробно про поисковую оптимизацию можно прочитать здесь. Если у вас очень важная страница, и вы понимаете, какие блоки хотели бы выделить, но не знаете, как это лучше сделать, напишите свой вопрос на portal@hse.ru. Мы постараемся помочь. 
- Категорически нельзя:  Размещать текст, скопированный из Word, без последующей очистки его от посторонних стилей. Это приводит к непредсказуемому отображению текстов в разных браузерах, в некоторых случаях на мобильных устройствах текст может выходить за границы экрана (посетитель в принципе не сможет прочитать текст), а может и просто стать невидимым. Подробно про размещение текстов написано здесь. Менять размер и стиль шрифта, красить текст в разные цвета. Это также приводит к некорректному отображению. В конце концов это просто некрасиво, когда сайт выглядит как школьная стенгазета. Выравнивать текст по ширине. На стационарном компьютере такое форматирование может выглядеть симпатично, но в мобильной версии два слова могут прилипнуть к краям экрана, а по центру страницы образуется пустота. Размещать тексты в виде изображений. Мы знаем, что для мероприятий часто готовятся рекламные постеры. Они предназначены для размещения на стенде, а не сайте. Тексты в виде картинок тяжело читать с мобильных устройств, они не индексируются поисковыми системами, недоступны для прочтения слабовидящими, использующими для ознакомления с сайтом специальные программы. Писать заголовки, используя только заглавные буквы. Наличие в тексте только заглавных букв усложняет его восприятие. Чем длиннее текст, набранный заглавными буквами, тем сложнее его прочитать. Кроме того, в интернете традиционно считается, что если автор пишет заглавными буквами, то это означает, что он кричит. Размещать заголовки в несколько строк. В мобильной версии они будут занимать весь экран.  
-**Размещение новостей: на что обратить внимание**
- У каждой новости должен быть короткий заголовок, аннотация, рубрика, ключевые слова, текст новости. Про это написано в инструкции и закреплено в Стандарте. Форматирование текстов. Абзац и переносы строки – это не одно и то же. И еще раз ссылка на инструкцию. Точки в заголовках не ставятся. Иллюстрации. Хорошо, когда новость иллюстрирует фотография, сделанная вами в рамках работы. Также здорово, если изображение передал вам автор для размещения на сайте. Категорически нельзя использовать изображения, найденные в сети. Обязательно проверяйте копирайт. Иногда достаточно указать, откуда скопировано изображение, иногда требуется письменное разрешение автора, а в некоторых случаях размещать у себя изображение в принципе нельзя. При необходимости вы можете взять изображение из бесплатного фотобанка. Иллюстрация не является обязательным элементом новости. Картинка должна быть горизонтальной и хорошего качества. Недопустимо размещение в качестве иллюстрации новости скриншотов, баннеров, листовок, обложек, постеров, логотипов. 
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
           <t xml:space="preserve">**https://portal.hse.ru/metaunits**
 В настоящее время сведения из блока «Показ в списках и на картах» (Данные → Показ в списках и на картах) не показываются на сайтах подразделений. Однако они используются для отображения информации о подразделениях в разделах портала:
 Здания
@@ -1767,11 +1713,142 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/script**
+Мы с осторожностью относимся к просьбам коллег разместить на сайте подразделения произвольные JavaScript'ы и сторонние iframe'ы. Подобные вставки оказываются очень уязвимыми элементами сайта с точки зрения безопасности. Через свою связь с внешими сайтами они могут стать рассадниками огромного числа вирусов и инфицировать компьютеры ничего не подозревающих посетителей портала.
+Гарантированной защиты от подобного не могут обеспечить даже крупные интернет-корпорации. Минимизировать ущерб возможно, только существенно сократив число подобных кодовых вставок в ресурсы портала.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/section-persons**
+На странице показываются все штатные сотрудники подразделения, проведенные в ЗиК (для Москвы) или ИС-ПРО (для кампусов). Подробнее про то, к кому обращаться в случае отсутствия трудустроенного в ВШЭ сотрудника написано здесь.
+Страница имеет автоматически формируемое техническое имя persons. Чтобы добавить автоматическую страницу «Сотрудники» на сайте необходимо в соответствующем пункте меню прописать адрес сайта/persons (например, для Управления развития и поддержки портала адрес страницы выглядит https://portal.hse.ru/persons). Заводить статическую страницу с таким адресом не нужно. 
+**Сортировка сотрудников по должностям на странице**
+Редактор подразделения имеет возможность изменить автоматическую сортировку сотрудников, установив сортировку по должностям. Для этого каждой должности внутри сайта подразделения необходимо установить свой порядковый номер. Например, Руководитель будет иметь порядковый номер 1, его заместитель — 2 (или любое другое число больше 1), профессор — 3.
+В этом случае на странице в алфавитном порядке будут показываться сначала люди с должностью Руководитель, потом люди с должностью Заместитель руководителя, потом — все сотрудники с должностью Профессор.
+В административном интерфейсе раздел можно найти по следующему пути: Данные → Должности. Для выставления порядкового номера необходимо кликнуть мышкой на значок «редактировать» и проставить соответствующий номер. 
+**Шаг 1**
+**Шаг 2**
+Обратите внимание, что данная страница имеет автоматический кэш — 4 часа. Если вы хотите сразу увидеть изменения, то пересохраните основную страницу подразделения.
+</t>
+        </is>
+      </c>
+    </row>
     <row r="28">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
       <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/meta**
+В редакторском режиме для сайтов, статических страниц, новостей и анонсов вы видите следующие поля для заполнения:
+ Быстрые ссылки  Описание документа Соцсети  
+**Описание документа**
+Самое важное поле – «Описание документа». По мере наполнения сайта не забывайте заполнять это поле для всех новых страниц, новостей, анонсов. Большая просьба также заполнить его для уже созданных сайтов и статических страниц.
+Из того, что вы напишете в этом поле, сформируется мета-тег description. Он описывает содержимое страницы для поисковых роботов (Яндекс и Google). Если description есть, ваша страница/сайт будет при прочих равных лучше индексироваться в поисковиках, окажутся выше в выдаче и, соответственно, увеличится поисковый трафик на ваш сайт. Кроме того, часто именно это описание Google подставляет в выдачу (на страницу результатов поиска).
+Что из себя представляет «Описание документа»? Это короткий связный текст, описывающий контент страницы. «Описание документа» – это фактически краткое описание того, что написано на главной странице сайта. Оптимизаторы сайтов рекомендуют делать описание на 160 знаков, можно чуть больше, но имейте в виду, что большинство поисковых роботов игнорируют то, что написано за первыми 160-180 знаками. Также нельзя делать из описания набор ключевых слов через запятую. Во-первых, это очень не нравится роботам, и результат может оказаться отрицательным. Во-вторых, эта информация может показываться людям, а им нужен более связный текст. 
+**Рекомендации по составлению мета-описаний (c сайта Яндекса):**
+ Мета-описания не должны содержать всего несколько слов. Должны описывать конкретную страницу сайта, а не сайт в целом. Мета-описания должны быть написаны для людей, нормальным человеческим языком — развернуто, правильно выстроенными предложениями, без злоупотреблений ключевыми словами, фразами, заглавными буквами, рекламными лозунгами и пр. Мета-описания должны быть емкими и при этом содержательными. Старайтесь выразить основную суть документа в нескольких предложениях. Содержимое тега meta должно быть актуальным, отражать текущее состояние страницы. Мета-описания должны соответствовать языку документа. 
+**Примеры плохих мета-описаний (с сайта Яндекса):**
+ Наполнение мета-описаний временной, служебной информацией, например: «Не забыть добавить здесь текст». Устаревшие описания. Например, цены на сайте изменились, описываемый документ теперь расположен по другому адресу, а описания при этом прежние. Размещение важной информации в конце текста. Старайтесь располагать наиболее важную информацию и фразы в начале мета-описаний. 
+**Примеры правильного заполнения мета-описаний:**
+https://elearning.hse.ru/mooc Массовые открытые онлайн курсы НИУ ВШЭ
+description: В открытом доступе на международной платформе Coursera и российской Национальной платформе открытого образования (НПОО) вы можете бесплатно изучать курсы лучших преподавателей Высшей школы экономики.
+https://www.hse.ru/abiturient Поступающим в НИУ ВШЭ
+description: Высшая школа экономики — это отличный старт для карьеры в бизнесе, на государственной службе и в науке. Здесь готовят высококлассных специалистов, нужных стране. Все, что нужно знать поступающим в НИУ ВШЭ - дни открытых дверей, проходной балл и другую информацию.
+https://www.hse.ru/figures/ Цифры и факты
+description: Что такое ВШЭ в цифрах, фактах, статистика, рейтинги, инфографика и многое другое, что вы хотели знать о Вышке.
+https://ma.hse.ru/ Абитуриентам магистратуры
+description: Прием и информация для поступающих в магистратуру НИУ ВШЭ. Список направлений подготовки и программ. Вопросы и ответы. Вступительные испытания и дни открытых дверей на официальном сайте.
+**Соцсети**
+Если вы хотите, чтобы ваш сайт или отдельная страница красиво выглядели в соцсетях, когда пользователи делятся ссылками, нужно эти поля заполнить.
+На картинках ниже можно увидеть, как отличаются ссылки в соцсетях в случае, если соответствующие поля заполнены, и если нет.
+Картинка 1: когда все заполнено
+Картинка 2: когда ничего не заполнено
+Чтобы посмотреть, как сейчас отображается та или иная страница при копировании ссылки в ВКонтакте, можно воспользоваться инструментом ВКонтакте pages.clearCache. Позволяет сбросить кэш соцсети для конкретной ссылки. После этого соцсеть запросит новые данные со искомой страницы и учтет внесенные на нее изменения.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/site**
+ Быстрые ссылки  Доступ к редактированию Наполнение сайта Размещение текстов Размещение новостей  
+**Доступ к редактированию**
+Доступ к редактированию сайта предоставляется в течение одного рабочего дня. Как получить доступ, написано здесь.
+Перейти к режиму редактирования сайта можно двумя способами:
+ По прямой ссылке: https://www.hse.ru/adm/ (там будет высвечиваться список подразделений, к которым у вас есть права); Путем клика на ссылку «Редактору» внизу главной страницы сайта, на редактирование которого у вас есть права. Далее надо будет нажать на ссылку «Данные». Если вы нажмете на ссылку «Редактору» на статической странице, новости или анонсе внутри сайта, то сразу попадете в режим редактирования этого конкретного элемента. 
+Отдельные права для редактирования английской версии не нужны. Подробно про работу с английской версией написано здесь.
+**Наполнение сайта**
+Для работы с сайтом вам в основном будут нужны четыре подраздела сайта:
+ Блоки (в этом подразделе осуществляется управление главной страницей сайта, включая добавление пунктов меню) Страницы (инструкция по созданию страницы) Новости (инструкция по созданию новости) Анонсы (инструкция по созданию анонса) 
+Если вы редактируете сайт структурного подразделения, то вам также будут нужны разделы «Функционал сотрудников подразделений» и «Показ в списках и на картах» (адреса и мета-информация подразделений).
+Очень часто первым желанием редактора бывает завести новый пункт меню. Однако в этом случае единственное, чего вы достигнете – это разочаруете посетителя своего сайта, так как при клике на пункт меню он получит ошибку. Кроме того, чем больше таких ошибок на сайте, тем хуже он индексируется поисковиками.
+Сначала надо создать страницы и наполнить их содержимым. Внимательно прочитайте про размещение текстов на портале и работу с таблицами.
+Только после того как созданы страницы, заводится пункт меню. Чтобы завести новый пункт меню необходимо перейти в раздел Блоки → Меню. В поле название пропишите название пункта меню, а в поле URL ссылку на страницу.
+**Меню: основные ошибки**
+ Пункт меню создан раньше, чем соответствующая страница. Ссылка прописана правильно, но страница не открывается. Проверьте, что в конце ссылки не стоит пробел. Удалите пробел. Дана ссылка на сайт в домене hse.ru, но при этом стоит галочка около пункта «Открывать в новом окне». Этот функционал необходимо использовать, если по каким-то причинам вы хотите сослаться на внешний сайт. 
+**Как вывести страницу «Сотрудники»?**
+Мы не рекомендуем вести такую страницу вручную, вы обязательно забудете скорректировать список при изменении кадрового состава. Для того чтобы вывести в меню автоматическую страницу «Сотрудники», необходимо прописать в поле URL пункта меню слово persons. Предварительно надо убедиться, что в вашем подразделении есть хотя бы один оформленный сотрудник. Ссылку на пустую страницу добавлять не нужно.
+Если вы точно знаете, что в вашем подразделении есть оформленные сотрудники, но страница не показывается, напишите об этом на адрес portal@hse.ru, указав в письме ссылку на сайт, о котором идет речь, и ссылку на сотрудника, имеющего трудоустройство в этом подразделении (трудоустройство должно показываться на странице).
+Подробно про то, как появляются персональные страницы на портале и про то, откуда берется на них информация, написано здесь.
+**Размещение текстов: что можно и что нельзя**
+**Можно и нужно:**
+ Если у вас на странице размещен не просто текст, а, например, есть необходимость вывести список участников мероприятия с фотографиями, то мы рекомендуем воспользоваться шаблоном составной страницы/новости/анонса. Инструкция по работе с такой страницей находится здесь. Принцип работы с составными страницами/новостями/анонсами одинаковый. После переключения обычной страницы в режим составной вы получаете набор готовых элементов для оформления страницы. Мы постарались, чтобы в разных браузерах и на разных устройствах эти элементы отображались корректно, однако, если вы заметили ошибку, то, пожалуйста, напишите нам об этом на portal@hse.ru. Если информация не требует сложного оформления, выбирайте режим «простой» страницы. Выделять в тексте подзаголовки разного уровня, если этого требует текст. Помните, что для этого нужно оформить текст как заголовок, а не выделить его жирным и увеличить шрифт. Заголовок — важный элемент структуры страницы, он поможет поисковикам лучше понять ваш сайт. Заголовком нельзя оформлять отдельные предложения или абзацы. Подробно про поисковую оптимизацию можно прочитать здесь. Если у вас очень важная страница, и вы понимаете, какие блоки хотели бы выделить, но не знаете, как это лучше сделать, напишите свой вопрос на portal@hse.ru. Мы постараемся помочь. 
+ Категорически нельзя:  Размещать текст, скопированный из Word, без последующей очистки его от посторонних стилей. Это приводит к непредсказуемому отображению текстов в разных браузерах, в некоторых случаях на мобильных устройствах текст может выходить за границы экрана (посетитель в принципе не сможет прочитать текст), а может и просто стать невидимым. Подробно про размещение текстов написано здесь. Менять размер и стиль шрифта, красить текст в разные цвета. Это также приводит к некорректному отображению. В конце концов это просто некрасиво, когда сайт выглядит как школьная стенгазета. Выравнивать текст по ширине. На стационарном компьютере такое форматирование может выглядеть симпатично, но в мобильной версии два слова могут прилипнуть к краям экрана, а по центру страницы образуется пустота. Размещать тексты в виде изображений. Мы знаем, что для мероприятий часто готовятся рекламные постеры. Они предназначены для размещения на стенде, а не сайте. Тексты в виде картинок тяжело читать с мобильных устройств, они не индексируются поисковыми системами, недоступны для прочтения слабовидящими, использующими для ознакомления с сайтом специальные программы. Писать заголовки, используя только заглавные буквы. Наличие в тексте только заглавных букв усложняет его восприятие. Чем длиннее текст, набранный заглавными буквами, тем сложнее его прочитать. Кроме того, в интернете традиционно считается, что если автор пишет заглавными буквами, то это означает, что он кричит. Размещать заголовки в несколько строк. В мобильной версии они будут занимать весь экран.  
+**Размещение новостей: на что обратить внимание**
+ У каждой новости должен быть короткий заголовок, аннотация, рубрика, ключевые слова, текст новости. Про это написано в инструкции и закреплено в Стандарте. Форматирование текстов. Абзац и переносы строки – это не одно и то же. И еще раз ссылка на инструкцию. Точки в заголовках не ставятся. Иллюстрации. Хорошо, когда новость иллюстрирует фотография, сделанная вами в рамках работы. Также здорово, если изображение передал вам автор для размещения на сайте. Категорически нельзя использовать изображения, найденные в сети. Обязательно проверяйте копирайт. Иногда достаточно указать, откуда скопировано изображение, иногда требуется письменное разрешение автора, а в некоторых случаях размещать у себя изображение в принципе нельзя. При необходимости вы можете взять изображение из бесплатного фотобанка. Иллюстрация не является обязательным элементом новости. Картинка должна быть горизонтальной и хорошего качества. Недопустимо размещение в качестве иллюстрации новости скриншотов, баннеров, листовок, обложек, постеров, логотипов. 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/resp**
+На сайтах подразделений существует функционал, позволяющий подразделению самостоятельно формировать списки сотрудников, к которым можно обращаться по тем или иным вопросам.
+Списки показываются в справочнике сотрудника, а также в личном кабинете сотрудника.
+В настоящее время на сайте подразделения заведены следующие категории функциональной ответственности.
+Ответственные от факультетов и филиалов за редактирование страниц подразделений
+Ответственные за персональные страницы сотрудников
+Добавление в список ответственных автоматически не дает им доступ к редактированию сайта и персональных страниц. Для этого необходимо получить соответствующие права в подразделении, отвечающем за соответствующий ресурс.
+Управление по информационным ресурсам выдает права (заявка на адрес portal@hse.ru)
+Ответственным от факультетов и филиалов за редактирование страниц подразделений
+Ответственным за персональные страницы сотрудников
+**Как изменить сведения об ответственных**
+**Добавление сотрудника:**
+Необходимо перейти в режим редактирования сайта конкретного подразделения (раздел Данные). В блоке "Функционал сотрудника подразделения" нажать кнопку "Добавить сотрудника", вбить в поле для поиска ФИО, выбрать сотрудника и галочками выбрать возможные категории его ответственности.
+**Удаление сотрудника из списка**
+Для удаления сотрудника необходимо убрать все галки в списке функциональной ответственности сотрудника.
+Обратите внимание, что ниже блока Функционал есть список "Активных ролей подразделения". В нем указаны те люди, которые имеют доступ к просмотру или редактированию данных на портале, относящихся к Вашему подразделению. Если среди них есть люди, которые больше не работают в ВШЭ или не имеют отношения к конкретному подразделению, то необходимо сообщить об этом на portal@hse.ru.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t xml:space="preserve">**https://portal.hse.ru/seo_recommends**
  Быстрые ссылки  Заголовки страниц Мета-описание страницы Заголовки в тексте Ссылки Изображения Общие рекомендации  
@@ -1851,93 +1928,16 @@
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/meta**
-В редакторском режиме для сайтов, статических страниц, новостей и анонсов вы видите следующие поля для заполнения:
- Быстрые ссылки  Описание документа Соцсети  
-**Описание документа**
-Самое важное поле – «Описание документа». По мере наполнения сайта не забывайте заполнять это поле для всех новых страниц, новостей, анонсов. Большая просьба также заполнить его для уже созданных сайтов и статических страниц.
-Из того, что вы напишете в этом поле, сформируется мета-тег description. Он описывает содержимое страницы для поисковых роботов (Яндекс и Google). Если description есть, ваша страница/сайт будет при прочих равных лучше индексироваться в поисковиках, окажутся выше в выдаче и, соответственно, увеличится поисковый трафик на ваш сайт. Кроме того, часто именно это описание Google подставляет в выдачу (на страницу результатов поиска).
-Что из себя представляет «Описание документа»? Это короткий связный текст, описывающий контент страницы. «Описание документа» – это фактически краткое описание того, что написано на главной странице сайта. Оптимизаторы сайтов рекомендуют делать описание на 160 знаков, можно чуть больше, но имейте в виду, что большинство поисковых роботов игнорируют то, что написано за первыми 160-180 знаками. Также нельзя делать из описания набор ключевых слов через запятую. Во-первых, это очень не нравится роботам, и результат может оказаться отрицательным. Во-вторых, эта информация может показываться людям, а им нужен более связный текст. 
-**Рекомендации по составлению мета-описаний (c сайта Яндекса):**
- Мета-описания не должны содержать всего несколько слов. Должны описывать конкретную страницу сайта, а не сайт в целом. Мета-описания должны быть написаны для людей, нормальным человеческим языком — развернуто, правильно выстроенными предложениями, без злоупотреблений ключевыми словами, фразами, заглавными буквами, рекламными лозунгами и пр. Мета-описания должны быть емкими и при этом содержательными. Старайтесь выразить основную суть документа в нескольких предложениях. Содержимое тега meta должно быть актуальным, отражать текущее состояние страницы. Мета-описания должны соответствовать языку документа. 
-**Примеры плохих мета-описаний (с сайта Яндекса):**
- Наполнение мета-описаний временной, служебной информацией, например: «Не забыть добавить здесь текст». Устаревшие описания. Например, цены на сайте изменились, описываемый документ теперь расположен по другому адресу, а описания при этом прежние. Размещение важной информации в конце текста. Старайтесь располагать наиболее важную информацию и фразы в начале мета-описаний. 
-**Примеры правильного заполнения мета-описаний:**
-https://elearning.hse.ru/mooc Массовые открытые онлайн курсы НИУ ВШЭ
-description: В открытом доступе на международной платформе Coursera и российской Национальной платформе открытого образования (НПОО) вы можете бесплатно изучать курсы лучших преподавателей Высшей школы экономики.
-https://www.hse.ru/abiturient Поступающим в НИУ ВШЭ
-description: Высшая школа экономики — это отличный старт для карьеры в бизнесе, на государственной службе и в науке. Здесь готовят высококлассных специалистов, нужных стране. Все, что нужно знать поступающим в НИУ ВШЭ - дни открытых дверей, проходной балл и другую информацию.
-https://www.hse.ru/figures/ Цифры и факты
-description: Что такое ВШЭ в цифрах, фактах, статистика, рейтинги, инфографика и многое другое, что вы хотели знать о Вышке.
-https://ma.hse.ru/ Абитуриентам магистратуры
-description: Прием и информация для поступающих в магистратуру НИУ ВШЭ. Список направлений подготовки и программ. Вопросы и ответы. Вступительные испытания и дни открытых дверей на официальном сайте.
-**Соцсети**
-Если вы хотите, чтобы ваш сайт или отдельная страница красиво выглядели в соцсетях, когда пользователи делятся ссылками, нужно эти поля заполнить.
-На картинках ниже можно увидеть, как отличаются ссылки в соцсетях в случае, если соответствующие поля заполнены, и если нет.
-Картинка 1: когда все заполнено
-Картинка 2: когда ничего не заполнено
-Чтобы посмотреть, как сейчас отображается та или иная страница при копировании ссылки в ВКонтакте, можно воспользоваться инструментом ВКонтакте pages.clearCache. Позволяет сбросить кэш соцсети для конкретной ссылки. После этого соцсеть запросит новые данные со искомой страницы и учтет внесенные на нее изменения.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/section-persons**
-На странице показываются все штатные сотрудники подразделения, проведенные в ЗиК (для Москвы) или ИС-ПРО (для кампусов). Подробнее про то, к кому обращаться в случае отсутствия трудустроенного в ВШЭ сотрудника написано здесь.
-Страница имеет автоматически формируемое техническое имя persons. Чтобы добавить автоматическую страницу «Сотрудники» на сайте необходимо в соответствующем пункте меню прописать адрес сайта/persons (например, для Управления развития и поддержки портала адрес страницы выглядит https://portal.hse.ru/persons). Заводить статическую страницу с таким адресом не нужно. 
-**Сортировка сотрудников по должностям на странице**
-Редактор подразделения имеет возможность изменить автоматическую сортировку сотрудников, установив сортировку по должностям. Для этого каждой должности внутри сайта подразделения необходимо установить свой порядковый номер. Например, Руководитель будет иметь порядковый номер 1, его заместитель — 2 (или любое другое число больше 1), профессор — 3.
-В этом случае на странице в алфавитном порядке будут показываться сначала люди с должностью Руководитель, потом люди с должностью Заместитель руководителя, потом — все сотрудники с должностью Профессор.
-В административном интерфейсе раздел можно найти по следующему пути: Данные → Должности. Для выставления порядкового номера необходимо кликнуть мышкой на значок «редактировать» и проставить соответствующий номер. 
-**Шаг 1**
-**Шаг 2**
-Обратите внимание, что данная страница имеет автоматический кэш — 4 часа. Если вы хотите сразу увидеть изменения, то пересохраните основную страницу подразделения.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/script**
-Мы с осторожностью относимся к просьбам коллег разместить на сайте подразделения произвольные JavaScript'ы и сторонние iframe'ы. Подобные вставки оказываются очень уязвимыми элементами сайта с точки зрения безопасности. Через свою связь с внешими сайтами они могут стать рассадниками огромного числа вирусов и инфицировать компьютеры ничего не подозревающих посетителей портала.
-Гарантированной защиты от подобного не могут обеспечить даже крупные интернет-корпорации. Минимизировать ущерб возможно, только существенно сократив число подобных кодовых вставок в ресурсы портала.
-</t>
-        </is>
-      </c>
-    </row>
     <row r="32">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t xml:space="preserve">**https://portal.hse.ru/newdesignbb**
-Чтобы включить доску объявлений на сайте образовательной программы, необходимо открыть блок «Доска объявлений» (Данные −&gt; Блоки) и поставить соответствующую галочку.
-В этом блоке можно добавить новые рубрики и фильтры. Обратите внимание, что по умолчанию доски объявлений содержат ряд типовых, часто встречающихся рубрик. Каждое объявление в обязательном порядке должно быть привязано хотя бы к одному фильтру (по умолчанию это курсы) и хотя бы к одной рубрике.
-Программам, которые имеют несколько специализаций, мы рекомендуем добавить дополнительный фильтр (не рубрику) «Специализации», чтобы иметь возможность публиковать объявления для студентов, обучающихся по разным трекам.Чтобы добавить новое объявление, в меню личного кабинета (hse.ru/user) в разделе «Мои задачи» редактор сайта образовательной программы должен выбрать пункт «Объявления на досках объявлений».
-На открывшейся странице будут доступны ссылки на добавление новых объявлений. Ниже находится список размещенных ранее объявлений (если таковые есть). 
-Обратите внимание: если вы являетесь редактором сайтов нескольких программ, то при создании нового объявления следует выбрать нужную доску из списка.
-Что не следует делать:
-Создавать фильтры и темы, не несущие смысловой нагрузки. К таким, например, относятся: «Важная информация», «Важно», «Не пропустите», «Всем».
-Использовать при написании заголовков только прописные (заглавные) буквы Неправильно: ОБНОВЛЕНО РАСПИСАНИЕ Правильно: Обновлено расписание
-Пренебрегать форматированием текста. Текст с большим количеством пробелов, интервалов и т.п. неудобно читать.
-Все материалы, связанные с образовательной программой, необходимо размещать на сайте этой программы. Например, расписание должно находиться на сайте образовательной программы, а не на сайте факультета.
-Инструкция по редактированию сайтов образовательных программ размещена здесь: http://portal.hse.ru/progs
+          <t xml:space="preserve">**https://portal.hse.ru/helpsite**
+Для получения доступа к  редактированию сайта необходимо направить заявку в свободной форме по электронному адресу portal@hse.ru. В заявке необходимо указать ФИО сотрудника и адрес сайта, к которому нужен доступ. 
+Для редактирования сайта необходимо иметь доступ в личный кабинет на портале.
+Заявка должна быть отправлена с корпоративного адреса электронной почты.
 </t>
         </is>
       </c>
@@ -1947,170 +1947,6 @@
         <v>31</v>
       </c>
       <c r="B33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/aspresponsible**
-**https://portal.hse.ru/aspresponsible**
-**Аспирантская школа по экономике**
-**https://portal.hse.ru/aspresponsible**
-**Аспирантская школа по менеджменту**
-**https://portal.hse.ru/aspresponsible**
-**Аспирантские школы: по государственному и муниципальному управлению; по философским наукам**
-**https://portal.hse.ru/aspresponsible**
-**Аспирантская школа по праву**
-**https://portal.hse.ru/aspresponsible**
-**Аспирантская школы: по социологическим наукам; по политическим наукам; по искусству и дизайну; по международным отношениям и зарубежным региональным исследованиям**
-**https://portal.hse.ru/aspresponsible**
-**Аспирантские школы: по историческим наукам; по филологическим наукам; по философским наукам; по культурологии**
-**https://portal.hse.ru/aspresponsible**
-**Аспирантская школа по техническим наукам**
-**https://portal.hse.ru/aspresponsible**
-**Аспирантские школы: по компьютерным наукам; по физике**
-**https://portal.hse.ru/aspresponsible**
-**Аспирантская школа по образованию**
-**https://portal.hse.ru/aspresponsible**
-**Аспирантская школа по психологии**
-**https://portal.hse.ru/aspresponsible**
-**Аспирантская школа по математике**
-**https://portal.hse.ru/aspresponsible**
-**Академическая аспирантура**
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/analytics**
-На портале НИУ ВШЭ установлены счетчики Google Analytics и Яндекс.Метрика. C их помощью можно узнать количество посещений сайта, проанализировать действия пользователей, понять, как они перешли на ту или иную страницу. Доступна также статистика скачивания файлов.
-Вопросами, связанными с посещаемостью страниц портала, занимается Отдел веб-аналитики и моделирования.
-**Доступ к аналитике**
-**Предоставление доступа для специалистов по привлечению трафика или рекламных агентств**
- Доступ предоставляется в отдельное представление Google Analytics. В выделенном представлении присутствуют данные отдельного поддомена. Настройки в представлении производятся специалистами по привлечению трафика или РА посредством GTM (Google Tag Manager). 
-**Предоставление доступа сотрудникам ВШЭ**
-Доступ предоставляется для сотрудников ВШЭ в Google Analytics или Я.Метрику без ограничений.
-Доступ предоставляется в течение одного рабочего дня.
-Запрос на предоставление доступа
-**Как узнать посещаемость сайта**
-**В Яндекс.Метрике**
-Самый простой способ узнать, сколько человек посетили страницу сайта вашего подразделения или мероприятия через Яндекс.Метрику, — использовать сервис стандартных отчетов «Заголовки страниц».
-В поле поиска задается название страницы. В результирующей таблице содержатся два значения для указанного временного диапазона: число просмотров (загрузок страницы) и число посетителей (количество уникальных людей, пришедших на вашу страницу). Подробная пользовательская инструкция Яндекс.Метрики доступна по адресу https://yandex.ru/support/metrika/
-**В Google Analytics**
-В меню сервиса, расположенном в левой части экрана, выбирается вкладка Поведение → Контент сайта → Все страницы. В строке поиска указывается url-адрес нужной страницы без указания сетевого протокола (https://).
-Для увеличения точности анализа нужно передвинуть соответствующий бегунок вверху экрана под строками выбора дат, а также выбрать более узкий временной промежуток. Подробная пользовательская инструкция Google Analytics находится по адресу https://support.google.com/analytics/
-**Как узнать число скачиваний файлов**
-**В Яндекс.Метрике**
-Стандартный отчет формируется так: Отчеты → Стандартные отчеты → Содержание → Загрузки файлов.
-Задаем необходимый временной промежуток, под графиком выбираем URL, загрузки файлов с которого нас интересуют.
-**В Google Analytics**
-В меню сервиса выбирается вкладка Поведение → События → Страницы. В строке поиска указывается url-адрес страницы, на которой находятся ссылки на файлы, без указания сетевого протокола (https://).
-Выбирается категория событий Download. Результирующая таблица показывает число скачанных с этой страницы файлов за выбранный промежуток времени.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/pay**
-На портале можно организовать прием платежей за участие в проводимых подразделениями НИУ ВШЭ мероприятиях. Заявка на создание формы приема платежей направляется руководителем подразделения на адрес underground@hse.ru. Срок оказания услуги — 2 рабочих дня с момента получения полного пакета необходимых сведений от заказчика при условии создания стандартной формы.
-**Что нужно указать в заявке**
-Обратите внимание, что по требованию финансового блока создание формы для приема платежей возможно только при наличии подписанного приказа на проведение мероприятия. Приказ создает подразделение-организатор мероприятия; документ согласуется с руководителями в соответствии с их полномочиями. Если доходы или расходы по мероприятию требуют проставления финансовых аналитик, в согласовании также участвует ПФУ. Копию договора необходимо приложить к заявке. В ней нужно указать:
-Номер учетного договора от ПФУ (номер БЭСТ), по которому будет вестись прием средств;Для учета поступающих средств по мероприятию в ИС-ПРО создается управленческий договор. Договор создается подразделением самостоятельно, если подразделение имеет доступ в ИС-ПРО с соответствующими правами, либо ответственным работником ПФУ.
-Наименование подразделения, которое будет осуществлять прием платежей;
-Шифр подразделения по ИС-ПРО;
-Адрес сайта в зоне hse.ru, где будет размещена страница мероприятия (желательно указать также адрес страницы с описанием особенностей оплаты);
-Список электронных почтовых адресов ответственных лиц в домене hse.ru для ежедневной выгрузки отчета по произведенным оплатам;
-Сроки приема платежей;
-Включен ли в сумму платежа НДС или нет;
-Требуется ли англоязычная версия формы;
-Список категорий участников (с переводом на английский язык при необходимости создания формы на английском языке) и соответствующие им суммы платежей в рублях;
-Текст договора-оферты, который будет размещен на странице формы приема платежей (его можно согласовать с юристами);
-При необходимости: бланки платежного извещения для оплаты участниками в валюте (в рублях) через банк для размещения на странице мероприятия;
-Если форма платежа нужна не для разового мероприятия, пожалуйста, добавьте в заявку информацию о типе платежа: оплата обучения, оплата проживания, оплата прочих услуг либо новый вид оплаты по договоренности с ПФУ и УБУ.
-Взаимодействие с участниками мероприятия проводится на основании договора-оферты, который должен быть размещен на странице мероприятия. В случае необходимости предоставления участникам мероприятия каких-либо подтверждающих документов их перечень необходимо в обязательном порядке предварительно согласовать с бухгалтерией НИУ ВШЭ.
-Важно!• Планируйте расценки на участие в мероприятии с учетом того, что на странице сбора платежей суммы к оплате указываются только в рублях, указание сумм в иностранных валютах не допускается, в том числе для иностранных участников.• Банк удерживает комиссию от суммы платежа. Комиссия с карт Сбербанка не взимается. Актуальный размер комиссии зависит от условий банка-эмитента карты платежа. По требованию банка выделять комиссию в сумме платежа на странице оплаты за мероприятие нельзя.
-**Варианты форм оплаты**
-Для стандартной формы оплаты допускается наличие нескольких категорий участников, каждой из которых может быть присвоена отдельная сумма к оплате. Например, для сотрудников НИУ ВШЭ - X руб., для иностранных граждан - Y руб. Автоматическая проверка статуса участника в момент оплаты не производится. Стандартная форма оплаты выглядит так:
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/brandbook_html_colours**
-Данные обозначения можно использовать при оформлении лендингов: для цвета подложки в шапке и основной колонке (контент-блок), цвета подложек в виджетах «Набор с выпадайками» и «Табы с карточками», виджетах «Цифра дня», «Плашка с цифрой», «Хронология», фонов виджетов «Программы», «Карусель», «Цифры», «Цифры и факты», «Ссылки», «Мероприятия», «Публикации», а также мобильного тулбара.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t xml:space="preserve">**https://portal.hse.ru/elibrary**
-С 2017 года в вашем распоряжении есть полный набор инструментов, предоставляемых НЭБ/РИНЦ. С их помощью можно уточнить и улучшить ваши показатели в РИНЦ. Большинство операций вы можете выполнить самостоятельно – и никто кроме вас не сможет это сделать должным образом. Но в некоторых случаях необходимо обратиться к представителям подразделений.
-Что можно сделать в первую очередь: 1) зарегистрироваться в РИНЦ:Science Index; 2) уточнить регистрационные данные для улучшения привязки публикаций; 3) проверить и скорректировать свой список публикаций; 4) проверить и скорректировать список ссылок на свои публикации.
-Ниже приведена краткая инструкция с учетом опыта работы с РИНЦ в НИУ ВШЭ. Полную инструкцию для авторов можно найти на сайте РИНЦ.
-ВНИМАНИЕ! Для корректной работы с сайтом РИНЦ необходимо отключить блокировку всплывающих окон для elibrary.ru.
-Инструкции
-Регистрация в Science IndexВнесение данных в регистрационную анкету и улучшение автоматической привязки публикацийРабота со списком публикацийРабота со ссылками на публикацииПорядок обращения к ответственным от подразделенийАнализ публикационной активности автора
-**Регистрация в Science Index**
-Если вы не зарегистрированы в Science Index, пройдите по этой ссылке: https://elibrary.ru/author_info.asp?isnew=1&amp;inreestr=on, либо выберите кнопку «Регистрация» в панели «Вход» на сайте elibrary.ru.
-Убедитесь, что в регистрационной анкете проставлена галочка «зарегистрировать меня как автора в системе Science Index».
-**Внесение данных в регистрационную анкету и улучшение автоматической привязки публикаций**
-При регистрации необходимо внести данные во все поля, обязательные для заполнения. Однако мы рекомендуем обратить внимание и на другие поля, так как это поможет автоматически привязать максимальное число ваших публикаций к аккаунту. Если вы уже зарегистрированы в Science Index, то можете внести эти данные, перейдя по ссылке: https://elibrary.ru/author_info.asp?isold=1, или пройдя в Личный кабинет → Профиль автора → Регистрационная карточка автора.
-1. Проверьте, указана ли аффилиация с НИУ ВШЭ
-2. В нижней части формы находятся поля, которые могут улучшить качество автоматической привязки публикаций
-В поле «Журналы» внесите журналы, в которых вы публиковались. В поле «Организации» укажите другие организации, в которых вы могли работать ранее. Если раньше у вас была другая фамилия, укажите ее в поле «Предыдущая фамилия (девичья)». Если вы публиковались или собираетесь публиковаться в зарубежных изданиях, укажите варианты написания фамилии латиницей – через запятую. В поле «Идентификационные коды автора» укажите любые другие свои идентификационные коды.
-3. После сохранения карточки в течение 2-10 дней вы получите уникальный идентификатор: SPIN-код автора.
-Он будет указан в панели «Сессия» слева, а также в начале регистрационной карточки. Необходимо указать этот SPIN-код в своем личном кабинете на портале НИУ ВШЭ.
-После получения SPIN-кода система выполнит привязку публикаций к вашему профилю, и вы получите возможность вносить исправления в список публикаций и список ссылок на публикации.
-**Работа со списком публикаций**
-После регистрации и заполнения карточки система попытается идентифицировать ваши работы автоматически и привязать их к вашему профилю. Однако возможны и ошибки идентификации.
-1. Начните с просмотра списка ваших публикаций (Профиль автора → Мои публикации). Проверьте, все ли публикации присутствуют в списке. Нет ли публикаций других авторов. Если таковые имеются, выберите их и нажмите «Удалить выделенные публикации…». Проверьте, правильно ли указана аффилиация для этих публикаций. Например, аффилиация с НИУ ВШЭ должна выглядеть так, как на рисунке ниже, то есть оформлена в виде гиперссылки со всплывающим полным названием.
-Если это не так, нажмите «Идентифицировать организацию, указанную в публикации в качестве места моей работы» в панели «Инструменты».
-2. Если в списке не обнаружены некоторые публикации, выберите в выпадающем списке «Показывать» «Непривязанные публикации, которые могут принадлежать данному автору». В открывшемся списке пометьте галочками принадлежащие вам публикации, после чего нажмите «Добавить выделенные публикации в список работ автора».
-3. Если некоторых публикаций нет ни в одном из указанных двух списков, это означает, что система не смогла идентифицировать публикации автоматически. В таком случае можно попытаться найти и привязать публикации вручную. Воспользуйтесь расширенным поиском (в левой верхней части страницы): вначале можно поискать по неполному имени и отчеству автора, затем, если, например, известно точное название публикации – по названию. После нажатия кнопки «Поиск» выводится список найденных публикаций – звездочкой помечены те, которые уже привязаны к вашему профилю. Если в списке найденных публикаций вы видите ту, которую необходимо привязать, щелкните по ее названию – откроется страница с описанием. В панели «Инструменты» выберите пункт «Добавить публикацию в список моих работ (если Вы являетесь ее автором)». После проверки публикация будет привязана к вашему профилю.
-4. Если не удалось найти публикацию ни в одном из этих случаев, вы можете обратиться к ответственному от вашего подразделения, чтобы он добавил нужную публикацию.
-**Работа со ссылками на публикации**
-Работа со ссылками во многом напоминает работу с публикациями
-1. Начните с просмотра списка ссылок: Профиль автора → Мои цитирования (либо в списке публикаций в панели «Инструменты» выберите «Вывести список ссылок на работы автора». Проверьте, нет ли в списке лишних ссылок. Если таковые имеются, выберите их и нажмите «Удалить выделенные ссылки из списка цитирований автора».
-2. В выпадающем списке «Показывать» выберите «Непривязанные ссылки, которые могут принадлежать данному автору».
-В открывшемся списке пометьте галочками принадлежащие вам публикации, после чего нажмите «Добавить выделенные ссылки в список цитирований автора».
-3. Если какие-то ссылки в этих списках отсутствуют, их можно попытаться привязать вручную. Для этого из Профиля автора перейдите в раздел «Поиск цитирований в РИНЦ». Довольно часто ссылки не могут быть привязаны, так как в цитирующей работе неверно указана ФИО автора. Поэтому можно начать поиск с ввода в поле «Автор цитируемой публикации» фамилии автора без инициалов, или даже части фамилии. Если вы хотели бы уточнить список ссылок на конкретную работу, можно в поле «Любое слово из текста ссылки» ввести часть названия работы. После нажатия кнопки «Поиск» выводится список работ с соответствующими им ссылками. Звездочка означает, что данная ссылка уже привязана к вашей публикации. Выберите в списке те ссылки, которые необходимо привязать и в панели «Инструменты» нажмите «Добавить выделенные ссылки в список моих цитирований».
-4. Если ссылки по-прежнему отсутствуют, вы можете обратиться к ответственному от вашего подразделения, чтобы он добавил цитирующие публикации в РИНЦ (см. ниже).
-**Порядок обращения к ответственным от подразделений**
-Как видно из сказанного выше, у автора имеется достаточно богатый набор инструментов для уточнения данных о своих публикациях – а следовательно, и для уточнения индексов цитирования. Единственное существенное ограничение – отсутствует возможность добавлять публикации. Причем это касается и добавления ссылок на ваши публикации – так как добавление ссылки равносильно добавлению публикации.
-Пожалуйста, примите во внимание, что ответственный от подразделения не сможет добавить публикацию, если у него не будет полного ее описания. А оператор со стороны РИНЦ может отказать в добавлении, если у него не будет ссылки на опубликованную статью или ее электронной копии.
-Поэтому при обращении к ответственному необходимо предоставить следующие данные. Если это статья, то 1) название статьи, 2) название журнала; 3) год (том, номер), 4) страницы; 5) тематика – желательно, по классификатору ГРНТИ; 6) список литературы, 7) прямая ссылка на опубликованную статью; 8) (желательно) электронная копия статьи.
-Если это книга/сборник, то 1) название, 2) издательство, 3) год (том, если есть), 4) место издания (город), 5) тематика – желательно, по классификатору ГРНТИ; 6) прямая ссылка на описание книги на сайте издательства; 7) (желательно) электронная копия книги.
-В том случае, если добавление публикаций требуется для их привязки в качестве ссылки на одну из ваших публикаций, приведите название своей публикации и далее список ссылающихся публикаций со всеми необходимыми данными (см. выше).
-Ответственного для своего подразделения вы можете найти в списке ниже. Если ответственного в списке нет, можно написать Ощепкову Ивану Владимировичу:
-**Анализ публикационной активности автора**
-Чтобы оценить влияние вносимых изменений на показатели публикационной активности (индекс Хирша и т.п.), пожалуйста, перейдите на страницу «Анализ публикационной активности автора». Попасть на эту страницу можно из раздела «Персональный профиль автора», а также из «Авторского указателя», щелкнув мышью на цветной иконке с гистограммой.
-Если вы внесли изменения, и это не отобразилось на статистике, нажмите «Обновить показатели автора» на панели «Инструменты».
-Как правило, внесенные изменения будут отражены в ваших показателях в тот же день. Однако в отдельных (напр., спорных) случаях изменения могут быть учтены лишь через некоторое время (от недели до двух месяцев). Если вы считаете, что некие изменения не были учтены в течение долгого времени, обратитесь к ответственному от вашего подразделения.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
         <is>
           <t xml:space="preserve">**https://portal.hse.ru/dpo_new**
 **https://portal.hse.ru/dpo_new**
@@ -2268,6 +2104,170 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/pay**
+На портале можно организовать прием платежей за участие в проводимых подразделениями НИУ ВШЭ мероприятиях. Заявка на создание формы приема платежей направляется руководителем подразделения на адрес underground@hse.ru. Срок оказания услуги — 2 рабочих дня с момента получения полного пакета необходимых сведений от заказчика при условии создания стандартной формы.
+**Что нужно указать в заявке**
+Обратите внимание, что по требованию финансового блока создание формы для приема платежей возможно только при наличии подписанного приказа на проведение мероприятия. Приказ создает подразделение-организатор мероприятия; документ согласуется с руководителями в соответствии с их полномочиями. Если доходы или расходы по мероприятию требуют проставления финансовых аналитик, в согласовании также участвует ПФУ. Копию договора необходимо приложить к заявке. В ней нужно указать:
+Номер учетного договора от ПФУ (номер БЭСТ), по которому будет вестись прием средств;Для учета поступающих средств по мероприятию в ИС-ПРО создается управленческий договор. Договор создается подразделением самостоятельно, если подразделение имеет доступ в ИС-ПРО с соответствующими правами, либо ответственным работником ПФУ.
+Наименование подразделения, которое будет осуществлять прием платежей;
+Шифр подразделения по ИС-ПРО;
+Адрес сайта в зоне hse.ru, где будет размещена страница мероприятия (желательно указать также адрес страницы с описанием особенностей оплаты);
+Список электронных почтовых адресов ответственных лиц в домене hse.ru для ежедневной выгрузки отчета по произведенным оплатам;
+Сроки приема платежей;
+Включен ли в сумму платежа НДС или нет;
+Требуется ли англоязычная версия формы;
+Список категорий участников (с переводом на английский язык при необходимости создания формы на английском языке) и соответствующие им суммы платежей в рублях;
+Текст договора-оферты, который будет размещен на странице формы приема платежей (его можно согласовать с юристами);
+При необходимости: бланки платежного извещения для оплаты участниками в валюте (в рублях) через банк для размещения на странице мероприятия;
+Если форма платежа нужна не для разового мероприятия, пожалуйста, добавьте в заявку информацию о типе платежа: оплата обучения, оплата проживания, оплата прочих услуг либо новый вид оплаты по договоренности с ПФУ и УБУ.
+Взаимодействие с участниками мероприятия проводится на основании договора-оферты, который должен быть размещен на странице мероприятия. В случае необходимости предоставления участникам мероприятия каких-либо подтверждающих документов их перечень необходимо в обязательном порядке предварительно согласовать с бухгалтерией НИУ ВШЭ.
+Важно!• Планируйте расценки на участие в мероприятии с учетом того, что на странице сбора платежей суммы к оплате указываются только в рублях, указание сумм в иностранных валютах не допускается, в том числе для иностранных участников.• Банк удерживает комиссию от суммы платежа. Комиссия с карт Сбербанка не взимается. Актуальный размер комиссии зависит от условий банка-эмитента карты платежа. По требованию банка выделять комиссию в сумме платежа на странице оплаты за мероприятие нельзя.
+**Варианты форм оплаты**
+Для стандартной формы оплаты допускается наличие нескольких категорий участников, каждой из которых может быть присвоена отдельная сумма к оплате. Например, для сотрудников НИУ ВШЭ - X руб., для иностранных граждан - Y руб. Автоматическая проверка статуса участника в момент оплаты не производится. Стандартная форма оплаты выглядит так:
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/analytics**
+На портале НИУ ВШЭ установлены счетчики Google Analytics и Яндекс.Метрика. C их помощью можно узнать количество посещений сайта, проанализировать действия пользователей, понять, как они перешли на ту или иную страницу. Доступна также статистика скачивания файлов.
+Вопросами, связанными с посещаемостью страниц портала, занимается Отдел веб-аналитики и моделирования.
+**Доступ к аналитике**
+**Предоставление доступа для специалистов по привлечению трафика или рекламных агентств**
+ Доступ предоставляется в отдельное представление Google Analytics. В выделенном представлении присутствуют данные отдельного поддомена. Настройки в представлении производятся специалистами по привлечению трафика или РА посредством GTM (Google Tag Manager). 
+**Предоставление доступа сотрудникам ВШЭ**
+Доступ предоставляется для сотрудников ВШЭ в Google Analytics или Я.Метрику без ограничений.
+Доступ предоставляется в течение одного рабочего дня.
+Запрос на предоставление доступа
+**Как узнать посещаемость сайта**
+**В Яндекс.Метрике**
+Самый простой способ узнать, сколько человек посетили страницу сайта вашего подразделения или мероприятия через Яндекс.Метрику, — использовать сервис стандартных отчетов «Заголовки страниц».
+В поле поиска задается название страницы. В результирующей таблице содержатся два значения для указанного временного диапазона: число просмотров (загрузок страницы) и число посетителей (количество уникальных людей, пришедших на вашу страницу). Подробная пользовательская инструкция Яндекс.Метрики доступна по адресу https://yandex.ru/support/metrika/
+**В Google Analytics**
+В меню сервиса, расположенном в левой части экрана, выбирается вкладка Поведение → Контент сайта → Все страницы. В строке поиска указывается url-адрес нужной страницы без указания сетевого протокола (https://).
+Для увеличения точности анализа нужно передвинуть соответствующий бегунок вверху экрана под строками выбора дат, а также выбрать более узкий временной промежуток. Подробная пользовательская инструкция Google Analytics находится по адресу https://support.google.com/analytics/
+**Как узнать число скачиваний файлов**
+**В Яндекс.Метрике**
+Стандартный отчет формируется так: Отчеты → Стандартные отчеты → Содержание → Загрузки файлов.
+Задаем необходимый временной промежуток, под графиком выбираем URL, загрузки файлов с которого нас интересуют.
+**В Google Analytics**
+В меню сервиса выбирается вкладка Поведение → События → Страницы. В строке поиска указывается url-адрес страницы, на которой находятся ссылки на файлы, без указания сетевого протокола (https://).
+Выбирается категория событий Download. Результирующая таблица показывает число скачанных с этой страницы файлов за выбранный промежуток времени.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/aspresponsible**
+**https://portal.hse.ru/aspresponsible**
+**Аспирантская школа по экономике**
+**https://portal.hse.ru/aspresponsible**
+**Аспирантская школа по менеджменту**
+**https://portal.hse.ru/aspresponsible**
+**Аспирантские школы: по государственному и муниципальному управлению; по философским наукам**
+**https://portal.hse.ru/aspresponsible**
+**Аспирантская школа по праву**
+**https://portal.hse.ru/aspresponsible**
+**Аспирантская школы: по социологическим наукам; по политическим наукам; по искусству и дизайну; по международным отношениям и зарубежным региональным исследованиям**
+**https://portal.hse.ru/aspresponsible**
+**Аспирантские школы: по историческим наукам; по филологическим наукам; по философским наукам; по культурологии**
+**https://portal.hse.ru/aspresponsible**
+**Аспирантская школа по техническим наукам**
+**https://portal.hse.ru/aspresponsible**
+**Аспирантские школы: по компьютерным наукам; по физике**
+**https://portal.hse.ru/aspresponsible**
+**Аспирантская школа по образованию**
+**https://portal.hse.ru/aspresponsible**
+**Аспирантская школа по психологии**
+**https://portal.hse.ru/aspresponsible**
+**Аспирантская школа по математике**
+**https://portal.hse.ru/aspresponsible**
+**Академическая аспирантура**
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/elibrary**
+С 2017 года в вашем распоряжении есть полный набор инструментов, предоставляемых НЭБ/РИНЦ. С их помощью можно уточнить и улучшить ваши показатели в РИНЦ. Большинство операций вы можете выполнить самостоятельно – и никто кроме вас не сможет это сделать должным образом. Но в некоторых случаях необходимо обратиться к представителям подразделений.
+Что можно сделать в первую очередь: 1) зарегистрироваться в РИНЦ:Science Index; 2) уточнить регистрационные данные для улучшения привязки публикаций; 3) проверить и скорректировать свой список публикаций; 4) проверить и скорректировать список ссылок на свои публикации.
+Ниже приведена краткая инструкция с учетом опыта работы с РИНЦ в НИУ ВШЭ. Полную инструкцию для авторов можно найти на сайте РИНЦ.
+ВНИМАНИЕ! Для корректной работы с сайтом РИНЦ необходимо отключить блокировку всплывающих окон для elibrary.ru.
+Инструкции
+Регистрация в Science IndexВнесение данных в регистрационную анкету и улучшение автоматической привязки публикацийРабота со списком публикацийРабота со ссылками на публикацииПорядок обращения к ответственным от подразделенийАнализ публикационной активности автора
+**Регистрация в Science Index**
+Если вы не зарегистрированы в Science Index, пройдите по этой ссылке: https://elibrary.ru/author_info.asp?isnew=1&amp;inreestr=on, либо выберите кнопку «Регистрация» в панели «Вход» на сайте elibrary.ru.
+Убедитесь, что в регистрационной анкете проставлена галочка «зарегистрировать меня как автора в системе Science Index».
+**Внесение данных в регистрационную анкету и улучшение автоматической привязки публикаций**
+При регистрации необходимо внести данные во все поля, обязательные для заполнения. Однако мы рекомендуем обратить внимание и на другие поля, так как это поможет автоматически привязать максимальное число ваших публикаций к аккаунту. Если вы уже зарегистрированы в Science Index, то можете внести эти данные, перейдя по ссылке: https://elibrary.ru/author_info.asp?isold=1, или пройдя в Личный кабинет → Профиль автора → Регистрационная карточка автора.
+1. Проверьте, указана ли аффилиация с НИУ ВШЭ
+2. В нижней части формы находятся поля, которые могут улучшить качество автоматической привязки публикаций
+В поле «Журналы» внесите журналы, в которых вы публиковались. В поле «Организации» укажите другие организации, в которых вы могли работать ранее. Если раньше у вас была другая фамилия, укажите ее в поле «Предыдущая фамилия (девичья)». Если вы публиковались или собираетесь публиковаться в зарубежных изданиях, укажите варианты написания фамилии латиницей – через запятую. В поле «Идентификационные коды автора» укажите любые другие свои идентификационные коды.
+3. После сохранения карточки в течение 2-10 дней вы получите уникальный идентификатор: SPIN-код автора.
+Он будет указан в панели «Сессия» слева, а также в начале регистрационной карточки. Необходимо указать этот SPIN-код в своем личном кабинете на портале НИУ ВШЭ.
+После получения SPIN-кода система выполнит привязку публикаций к вашему профилю, и вы получите возможность вносить исправления в список публикаций и список ссылок на публикации.
+**Работа со списком публикаций**
+После регистрации и заполнения карточки система попытается идентифицировать ваши работы автоматически и привязать их к вашему профилю. Однако возможны и ошибки идентификации.
+1. Начните с просмотра списка ваших публикаций (Профиль автора → Мои публикации). Проверьте, все ли публикации присутствуют в списке. Нет ли публикаций других авторов. Если таковые имеются, выберите их и нажмите «Удалить выделенные публикации…». Проверьте, правильно ли указана аффилиация для этих публикаций. Например, аффилиация с НИУ ВШЭ должна выглядеть так, как на рисунке ниже, то есть оформлена в виде гиперссылки со всплывающим полным названием.
+Если это не так, нажмите «Идентифицировать организацию, указанную в публикации в качестве места моей работы» в панели «Инструменты».
+2. Если в списке не обнаружены некоторые публикации, выберите в выпадающем списке «Показывать» «Непривязанные публикации, которые могут принадлежать данному автору». В открывшемся списке пометьте галочками принадлежащие вам публикации, после чего нажмите «Добавить выделенные публикации в список работ автора».
+3. Если некоторых публикаций нет ни в одном из указанных двух списков, это означает, что система не смогла идентифицировать публикации автоматически. В таком случае можно попытаться найти и привязать публикации вручную. Воспользуйтесь расширенным поиском (в левой верхней части страницы): вначале можно поискать по неполному имени и отчеству автора, затем, если, например, известно точное название публикации – по названию. После нажатия кнопки «Поиск» выводится список найденных публикаций – звездочкой помечены те, которые уже привязаны к вашему профилю. Если в списке найденных публикаций вы видите ту, которую необходимо привязать, щелкните по ее названию – откроется страница с описанием. В панели «Инструменты» выберите пункт «Добавить публикацию в список моих работ (если Вы являетесь ее автором)». После проверки публикация будет привязана к вашему профилю.
+4. Если не удалось найти публикацию ни в одном из этих случаев, вы можете обратиться к ответственному от вашего подразделения, чтобы он добавил нужную публикацию.
+**Работа со ссылками на публикации**
+Работа со ссылками во многом напоминает работу с публикациями
+1. Начните с просмотра списка ссылок: Профиль автора → Мои цитирования (либо в списке публикаций в панели «Инструменты» выберите «Вывести список ссылок на работы автора». Проверьте, нет ли в списке лишних ссылок. Если таковые имеются, выберите их и нажмите «Удалить выделенные ссылки из списка цитирований автора».
+2. В выпадающем списке «Показывать» выберите «Непривязанные ссылки, которые могут принадлежать данному автору».
+В открывшемся списке пометьте галочками принадлежащие вам публикации, после чего нажмите «Добавить выделенные ссылки в список цитирований автора».
+3. Если какие-то ссылки в этих списках отсутствуют, их можно попытаться привязать вручную. Для этого из Профиля автора перейдите в раздел «Поиск цитирований в РИНЦ». Довольно часто ссылки не могут быть привязаны, так как в цитирующей работе неверно указана ФИО автора. Поэтому можно начать поиск с ввода в поле «Автор цитируемой публикации» фамилии автора без инициалов, или даже части фамилии. Если вы хотели бы уточнить список ссылок на конкретную работу, можно в поле «Любое слово из текста ссылки» ввести часть названия работы. После нажатия кнопки «Поиск» выводится список работ с соответствующими им ссылками. Звездочка означает, что данная ссылка уже привязана к вашей публикации. Выберите в списке те ссылки, которые необходимо привязать и в панели «Инструменты» нажмите «Добавить выделенные ссылки в список моих цитирований».
+4. Если ссылки по-прежнему отсутствуют, вы можете обратиться к ответственному от вашего подразделения, чтобы он добавил цитирующие публикации в РИНЦ (см. ниже).
+**Порядок обращения к ответственным от подразделений**
+Как видно из сказанного выше, у автора имеется достаточно богатый набор инструментов для уточнения данных о своих публикациях – а следовательно, и для уточнения индексов цитирования. Единственное существенное ограничение – отсутствует возможность добавлять публикации. Причем это касается и добавления ссылок на ваши публикации – так как добавление ссылки равносильно добавлению публикации.
+Пожалуйста, примите во внимание, что ответственный от подразделения не сможет добавить публикацию, если у него не будет полного ее описания. А оператор со стороны РИНЦ может отказать в добавлении, если у него не будет ссылки на опубликованную статью или ее электронной копии.
+Поэтому при обращении к ответственному необходимо предоставить следующие данные. Если это статья, то 1) название статьи, 2) название журнала; 3) год (том, номер), 4) страницы; 5) тематика – желательно, по классификатору ГРНТИ; 6) список литературы, 7) прямая ссылка на опубликованную статью; 8) (желательно) электронная копия статьи.
+Если это книга/сборник, то 1) название, 2) издательство, 3) год (том, если есть), 4) место издания (город), 5) тематика – желательно, по классификатору ГРНТИ; 6) прямая ссылка на описание книги на сайте издательства; 7) (желательно) электронная копия книги.
+В том случае, если добавление публикаций требуется для их привязки в качестве ссылки на одну из ваших публикаций, приведите название своей публикации и далее список ссылающихся публикаций со всеми необходимыми данными (см. выше).
+Ответственного для своего подразделения вы можете найти в списке ниже. Если ответственного в списке нет, можно написать Ощепкову Ивану Владимировичу:
+**Анализ публикационной активности автора**
+Чтобы оценить влияние вносимых изменений на показатели публикационной активности (индекс Хирша и т.п.), пожалуйста, перейдите на страницу «Анализ публикационной активности автора». Попасть на эту страницу можно из раздела «Персональный профиль автора», а также из «Авторского указателя», щелкнув мышью на цветной иконке с гистограммой.
+Если вы внесли изменения, и это не отобразилось на статистике, нажмите «Обновить показатели автора» на панели «Инструменты».
+Как правило, внесенные изменения будут отражены в ваших показателях в тот же день. Однако в отдельных (напр., спорных) случаях изменения могут быть учтены лишь через некоторое время (от недели до двух месяцев). Если вы считаете, что некие изменения не были учтены в течение долгого времени, обратитесь к ответственному от вашего подразделения.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**https://portal.hse.ru/brandbook_html_colours**
+Данные обозначения можно использовать при оформлении лендингов: для цвета подложки в шапке и основной колонке (контент-блок), цвета подложек в виджетах «Набор с выпадайками» и «Табы с карточками», виджетах «Цифра дня», «Плашка с цифрой», «Хронология», фонов виджетов «Программы», «Карусель», «Цифры», «Цифры и факты», «Ссылки», «Мероприятия», «Публикации», а также мобильного тулбара.
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>